<commit_message>
Added static debug joints to pancak debug
</commit_message>
<xml_diff>
--- a/TODO altCtrlPancake.xlsx
+++ b/TODO altCtrlPancake.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ashley Sands\Amstrike Games\SimPancake3000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCC633F-C8CC-44D9-A7F0-2B7AFF7F9751}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1542D288-9E38-453D-BB91-44C6AC4F9DE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6732AF01-4E77-4178-A282-B4B033BA40EA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6732AF01-4E77-4178-A282-B4B033BA40EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Todo (Game Main)" sheetId="2" r:id="rId2"/>
     <sheet name="Todo (Arduino)" sheetId="4" r:id="rId3"/>
+    <sheet name="Working outs" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="98">
   <si>
     <t>Project Sheet - Summary</t>
   </si>
@@ -305,15 +306,52 @@
   <si>
     <t>the pancake need to move inwards</t>
   </si>
+  <si>
+    <t>Gravity</t>
+  </si>
+  <si>
+    <t>Translated Vector3 (x, y, z)</t>
+  </si>
+  <si>
+    <t>x+z</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">b = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotSpeed </t>
+  </si>
+  <si>
+    <t>The pancakes are not being removed from the pancake list in FryingPan_pancake</t>
+  </si>
+  <si>
+    <t>Fixed Flip not rotating</t>
+  </si>
+  <si>
+    <t>flaten pancake when it out of the pan</t>
+  </si>
+  <si>
+    <t>blend the pancakes shape when entering the pan</t>
+  </si>
+  <si>
+    <t>Level out pancake once below rotate thresshold</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -720,7 +758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -834,6 +872,21 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -873,71 +926,20 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1134,6 +1136,50 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1176,29 +1222,29 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B2D132A-8E44-48F1-BBB2-2C53A683D787}" name="Main" displayName="Main" ref="A3:G50" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A3:G50" xr:uid="{041E981F-6BC0-4FDE-ACBA-E530F1EEC1B5}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{824F3C5E-1D9A-43A1-B8C9-BD326514D302}" name="ID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{1150AD6D-6BBD-4CBF-9E9A-9902A96F9F82}" name="Task Name" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{F083697A-B89D-45BD-9721-20A038AAB4B0}" name="Task Details" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{85C72231-B520-4C6B-9B33-80C7B98FAEAF}" name="Status" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{4B87CB35-1B38-4C75-BBE3-CA245029C4B8}" name="Group" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{B40BFB71-0609-470A-9EAD-D610C0B87C75}" name="Sub Group" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{23817CE4-D3E3-4F39-ABA0-28388712A836}" name="Notes" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{824F3C5E-1D9A-43A1-B8C9-BD326514D302}" name="ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{1150AD6D-6BBD-4CBF-9E9A-9902A96F9F82}" name="Task Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{F083697A-B89D-45BD-9721-20A038AAB4B0}" name="Task Details" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{85C72231-B520-4C6B-9B33-80C7B98FAEAF}" name="Status" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{4B87CB35-1B38-4C75-BBE3-CA245029C4B8}" name="Group" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{B40BFB71-0609-470A-9EAD-D610C0B87C75}" name="Sub Group" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{23817CE4-D3E3-4F39-ABA0-28388712A836}" name="Notes" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60864319-97C2-48A4-B74F-713E907C5D25}" name="Arduino" displayName="Arduino" ref="A3:G50" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60864319-97C2-48A4-B74F-713E907C5D25}" name="Arduino" displayName="Arduino" ref="A3:G50" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A3:G50" xr:uid="{041E981F-6BC0-4FDE-ACBA-E530F1EEC1B5}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{12C5545D-8B1E-4FB2-8748-F7DBD896D325}" name="ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{8D4C031C-DE34-4573-B782-3D586DEEE833}" name="Task Name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{A2A6B64D-29D1-48FF-A65C-BA0EBD121B5B}" name="Task Details" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{45A6DF31-36F1-4C08-B878-330C15541E2C}" name="Status" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{E20DE365-0A63-46A6-B55D-5E36FCC83D00}" name="Group" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{A90C5265-ADB6-421D-9C00-5E9716201C56}" name="Sub Group" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{92972826-2FDE-4271-B1AE-3D18F97AB66D}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{12C5545D-8B1E-4FB2-8748-F7DBD896D325}" name="ID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{8D4C031C-DE34-4573-B782-3D586DEEE833}" name="Task Name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A2A6B64D-29D1-48FF-A65C-BA0EBD121B5B}" name="Task Details" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{45A6DF31-36F1-4C08-B878-330C15541E2C}" name="Status" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E20DE365-0A63-46A6-B55D-5E36FCC83D00}" name="Group" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{A90C5265-ADB6-421D-9C00-5E9716201C56}" name="Sub Group" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{92972826-2FDE-4271-B1AE-3D18F97AB66D}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1522,17 +1568,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
       <c r="J1" s="33"/>
       <c r="K1" s="33"/>
       <c r="L1" s="33"/>
@@ -1580,7 +1626,7 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">_xlfn.DAYS(E4,NOW())</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>6</v>
@@ -1597,24 +1643,24 @@
       </c>
       <c r="C6" s="12">
         <f ca="1">1-IF(E5&lt;&gt;0,(C5/E5),0)</f>
-        <v>0.1428571428571429</v>
-      </c>
-      <c r="D6" s="89" t="s">
+        <v>0.2142857142857143</v>
+      </c>
+      <c r="D6" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="89"/>
+      <c r="E6" s="76"/>
     </row>
     <row r="8" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="90" t="s">
+      <c r="B8" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -1629,21 +1675,21 @@
       </c>
       <c r="E9" s="14">
         <f>C14+C15+G14+G15+C16+G16</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="14">
         <f>C9+E9</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="17">
         <f>C15+G15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1652,14 +1698,14 @@
       </c>
       <c r="C10" s="18">
         <f>C9/G9</f>
-        <v>0.14814814814814814</v>
+        <v>0.12903225806451613</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="19">
         <f>E9/G9</f>
-        <v>0.85185185185185186</v>
+        <v>0.87096774193548387</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>14</v>
@@ -1673,7 +1719,7 @@
       </c>
       <c r="I10" s="21">
         <f>I9/G9</f>
-        <v>0</v>
+        <v>3.2258064516129031E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1685,27 +1731,27 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="77"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="82"/>
       <c r="E13" s="22"/>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="76"/>
-      <c r="H13" s="77"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="82"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
@@ -1713,11 +1759,11 @@
       </c>
       <c r="C14" s="24">
         <f>COUNTIF(Main[Status], "-")</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D14" s="25">
         <f>C14/C20</f>
-        <v>1</v>
+        <v>0.95652173913043481</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="23" t="s">
@@ -1729,7 +1775,7 @@
       </c>
       <c r="H14" s="25">
         <f>G14/G20</f>
-        <v>0.21052631578947367</v>
+        <v>0.17391304347826086</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1738,11 +1784,11 @@
       </c>
       <c r="C15" s="24">
         <f>COUNTIF(Main[Status], "wip")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="25">
         <f>C15/C20</f>
-        <v>0</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="23" t="s">
@@ -1804,7 +1850,7 @@
       </c>
       <c r="H17" s="25">
         <f>G17/G20</f>
-        <v>0.21052631578947367</v>
+        <v>0.17391304347826086</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1863,7 +1909,7 @@
       </c>
       <c r="C20" s="28">
         <f>COUNTA(Main[Status])</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D20" s="29">
         <f>SUM(D14:D19)</f>
@@ -1875,11 +1921,11 @@
       </c>
       <c r="G20" s="28">
         <f>COUNTA(Main[Status])</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H20" s="29">
         <f>SUM(H14:H19)</f>
-        <v>0.42105263157894735</v>
+        <v>0.34782608695652173</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1895,7 +1941,7 @@
       </c>
       <c r="G21" s="30">
         <f>H14+H15+H16</f>
-        <v>0.21052631578947367</v>
+        <v>0.17391304347826086</v>
       </c>
       <c r="S21" s="67"/>
     </row>
@@ -1912,32 +1958,32 @@
       </c>
       <c r="G22" s="32">
         <f>H17+H18+H19</f>
-        <v>0.21052631578947367</v>
+        <v>0.17391304347826086</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="80"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81" t="s">
+      <c r="B25" s="85"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="81"/>
-      <c r="I25" s="81"/>
-      <c r="J25" s="81"/>
-      <c r="K25" s="81"/>
-      <c r="L25" s="82" t="s">
+      <c r="H25" s="86"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="86"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="M25" s="83"/>
-      <c r="N25" s="84"/>
+      <c r="M25" s="88"/>
+      <c r="N25" s="89"/>
       <c r="O25" s="63"/>
     </row>
     <row r="26" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
@@ -1947,28 +1993,28 @@
       <c r="D26" s="35"/>
       <c r="E26" s="35"/>
       <c r="F26" s="35"/>
-      <c r="G26" s="85" t="s">
+      <c r="G26" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="85" t="s">
+      <c r="H26" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="I26" s="85" t="s">
+      <c r="I26" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="J26" s="85" t="s">
+      <c r="J26" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="78" t="s">
+      <c r="K26" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="L26" s="86" t="s">
+      <c r="L26" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="M26" s="87" t="s">
+      <c r="M26" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="N26" s="78" t="s">
+      <c r="N26" s="83" t="s">
         <v>43</v>
       </c>
       <c r="O26" s="64"/>
@@ -1992,14 +2038,14 @@
       <c r="F27" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="85"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="85"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="86"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="78"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="83"/>
+      <c r="L27" s="91"/>
+      <c r="M27" s="92"/>
+      <c r="N27" s="83"/>
       <c r="O27" s="64" t="s">
         <v>54</v>
       </c>
@@ -2299,11 +2345,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="F12:H12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="N26:N27"/>
@@ -2317,8 +2358,13 @@
     <mergeCell ref="K26:K27"/>
     <mergeCell ref="L26:L27"/>
     <mergeCell ref="M26:M27"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="F12:H12"/>
   </mergeCells>
-  <conditionalFormatting sqref="C22 C10">
+  <conditionalFormatting sqref="C10 C22">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2377,8 +2423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BDFBF0-BDE3-48CD-9C74-022AECEC1124}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2395,15 +2441,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="H1" s="72"/>
       <c r="I1" s="72"/>
     </row>
@@ -2456,7 +2502,9 @@
       <c r="D5" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="74"/>
+      <c r="G5" s="74" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="73">
@@ -2695,32 +2743,52 @@
       <c r="A23" s="73">
         <v>19</v>
       </c>
-      <c r="B23" s="74"/>
+      <c r="B23" s="74" t="s">
+        <v>94</v>
+      </c>
       <c r="C23" s="74"/>
+      <c r="D23" s="73" t="s">
+        <v>19</v>
+      </c>
       <c r="G23" s="74"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="73">
         <v>20</v>
       </c>
-      <c r="B24" s="74"/>
+      <c r="B24" s="74" t="s">
+        <v>95</v>
+      </c>
       <c r="C24" s="74"/>
+      <c r="D24" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G24" s="74"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="73">
         <v>21</v>
       </c>
-      <c r="B25" s="74"/>
+      <c r="B25" s="74" t="s">
+        <v>96</v>
+      </c>
       <c r="C25" s="74"/>
+      <c r="D25" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G25" s="74"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="73">
         <v>22</v>
       </c>
-      <c r="B26" s="74"/>
+      <c r="B26" s="74" t="s">
+        <v>97</v>
+      </c>
       <c r="C26" s="74"/>
+      <c r="D26" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G26" s="74"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -2901,15 +2969,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="H1" s="72"/>
       <c r="I1" s="72"/>
     </row>
@@ -3049,4 +3117,3301 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A58165-66D3-4FDC-A087-9321E2B81B62}">
+  <dimension ref="A2:AC125"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B2" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="I2" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="97"/>
+      <c r="K2" s="97"/>
+      <c r="P2" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="97"/>
+      <c r="W2" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="X2" s="97"/>
+      <c r="Y2" s="97"/>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>9.81</v>
+      </c>
+      <c r="C3">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="D3">
+        <f>B3*C3</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="I3">
+        <v>9.81</v>
+      </c>
+      <c r="J3">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="K3">
+        <f>I3*J3</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="P3">
+        <v>9.81</v>
+      </c>
+      <c r="Q3">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="R3">
+        <f>P3*Q3</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="W3">
+        <v>9.81</v>
+      </c>
+      <c r="X3">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="Y3">
+        <f>W3*X3</f>
+        <v>0.19620000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D4" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="K4" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
+      <c r="R4" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S4" s="97"/>
+      <c r="T4" s="97"/>
+      <c r="Y4" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z4" s="97"/>
+      <c r="AA4" s="97"/>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D5" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E5">
+        <v>4.6255750000000004</v>
+      </c>
+      <c r="F5">
+        <v>1.323062</v>
+      </c>
+      <c r="K5" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L5">
+        <f>E24-K3</f>
+        <v>4.036975</v>
+      </c>
+      <c r="M5">
+        <v>1.323062</v>
+      </c>
+      <c r="R5" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S5">
+        <f>L24-R3</f>
+        <v>3.4483749999999995</v>
+      </c>
+      <c r="T5">
+        <v>1.323062</v>
+      </c>
+      <c r="Y5" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z5">
+        <f>S24-Y3</f>
+        <v>2.8597749999999991</v>
+      </c>
+      <c r="AA5">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="96">
+        <f>D5+F5</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E7" s="94"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="96"/>
+      <c r="I7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" s="96">
+        <f>K5+M5</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L7" s="94"/>
+      <c r="N7" s="95"/>
+      <c r="P7" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>88</v>
+      </c>
+      <c r="R7" s="96">
+        <f>R5+T5</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S7" s="94"/>
+      <c r="U7" s="95"/>
+      <c r="W7" t="s">
+        <v>90</v>
+      </c>
+      <c r="X7" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y7" s="96">
+        <f>Y5+AA5</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z7" s="94"/>
+      <c r="AB7" s="95"/>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="96">
+        <f>E5</f>
+        <v>4.6255750000000004</v>
+      </c>
+      <c r="I8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" s="96">
+        <f>L5</f>
+        <v>4.036975</v>
+      </c>
+      <c r="P8" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>89</v>
+      </c>
+      <c r="R8" s="96">
+        <f>S5</f>
+        <v>3.4483749999999995</v>
+      </c>
+      <c r="W8" t="s">
+        <v>91</v>
+      </c>
+      <c r="X8" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y8" s="96">
+        <f>Z5</f>
+        <v>2.8597749999999991</v>
+      </c>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="96">
+        <f>D8/D7</f>
+        <v>3.4961131670613956</v>
+      </c>
+      <c r="E10">
+        <f>D10*180</f>
+        <v>629.30037007105125</v>
+      </c>
+      <c r="F10" s="95"/>
+      <c r="G10" s="95">
+        <f>E10*C3</f>
+        <v>12.586007401421025</v>
+      </c>
+      <c r="J10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="96">
+        <f>K8/K7</f>
+        <v>3.0512361063430333</v>
+      </c>
+      <c r="L10">
+        <f>K10*180</f>
+        <v>549.22249914174597</v>
+      </c>
+      <c r="M10" s="95"/>
+      <c r="N10" s="95">
+        <f>L10*J3</f>
+        <v>10.984449982834919</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>92</v>
+      </c>
+      <c r="R10" s="96">
+        <f>R8/R7</f>
+        <v>2.606359045624671</v>
+      </c>
+      <c r="S10">
+        <f>R10*180</f>
+        <v>469.14462821244081</v>
+      </c>
+      <c r="T10" s="95"/>
+      <c r="U10" s="95">
+        <f>S10*Q3</f>
+        <v>9.3828925642488166</v>
+      </c>
+      <c r="X10" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y10" s="96">
+        <f>Y8/Y7</f>
+        <v>2.1614819849063083</v>
+      </c>
+      <c r="Z10">
+        <f>Y10*180</f>
+        <v>389.06675728313547</v>
+      </c>
+      <c r="AA10" s="95"/>
+      <c r="AB10" s="95">
+        <f>Z10*X3</f>
+        <v>7.7813351456627098</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="G11" s="95"/>
+      <c r="N11" s="95"/>
+      <c r="U11" s="95"/>
+      <c r="AB11" s="95"/>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D13" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
+      <c r="K13" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="R13" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S13" s="97"/>
+      <c r="T13" s="97"/>
+      <c r="Y13" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z13" s="97"/>
+      <c r="AA13" s="97"/>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D14" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E14">
+        <f>E5-D3</f>
+        <v>4.4293750000000003</v>
+      </c>
+      <c r="F14">
+        <v>1.323062</v>
+      </c>
+      <c r="K14" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L14">
+        <f>L5-K3</f>
+        <v>3.8407749999999998</v>
+      </c>
+      <c r="M14">
+        <v>1.323062</v>
+      </c>
+      <c r="R14" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S14">
+        <f>S5-R3</f>
+        <v>3.2521749999999994</v>
+      </c>
+      <c r="T14">
+        <v>1.323062</v>
+      </c>
+      <c r="Y14" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z14">
+        <f>Z5-Y3</f>
+        <v>2.6635749999999989</v>
+      </c>
+      <c r="AA14">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="96">
+        <f>D14+F14</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E16" s="94"/>
+      <c r="I16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" t="s">
+        <v>88</v>
+      </c>
+      <c r="K16" s="96">
+        <f>K14+M14</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L16" s="94"/>
+      <c r="P16" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>88</v>
+      </c>
+      <c r="R16" s="96">
+        <f>R14+T14</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S16" s="94"/>
+      <c r="W16" t="s">
+        <v>90</v>
+      </c>
+      <c r="X16" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y16" s="96">
+        <f>Y14+AA14</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z16" s="94"/>
+    </row>
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="96">
+        <f>E14</f>
+        <v>4.4293750000000003</v>
+      </c>
+      <c r="G17" s="95"/>
+      <c r="H17" s="96"/>
+      <c r="I17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="96">
+        <f>L14</f>
+        <v>3.8407749999999998</v>
+      </c>
+      <c r="N17" s="95"/>
+      <c r="P17" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>89</v>
+      </c>
+      <c r="R17" s="96">
+        <f>S14</f>
+        <v>3.2521749999999994</v>
+      </c>
+      <c r="U17" s="95"/>
+      <c r="W17" t="s">
+        <v>91</v>
+      </c>
+      <c r="X17" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y17" s="96">
+        <f>Z14</f>
+        <v>2.6635749999999989</v>
+      </c>
+      <c r="AB17" s="95"/>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="96">
+        <f>D17/D16</f>
+        <v>3.347820813488608</v>
+      </c>
+      <c r="E19">
+        <f>D19*180</f>
+        <v>602.60774642794945</v>
+      </c>
+      <c r="F19" s="95"/>
+      <c r="G19" s="95">
+        <f>E19*C3</f>
+        <v>12.05215492855899</v>
+      </c>
+      <c r="J19" t="s">
+        <v>92</v>
+      </c>
+      <c r="K19" s="96">
+        <f>K17/K16</f>
+        <v>2.9029437527702457</v>
+      </c>
+      <c r="L19">
+        <f>K19*180</f>
+        <v>522.52987549864429</v>
+      </c>
+      <c r="M19" s="95"/>
+      <c r="N19" s="95">
+        <f>L19*J3</f>
+        <v>10.450597509972885</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>92</v>
+      </c>
+      <c r="R19" s="96">
+        <f>R17/R16</f>
+        <v>2.4580666920518834</v>
+      </c>
+      <c r="S19">
+        <f>R19*180</f>
+        <v>442.45200456933901</v>
+      </c>
+      <c r="T19" s="95"/>
+      <c r="U19" s="95">
+        <f>S19*Q3</f>
+        <v>8.8490400913867813</v>
+      </c>
+      <c r="X19" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y19" s="96">
+        <f>Y17/Y16</f>
+        <v>2.0131896313335211</v>
+      </c>
+      <c r="Z19">
+        <f>Y19*180</f>
+        <v>362.37413364003379</v>
+      </c>
+      <c r="AA19" s="95"/>
+      <c r="AB19" s="95">
+        <f>Z19*X3</f>
+        <v>7.2474826728006763</v>
+      </c>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="D20" s="94"/>
+      <c r="F20" s="95"/>
+      <c r="G20" s="95"/>
+      <c r="K20" s="94"/>
+      <c r="M20" s="95"/>
+      <c r="N20" s="95"/>
+      <c r="R20" s="94"/>
+      <c r="T20" s="95"/>
+      <c r="U20" s="95"/>
+      <c r="Y20" s="94"/>
+      <c r="AA20" s="95"/>
+      <c r="AB20" s="95"/>
+    </row>
+    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="G21" s="95"/>
+      <c r="N21" s="95"/>
+      <c r="U21" s="95"/>
+      <c r="AB21" s="95"/>
+    </row>
+    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="D23" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="K23" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L23" s="97"/>
+      <c r="M23" s="97"/>
+      <c r="R23" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S23" s="97"/>
+      <c r="T23" s="97"/>
+      <c r="Y23" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z23" s="97"/>
+      <c r="AA23" s="97"/>
+    </row>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="D24" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E24">
+        <f>E14-D3</f>
+        <v>4.2331750000000001</v>
+      </c>
+      <c r="F24">
+        <v>1.323062</v>
+      </c>
+      <c r="K24" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L24">
+        <f>L14-K3</f>
+        <v>3.6445749999999997</v>
+      </c>
+      <c r="M24">
+        <v>1.323062</v>
+      </c>
+      <c r="R24" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S24">
+        <f>S14-R3</f>
+        <v>3.0559749999999992</v>
+      </c>
+      <c r="T24">
+        <v>1.323062</v>
+      </c>
+      <c r="Y24" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z24">
+        <f>Z14-Y3</f>
+        <v>2.4673749999999988</v>
+      </c>
+      <c r="AA24">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="96">
+        <f>D24+F24</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E26" s="94"/>
+      <c r="I26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26" t="s">
+        <v>88</v>
+      </c>
+      <c r="K26" s="96">
+        <f>K24+M24</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L26" s="94"/>
+      <c r="P26" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>88</v>
+      </c>
+      <c r="R26" s="96">
+        <f>R24+T24</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S26" s="94"/>
+      <c r="W26" t="s">
+        <v>90</v>
+      </c>
+      <c r="X26" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y26" s="96">
+        <f>Y24+AA24</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z26" s="94"/>
+    </row>
+    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="96">
+        <f>E24</f>
+        <v>4.2331750000000001</v>
+      </c>
+      <c r="I27" t="s">
+        <v>91</v>
+      </c>
+      <c r="J27" t="s">
+        <v>89</v>
+      </c>
+      <c r="K27" s="96">
+        <f>L24</f>
+        <v>3.6445749999999997</v>
+      </c>
+      <c r="P27" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>89</v>
+      </c>
+      <c r="R27" s="96">
+        <f>S24</f>
+        <v>3.0559749999999992</v>
+      </c>
+      <c r="W27" t="s">
+        <v>91</v>
+      </c>
+      <c r="X27" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y27" s="96">
+        <f>Z24</f>
+        <v>2.4673749999999988</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="96">
+        <f>D27/D26</f>
+        <v>3.1995284599158205</v>
+      </c>
+      <c r="E29">
+        <f>D29*180</f>
+        <v>575.91512278484765</v>
+      </c>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95">
+        <f>E29*C3</f>
+        <v>11.518302455696952</v>
+      </c>
+      <c r="J29" t="s">
+        <v>92</v>
+      </c>
+      <c r="K29" s="96">
+        <f>K27/K26</f>
+        <v>2.7546513991974582</v>
+      </c>
+      <c r="L29">
+        <f>K29*180</f>
+        <v>495.83725185554249</v>
+      </c>
+      <c r="M29" s="95"/>
+      <c r="N29" s="95">
+        <f>L29*J3</f>
+        <v>9.9167450371108501</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>92</v>
+      </c>
+      <c r="R29" s="96">
+        <f>R27/R26</f>
+        <v>2.3097743384790959</v>
+      </c>
+      <c r="S29">
+        <f>R29*180</f>
+        <v>415.75938092623727</v>
+      </c>
+      <c r="T29" s="95"/>
+      <c r="U29" s="95">
+        <f>S29*Q3</f>
+        <v>8.315187618524746</v>
+      </c>
+      <c r="X29" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y29" s="96">
+        <f>Y27/Y26</f>
+        <v>1.8648972777607336</v>
+      </c>
+      <c r="Z29">
+        <f>Y29*180</f>
+        <v>335.68150999693205</v>
+      </c>
+      <c r="AA29" s="95"/>
+      <c r="AB29" s="95">
+        <f>Z29*X3</f>
+        <v>6.713630199938641</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="G31" s="95">
+        <f>G29+G19+G10</f>
+        <v>36.156464785676967</v>
+      </c>
+      <c r="N31" s="95">
+        <f>N29+N19+N10</f>
+        <v>31.351792529918654</v>
+      </c>
+      <c r="U31" s="95">
+        <f>U29+U19+U10</f>
+        <v>26.547120274160346</v>
+      </c>
+      <c r="AB31" s="95">
+        <f>AB29+AB19+AB10</f>
+        <v>21.742448018402026</v>
+      </c>
+      <c r="AC31" s="95">
+        <f>SUM(G31:AB31)</f>
+        <v>115.79782560815799</v>
+      </c>
+    </row>
+    <row r="32" spans="2:29" s="98" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B33" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="I33" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="J33" s="97"/>
+      <c r="K33" s="97"/>
+      <c r="P33" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q33" s="97"/>
+      <c r="R33" s="97"/>
+      <c r="W33" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="X33" s="97"/>
+      <c r="Y33" s="97"/>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>9.81</v>
+      </c>
+      <c r="C34">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="D34">
+        <f>B34*C34</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="I34">
+        <v>9.81</v>
+      </c>
+      <c r="J34">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="K34">
+        <f>I34*J34</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="P34">
+        <v>9.81</v>
+      </c>
+      <c r="Q34">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="R34">
+        <f>P34*Q34</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="W34">
+        <v>9.81</v>
+      </c>
+      <c r="X34">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="Y34">
+        <f>W34*X34</f>
+        <v>0.19620000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D35" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="97"/>
+      <c r="F35" s="97"/>
+      <c r="K35" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L35" s="97"/>
+      <c r="M35" s="97"/>
+      <c r="R35" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S35" s="97"/>
+      <c r="T35" s="97"/>
+      <c r="Y35" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z35" s="97"/>
+      <c r="AA35" s="97"/>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D36" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E36">
+        <f>Z24-D34</f>
+        <v>2.2711749999999986</v>
+      </c>
+      <c r="F36">
+        <v>1.323062</v>
+      </c>
+      <c r="K36" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L36">
+        <f>E55-K34</f>
+        <v>1.6825749999999986</v>
+      </c>
+      <c r="M36">
+        <v>1.323062</v>
+      </c>
+      <c r="R36" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S36">
+        <f>L55-R34</f>
+        <v>1.0939749999999988</v>
+      </c>
+      <c r="T36">
+        <v>1.323062</v>
+      </c>
+      <c r="Y36" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z36">
+        <f>S55-Y34</f>
+        <v>0.50537499999999869</v>
+      </c>
+      <c r="AA36">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="96">
+        <f>D36+F36</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E38" s="94"/>
+      <c r="G38" s="95"/>
+      <c r="H38" s="96"/>
+      <c r="I38" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" t="s">
+        <v>88</v>
+      </c>
+      <c r="K38" s="96">
+        <f>K36+M36</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L38" s="94"/>
+      <c r="N38" s="95"/>
+      <c r="P38" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>88</v>
+      </c>
+      <c r="R38" s="96">
+        <f>R36+T36</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S38" s="94"/>
+      <c r="U38" s="95"/>
+      <c r="W38" t="s">
+        <v>90</v>
+      </c>
+      <c r="X38" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y38" s="96">
+        <f>Y36+AA36</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z38" s="94"/>
+      <c r="AB38" s="95"/>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="96">
+        <f>E36</f>
+        <v>2.2711749999999986</v>
+      </c>
+      <c r="I39" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39" s="96">
+        <f>L36</f>
+        <v>1.6825749999999986</v>
+      </c>
+      <c r="P39" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>89</v>
+      </c>
+      <c r="R39" s="96">
+        <f>S36</f>
+        <v>1.0939749999999988</v>
+      </c>
+      <c r="W39" t="s">
+        <v>91</v>
+      </c>
+      <c r="X39" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y39" s="96">
+        <f>Z36</f>
+        <v>0.50537499999999869</v>
+      </c>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="96">
+        <f>D39/D38</f>
+        <v>1.7166049241879462</v>
+      </c>
+      <c r="E41">
+        <f>D41*180</f>
+        <v>308.98888635383031</v>
+      </c>
+      <c r="F41" s="95"/>
+      <c r="G41" s="95">
+        <f>E41*C34</f>
+        <v>6.1797777270766066</v>
+      </c>
+      <c r="J41" t="s">
+        <v>92</v>
+      </c>
+      <c r="K41" s="96">
+        <f>K39/K38</f>
+        <v>1.2717278634695841</v>
+      </c>
+      <c r="L41">
+        <f>K41*180</f>
+        <v>228.91101542452515</v>
+      </c>
+      <c r="M41" s="95"/>
+      <c r="N41" s="95">
+        <f>L41*J34</f>
+        <v>4.5782203084905033</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>92</v>
+      </c>
+      <c r="R41" s="96">
+        <f>R39/R38</f>
+        <v>0.82685080275122236</v>
+      </c>
+      <c r="S41">
+        <f>R41*180</f>
+        <v>148.83314449522001</v>
+      </c>
+      <c r="T41" s="95"/>
+      <c r="U41" s="95">
+        <f>S41*Q34</f>
+        <v>2.9766628899044001</v>
+      </c>
+      <c r="X41" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y41" s="96">
+        <f>Y39/Y38</f>
+        <v>0.38197374203286033</v>
+      </c>
+      <c r="Z41">
+        <f>Y41*180</f>
+        <v>68.755273565914862</v>
+      </c>
+      <c r="AA41" s="95"/>
+      <c r="AB41" s="95">
+        <f>Z41*X34</f>
+        <v>1.3751054713182973</v>
+      </c>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="G42" s="95"/>
+      <c r="N42" s="95"/>
+      <c r="U42" s="95"/>
+      <c r="AB42" s="95"/>
+    </row>
+    <row r="44" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D44" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="97"/>
+      <c r="F44" s="97"/>
+      <c r="K44" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L44" s="97"/>
+      <c r="M44" s="97"/>
+      <c r="R44" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S44" s="97"/>
+      <c r="T44" s="97"/>
+      <c r="Y44" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z44" s="97"/>
+      <c r="AA44" s="97"/>
+    </row>
+    <row r="45" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D45" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E45">
+        <f>E36-D34</f>
+        <v>2.0749749999999985</v>
+      </c>
+      <c r="F45">
+        <v>1.323062</v>
+      </c>
+      <c r="K45" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L45">
+        <f>L36-K34</f>
+        <v>1.4863749999999987</v>
+      </c>
+      <c r="M45">
+        <v>1.323062</v>
+      </c>
+      <c r="R45" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S45">
+        <f>S36-R34</f>
+        <v>0.89777499999999877</v>
+      </c>
+      <c r="T45">
+        <v>1.323062</v>
+      </c>
+      <c r="Y45" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z45">
+        <f>Z36-Y34</f>
+        <v>0.30917499999999865</v>
+      </c>
+      <c r="AA45">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="47" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="96">
+        <f>D45+F45</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E47" s="94"/>
+      <c r="I47" t="s">
+        <v>90</v>
+      </c>
+      <c r="J47" t="s">
+        <v>88</v>
+      </c>
+      <c r="K47" s="96">
+        <f>K45+M45</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L47" s="94"/>
+      <c r="P47" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>88</v>
+      </c>
+      <c r="R47" s="96">
+        <f>R45+T45</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S47" s="94"/>
+      <c r="W47" t="s">
+        <v>90</v>
+      </c>
+      <c r="X47" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y47" s="96">
+        <f>Y45+AA45</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z47" s="94"/>
+    </row>
+    <row r="48" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" s="96">
+        <f>E45</f>
+        <v>2.0749749999999985</v>
+      </c>
+      <c r="G48" s="95"/>
+      <c r="H48" s="96"/>
+      <c r="I48" t="s">
+        <v>91</v>
+      </c>
+      <c r="J48" t="s">
+        <v>89</v>
+      </c>
+      <c r="K48" s="96">
+        <f>L45</f>
+        <v>1.4863749999999987</v>
+      </c>
+      <c r="N48" s="95"/>
+      <c r="P48" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>89</v>
+      </c>
+      <c r="R48" s="96">
+        <f>S45</f>
+        <v>0.89777499999999877</v>
+      </c>
+      <c r="U48" s="95"/>
+      <c r="W48" t="s">
+        <v>91</v>
+      </c>
+      <c r="X48" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y48" s="96">
+        <f>Z45</f>
+        <v>0.30917499999999865</v>
+      </c>
+      <c r="AB48" s="95"/>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" s="96">
+        <f>D48/D47</f>
+        <v>1.5683125706151588</v>
+      </c>
+      <c r="E50">
+        <f>D50*180</f>
+        <v>282.29626271072857</v>
+      </c>
+      <c r="F50" s="95"/>
+      <c r="G50" s="95">
+        <f>E50*C34</f>
+        <v>5.6459252542145713</v>
+      </c>
+      <c r="J50" t="s">
+        <v>92</v>
+      </c>
+      <c r="K50" s="96">
+        <f>K48/K47</f>
+        <v>1.123435509896797</v>
+      </c>
+      <c r="L50">
+        <f>K50*180</f>
+        <v>202.21839178142346</v>
+      </c>
+      <c r="M50" s="95"/>
+      <c r="N50" s="95">
+        <f>L50*J34</f>
+        <v>4.0443678356284689</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>92</v>
+      </c>
+      <c r="R50" s="96">
+        <f>R48/R47</f>
+        <v>0.678558449178435</v>
+      </c>
+      <c r="S50">
+        <f>R50*180</f>
+        <v>122.1405208521183</v>
+      </c>
+      <c r="T50" s="95"/>
+      <c r="U50" s="95">
+        <f>S50*Q34</f>
+        <v>2.4428104170423661</v>
+      </c>
+      <c r="X50" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y50" s="96">
+        <f>Y48/Y47</f>
+        <v>0.233681388460073</v>
+      </c>
+      <c r="Z50">
+        <f>Y50*180</f>
+        <v>42.062649922813137</v>
+      </c>
+      <c r="AA50" s="95"/>
+      <c r="AB50" s="95">
+        <f>Z50*X34</f>
+        <v>0.84125299845626278</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D51" s="94"/>
+      <c r="F51" s="95"/>
+      <c r="G51" s="95"/>
+      <c r="K51" s="94"/>
+      <c r="M51" s="95"/>
+      <c r="N51" s="95"/>
+      <c r="R51" s="94"/>
+      <c r="T51" s="95"/>
+      <c r="U51" s="95"/>
+      <c r="Y51" s="94"/>
+      <c r="AA51" s="95"/>
+      <c r="AB51" s="95"/>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G52" s="95"/>
+      <c r="N52" s="95"/>
+      <c r="U52" s="95"/>
+      <c r="AB52" s="95"/>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D54" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E54" s="97"/>
+      <c r="F54" s="97"/>
+      <c r="K54" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L54" s="97"/>
+      <c r="M54" s="97"/>
+      <c r="R54" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S54" s="97"/>
+      <c r="T54" s="97"/>
+      <c r="Y54" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z54" s="97"/>
+      <c r="AA54" s="97"/>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D55" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E55">
+        <f>E45-D34</f>
+        <v>1.8787749999999985</v>
+      </c>
+      <c r="F55">
+        <v>1.323062</v>
+      </c>
+      <c r="K55" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L55">
+        <f>L45-K34</f>
+        <v>1.2901749999999987</v>
+      </c>
+      <c r="M55">
+        <v>1.323062</v>
+      </c>
+      <c r="R55" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S55">
+        <f>S45-R34</f>
+        <v>0.70157499999999873</v>
+      </c>
+      <c r="T55">
+        <v>1.323062</v>
+      </c>
+      <c r="Y55" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z55">
+        <f>Z45-Y34</f>
+        <v>0.11297499999999863</v>
+      </c>
+      <c r="AA55">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" s="96">
+        <f>D55+F55</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E57" s="94"/>
+      <c r="I57" t="s">
+        <v>90</v>
+      </c>
+      <c r="J57" t="s">
+        <v>88</v>
+      </c>
+      <c r="K57" s="96">
+        <f>K55+M55</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L57" s="94"/>
+      <c r="P57" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>88</v>
+      </c>
+      <c r="R57" s="96">
+        <f>R55+T55</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S57" s="94"/>
+      <c r="W57" t="s">
+        <v>90</v>
+      </c>
+      <c r="X57" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y57" s="96">
+        <f>Y55+AA55</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z57" s="94"/>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>91</v>
+      </c>
+      <c r="C58" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="96">
+        <f>E55</f>
+        <v>1.8787749999999985</v>
+      </c>
+      <c r="I58" t="s">
+        <v>91</v>
+      </c>
+      <c r="J58" t="s">
+        <v>89</v>
+      </c>
+      <c r="K58" s="96">
+        <f>L55</f>
+        <v>1.2901749999999987</v>
+      </c>
+      <c r="P58" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>89</v>
+      </c>
+      <c r="R58" s="96">
+        <f>S55</f>
+        <v>0.70157499999999873</v>
+      </c>
+      <c r="W58" t="s">
+        <v>91</v>
+      </c>
+      <c r="X58" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y58" s="96">
+        <f>Z55</f>
+        <v>0.11297499999999863</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="96">
+        <f>D58/D57</f>
+        <v>1.4200202170423715</v>
+      </c>
+      <c r="E60">
+        <f>D60*180</f>
+        <v>255.60363906762686</v>
+      </c>
+      <c r="F60" s="95"/>
+      <c r="G60" s="95">
+        <f>E60*C34</f>
+        <v>5.1120727813525368</v>
+      </c>
+      <c r="J60" t="s">
+        <v>92</v>
+      </c>
+      <c r="K60" s="96">
+        <f>K58/K57</f>
+        <v>0.97514315632400972</v>
+      </c>
+      <c r="L60">
+        <f>K60*180</f>
+        <v>175.52576813832175</v>
+      </c>
+      <c r="M60" s="95"/>
+      <c r="N60" s="95">
+        <f>L60*J34</f>
+        <v>3.5105153627664349</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>92</v>
+      </c>
+      <c r="R60" s="96">
+        <f>R58/R57</f>
+        <v>0.53026609560564764</v>
+      </c>
+      <c r="S60">
+        <f>R60*180</f>
+        <v>95.447897209016574</v>
+      </c>
+      <c r="T60" s="95"/>
+      <c r="U60" s="95">
+        <f>S60*Q34</f>
+        <v>1.9089579441803315</v>
+      </c>
+      <c r="X60" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y60" s="96">
+        <f>Y58/Y57</f>
+        <v>8.538903488728565E-2</v>
+      </c>
+      <c r="Z60">
+        <f>Y60*180</f>
+        <v>15.370026279711418</v>
+      </c>
+      <c r="AA60" s="95"/>
+      <c r="AB60" s="95">
+        <f>Z60*X34</f>
+        <v>0.30740052559422837</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G62" s="95">
+        <f>G60+G50+G41</f>
+        <v>16.937775762643717</v>
+      </c>
+      <c r="N62" s="95">
+        <f>N60+N50+N41</f>
+        <v>12.133103506885409</v>
+      </c>
+      <c r="U62" s="95">
+        <f>U60+U50+U41</f>
+        <v>7.3284312511270979</v>
+      </c>
+      <c r="AB62" s="95">
+        <f>AB60+AB50+AB41</f>
+        <v>2.5237589953687882</v>
+      </c>
+      <c r="AC62" s="95">
+        <f>SUM(G62:AB62)</f>
+        <v>38.923069516025009</v>
+      </c>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A63" s="98"/>
+      <c r="B63" s="98"/>
+      <c r="C63" s="98"/>
+      <c r="D63" s="98"/>
+      <c r="E63" s="98"/>
+      <c r="F63" s="98"/>
+      <c r="G63" s="98"/>
+      <c r="H63" s="98"/>
+      <c r="I63" s="98"/>
+      <c r="J63" s="98"/>
+      <c r="K63" s="98"/>
+      <c r="L63" s="98"/>
+      <c r="M63" s="98"/>
+      <c r="N63" s="98"/>
+      <c r="O63" s="98"/>
+      <c r="P63" s="98"/>
+      <c r="Q63" s="98"/>
+      <c r="R63" s="98"/>
+      <c r="S63" s="98"/>
+      <c r="T63" s="98"/>
+      <c r="U63" s="98"/>
+      <c r="V63" s="98"/>
+      <c r="W63" s="98"/>
+      <c r="X63" s="98"/>
+      <c r="Y63" s="98"/>
+      <c r="Z63" s="98"/>
+      <c r="AA63" s="98"/>
+      <c r="AB63" s="98"/>
+      <c r="AC63" s="98"/>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B64" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64" s="97"/>
+      <c r="D64" s="97"/>
+      <c r="I64" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="J64" s="97"/>
+      <c r="K64" s="97"/>
+      <c r="P64" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q64" s="97"/>
+      <c r="R64" s="97"/>
+      <c r="W64" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="X64" s="97"/>
+      <c r="Y64" s="97"/>
+    </row>
+    <row r="65" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>9.81</v>
+      </c>
+      <c r="C65">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="D65">
+        <f>B65*C65</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="I65">
+        <v>9.81</v>
+      </c>
+      <c r="J65">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="K65">
+        <f>I65*J65</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="P65">
+        <v>9.81</v>
+      </c>
+      <c r="Q65">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="R65">
+        <f>P65*Q65</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="W65">
+        <v>9.81</v>
+      </c>
+      <c r="X65">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="Y65">
+        <f>W65*X65</f>
+        <v>0.19620000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D66" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E66" s="97"/>
+      <c r="F66" s="97"/>
+      <c r="K66" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L66" s="97"/>
+      <c r="M66" s="97"/>
+      <c r="R66" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S66" s="97"/>
+      <c r="T66" s="97"/>
+      <c r="Y66" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z66" s="97"/>
+      <c r="AA66" s="97"/>
+    </row>
+    <row r="67" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D67" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E67">
+        <v>4.6255750000000004</v>
+      </c>
+      <c r="F67">
+        <v>1.323062</v>
+      </c>
+      <c r="K67" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L67">
+        <f>E86-K65</f>
+        <v>4.036975</v>
+      </c>
+      <c r="M67">
+        <v>1.323062</v>
+      </c>
+      <c r="R67" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S67">
+        <f>L86-R65</f>
+        <v>3.4483749999999995</v>
+      </c>
+      <c r="T67">
+        <v>1.323062</v>
+      </c>
+      <c r="Y67" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z67">
+        <f>S86-Y65</f>
+        <v>2.8597749999999991</v>
+      </c>
+      <c r="AA67">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="69" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" t="s">
+        <v>88</v>
+      </c>
+      <c r="D69" s="96">
+        <f>D67+F67</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E69" s="94"/>
+      <c r="G69" s="95"/>
+      <c r="H69" s="96"/>
+      <c r="I69" t="s">
+        <v>90</v>
+      </c>
+      <c r="J69" t="s">
+        <v>88</v>
+      </c>
+      <c r="K69" s="96">
+        <f>K67+M67</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L69" s="94"/>
+      <c r="N69" s="95"/>
+      <c r="P69" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>88</v>
+      </c>
+      <c r="R69" s="96">
+        <f>R67+T67</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S69" s="94"/>
+      <c r="U69" s="95"/>
+      <c r="W69" t="s">
+        <v>90</v>
+      </c>
+      <c r="X69" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y69" s="96">
+        <f>Y67+AA67</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z69" s="94"/>
+      <c r="AB69" s="95"/>
+    </row>
+    <row r="70" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" t="s">
+        <v>89</v>
+      </c>
+      <c r="D70" s="96">
+        <f>E67</f>
+        <v>4.6255750000000004</v>
+      </c>
+      <c r="I70" t="s">
+        <v>91</v>
+      </c>
+      <c r="J70" t="s">
+        <v>89</v>
+      </c>
+      <c r="K70" s="96">
+        <f>L67</f>
+        <v>4.036975</v>
+      </c>
+      <c r="P70" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>89</v>
+      </c>
+      <c r="R70" s="96">
+        <f>S67</f>
+        <v>3.4483749999999995</v>
+      </c>
+      <c r="W70" t="s">
+        <v>91</v>
+      </c>
+      <c r="X70" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y70" s="96">
+        <f>Z67</f>
+        <v>2.8597749999999991</v>
+      </c>
+    </row>
+    <row r="72" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" s="96">
+        <f>D70/D69</f>
+        <v>3.4961131670613956</v>
+      </c>
+      <c r="E72">
+        <f>D72*180</f>
+        <v>629.30037007105125</v>
+      </c>
+      <c r="F72" s="95"/>
+      <c r="G72" s="95">
+        <f>E72*C65</f>
+        <v>12.586007401421025</v>
+      </c>
+      <c r="J72" t="s">
+        <v>92</v>
+      </c>
+      <c r="K72" s="96">
+        <f>K70/K69</f>
+        <v>3.0512361063430333</v>
+      </c>
+      <c r="L72">
+        <f>K72*180</f>
+        <v>549.22249914174597</v>
+      </c>
+      <c r="M72" s="95"/>
+      <c r="N72" s="95">
+        <f>L72*J65</f>
+        <v>10.984449982834919</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>92</v>
+      </c>
+      <c r="R72" s="96">
+        <f>R70/R69</f>
+        <v>2.606359045624671</v>
+      </c>
+      <c r="S72">
+        <f>R72*180</f>
+        <v>469.14462821244081</v>
+      </c>
+      <c r="T72" s="95"/>
+      <c r="U72" s="95">
+        <f>S72*Q65</f>
+        <v>9.3828925642488166</v>
+      </c>
+      <c r="X72" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y72" s="96">
+        <f>Y70/Y69</f>
+        <v>2.1614819849063083</v>
+      </c>
+      <c r="Z72">
+        <f>Y72*180</f>
+        <v>389.06675728313547</v>
+      </c>
+      <c r="AA72" s="95"/>
+      <c r="AB72" s="95">
+        <f>Z72*X65</f>
+        <v>7.7813351456627098</v>
+      </c>
+    </row>
+    <row r="73" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="G73" s="95"/>
+      <c r="N73" s="95"/>
+      <c r="U73" s="95"/>
+      <c r="AB73" s="95"/>
+    </row>
+    <row r="75" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D75" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E75" s="97"/>
+      <c r="F75" s="97"/>
+      <c r="K75" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L75" s="97"/>
+      <c r="M75" s="97"/>
+      <c r="R75" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S75" s="97"/>
+      <c r="T75" s="97"/>
+      <c r="Y75" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z75" s="97"/>
+      <c r="AA75" s="97"/>
+    </row>
+    <row r="76" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D76" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E76">
+        <f>E67-D65</f>
+        <v>4.4293750000000003</v>
+      </c>
+      <c r="F76">
+        <v>1.323062</v>
+      </c>
+      <c r="K76" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L76">
+        <f>L67-K65</f>
+        <v>3.8407749999999998</v>
+      </c>
+      <c r="M76">
+        <v>1.323062</v>
+      </c>
+      <c r="R76" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S76">
+        <f>S67-R65</f>
+        <v>3.2521749999999994</v>
+      </c>
+      <c r="T76">
+        <v>1.323062</v>
+      </c>
+      <c r="Y76" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z76">
+        <f>Z67-Y65</f>
+        <v>2.6635749999999989</v>
+      </c>
+      <c r="AA76">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="78" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" t="s">
+        <v>88</v>
+      </c>
+      <c r="D78" s="96">
+        <f>D76+F76</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E78" s="94"/>
+      <c r="I78" t="s">
+        <v>90</v>
+      </c>
+      <c r="J78" t="s">
+        <v>88</v>
+      </c>
+      <c r="K78" s="96">
+        <f>K76+M76</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L78" s="94"/>
+      <c r="P78" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>88</v>
+      </c>
+      <c r="R78" s="96">
+        <f>R76+T76</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S78" s="94"/>
+      <c r="W78" t="s">
+        <v>90</v>
+      </c>
+      <c r="X78" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y78" s="96">
+        <f>Y76+AA76</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z78" s="94"/>
+    </row>
+    <row r="79" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>91</v>
+      </c>
+      <c r="C79" t="s">
+        <v>89</v>
+      </c>
+      <c r="D79" s="96">
+        <f>E76</f>
+        <v>4.4293750000000003</v>
+      </c>
+      <c r="G79" s="95"/>
+      <c r="H79" s="96"/>
+      <c r="I79" t="s">
+        <v>91</v>
+      </c>
+      <c r="J79" t="s">
+        <v>89</v>
+      </c>
+      <c r="K79" s="96">
+        <f>L76</f>
+        <v>3.8407749999999998</v>
+      </c>
+      <c r="N79" s="95"/>
+      <c r="P79" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>89</v>
+      </c>
+      <c r="R79" s="96">
+        <f>S76</f>
+        <v>3.2521749999999994</v>
+      </c>
+      <c r="U79" s="95"/>
+      <c r="W79" t="s">
+        <v>91</v>
+      </c>
+      <c r="X79" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y79" s="96">
+        <f>Z76</f>
+        <v>2.6635749999999989</v>
+      </c>
+      <c r="AB79" s="95"/>
+    </row>
+    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>92</v>
+      </c>
+      <c r="D81" s="96">
+        <f>D79/D78</f>
+        <v>3.347820813488608</v>
+      </c>
+      <c r="E81">
+        <f>D81*180</f>
+        <v>602.60774642794945</v>
+      </c>
+      <c r="F81" s="95"/>
+      <c r="G81" s="95">
+        <f>E81*C65</f>
+        <v>12.05215492855899</v>
+      </c>
+      <c r="J81" t="s">
+        <v>92</v>
+      </c>
+      <c r="K81" s="96">
+        <f>K79/K78</f>
+        <v>2.9029437527702457</v>
+      </c>
+      <c r="L81">
+        <f>K81*180</f>
+        <v>522.52987549864429</v>
+      </c>
+      <c r="M81" s="95"/>
+      <c r="N81" s="95">
+        <f>L81*J65</f>
+        <v>10.450597509972885</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>92</v>
+      </c>
+      <c r="R81" s="96">
+        <f>R79/R78</f>
+        <v>2.4580666920518834</v>
+      </c>
+      <c r="S81">
+        <f>R81*180</f>
+        <v>442.45200456933901</v>
+      </c>
+      <c r="T81" s="95"/>
+      <c r="U81" s="95">
+        <f>S81*Q65</f>
+        <v>8.8490400913867813</v>
+      </c>
+      <c r="X81" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y81" s="96">
+        <f>Y79/Y78</f>
+        <v>2.0131896313335211</v>
+      </c>
+      <c r="Z81">
+        <f>Y81*180</f>
+        <v>362.37413364003379</v>
+      </c>
+      <c r="AA81" s="95"/>
+      <c r="AB81" s="95">
+        <f>Z81*X65</f>
+        <v>7.2474826728006763</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D82" s="94"/>
+      <c r="F82" s="95"/>
+      <c r="G82" s="95"/>
+      <c r="K82" s="94"/>
+      <c r="M82" s="95"/>
+      <c r="N82" s="95"/>
+      <c r="R82" s="94"/>
+      <c r="T82" s="95"/>
+      <c r="U82" s="95"/>
+      <c r="Y82" s="94"/>
+      <c r="AA82" s="95"/>
+      <c r="AB82" s="95"/>
+    </row>
+    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G83" s="95"/>
+      <c r="N83" s="95"/>
+      <c r="U83" s="95"/>
+      <c r="AB83" s="95"/>
+    </row>
+    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D85" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E85" s="97"/>
+      <c r="F85" s="97"/>
+      <c r="K85" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L85" s="97"/>
+      <c r="M85" s="97"/>
+      <c r="R85" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S85" s="97"/>
+      <c r="T85" s="97"/>
+      <c r="Y85" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z85" s="97"/>
+      <c r="AA85" s="97"/>
+    </row>
+    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D86" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E86">
+        <f>E76-D65</f>
+        <v>4.2331750000000001</v>
+      </c>
+      <c r="F86">
+        <v>1.323062</v>
+      </c>
+      <c r="K86" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L86">
+        <f>L76-K65</f>
+        <v>3.6445749999999997</v>
+      </c>
+      <c r="M86">
+        <v>1.323062</v>
+      </c>
+      <c r="R86" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S86">
+        <f>S76-R65</f>
+        <v>3.0559749999999992</v>
+      </c>
+      <c r="T86">
+        <v>1.323062</v>
+      </c>
+      <c r="Y86" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z86">
+        <f>Z76-Y65</f>
+        <v>2.4673749999999988</v>
+      </c>
+      <c r="AA86">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+      <c r="C88" t="s">
+        <v>88</v>
+      </c>
+      <c r="D88" s="96">
+        <f>D86+F86</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E88" s="94"/>
+      <c r="I88" t="s">
+        <v>90</v>
+      </c>
+      <c r="J88" t="s">
+        <v>88</v>
+      </c>
+      <c r="K88" s="96">
+        <f>K86+M86</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L88" s="94"/>
+      <c r="P88" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>88</v>
+      </c>
+      <c r="R88" s="96">
+        <f>R86+T86</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S88" s="94"/>
+      <c r="W88" t="s">
+        <v>90</v>
+      </c>
+      <c r="X88" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y88" s="96">
+        <f>Y86+AA86</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z88" s="94"/>
+    </row>
+    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89" t="s">
+        <v>89</v>
+      </c>
+      <c r="D89" s="96">
+        <f>E86</f>
+        <v>4.2331750000000001</v>
+      </c>
+      <c r="I89" t="s">
+        <v>91</v>
+      </c>
+      <c r="J89" t="s">
+        <v>89</v>
+      </c>
+      <c r="K89" s="96">
+        <f>L86</f>
+        <v>3.6445749999999997</v>
+      </c>
+      <c r="P89" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>89</v>
+      </c>
+      <c r="R89" s="96">
+        <f>S86</f>
+        <v>3.0559749999999992</v>
+      </c>
+      <c r="W89" t="s">
+        <v>91</v>
+      </c>
+      <c r="X89" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y89" s="96">
+        <f>Z86</f>
+        <v>2.4673749999999988</v>
+      </c>
+    </row>
+    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>92</v>
+      </c>
+      <c r="D91" s="96">
+        <f>D89/D88</f>
+        <v>3.1995284599158205</v>
+      </c>
+      <c r="E91">
+        <f>D91*180</f>
+        <v>575.91512278484765</v>
+      </c>
+      <c r="F91" s="95"/>
+      <c r="G91" s="95">
+        <f>E91*C65</f>
+        <v>11.518302455696952</v>
+      </c>
+      <c r="J91" t="s">
+        <v>92</v>
+      </c>
+      <c r="K91" s="96">
+        <f>K89/K88</f>
+        <v>2.7546513991974582</v>
+      </c>
+      <c r="L91">
+        <f>K91*180</f>
+        <v>495.83725185554249</v>
+      </c>
+      <c r="M91" s="95"/>
+      <c r="N91" s="95">
+        <f>L91*J65</f>
+        <v>9.9167450371108501</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>92</v>
+      </c>
+      <c r="R91" s="96">
+        <f>R89/R88</f>
+        <v>2.3097743384790959</v>
+      </c>
+      <c r="S91">
+        <f>R91*180</f>
+        <v>415.75938092623727</v>
+      </c>
+      <c r="T91" s="95"/>
+      <c r="U91" s="95">
+        <f>S91*Q65</f>
+        <v>8.315187618524746</v>
+      </c>
+      <c r="X91" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y91" s="96">
+        <f>Y89/Y88</f>
+        <v>1.8648972777607336</v>
+      </c>
+      <c r="Z91">
+        <f>Y91*180</f>
+        <v>335.68150999693205</v>
+      </c>
+      <c r="AA91" s="95"/>
+      <c r="AB91" s="95">
+        <f>Z91*X65</f>
+        <v>6.713630199938641</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G93" s="95">
+        <f>G91+G81+G72</f>
+        <v>36.156464785676967</v>
+      </c>
+      <c r="N93" s="95">
+        <f>N91+N81+N72</f>
+        <v>31.351792529918654</v>
+      </c>
+      <c r="U93" s="95">
+        <f>U91+U81+U72</f>
+        <v>26.547120274160346</v>
+      </c>
+      <c r="AB93" s="95">
+        <f>AB91+AB81+AB72</f>
+        <v>21.742448018402026</v>
+      </c>
+      <c r="AC93" s="95">
+        <f>SUM(G93:AB93)</f>
+        <v>115.79782560815799</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A94" s="98"/>
+      <c r="B94" s="98"/>
+      <c r="C94" s="98"/>
+      <c r="D94" s="98"/>
+      <c r="E94" s="98"/>
+      <c r="F94" s="98"/>
+      <c r="G94" s="98"/>
+      <c r="H94" s="98"/>
+      <c r="I94" s="98"/>
+      <c r="J94" s="98"/>
+      <c r="K94" s="98"/>
+      <c r="L94" s="98"/>
+      <c r="M94" s="98"/>
+      <c r="N94" s="98"/>
+      <c r="O94" s="98"/>
+      <c r="P94" s="98"/>
+      <c r="Q94" s="98"/>
+      <c r="R94" s="98"/>
+      <c r="S94" s="98"/>
+      <c r="T94" s="98"/>
+      <c r="U94" s="98"/>
+      <c r="V94" s="98"/>
+      <c r="W94" s="98"/>
+      <c r="X94" s="98"/>
+      <c r="Y94" s="98"/>
+      <c r="Z94" s="98"/>
+      <c r="AA94" s="98"/>
+      <c r="AB94" s="98"/>
+      <c r="AC94" s="98"/>
+    </row>
+    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B95" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="C95" s="97"/>
+      <c r="D95" s="97"/>
+      <c r="I95" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="J95" s="97"/>
+      <c r="K95" s="97"/>
+      <c r="P95" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q95" s="97"/>
+      <c r="R95" s="97"/>
+      <c r="W95" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="X95" s="97"/>
+      <c r="Y95" s="97"/>
+    </row>
+    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>9.81</v>
+      </c>
+      <c r="C96">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="D96">
+        <f>B96*C96</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="I96">
+        <v>9.81</v>
+      </c>
+      <c r="J96">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="K96">
+        <f>I96*J96</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="P96">
+        <v>9.81</v>
+      </c>
+      <c r="Q96">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="R96">
+        <f>P96*Q96</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="W96">
+        <v>9.81</v>
+      </c>
+      <c r="X96">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="Y96">
+        <f>W96*X96</f>
+        <v>0.19620000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D97" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E97" s="97"/>
+      <c r="F97" s="97"/>
+      <c r="K97" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L97" s="97"/>
+      <c r="M97" s="97"/>
+      <c r="R97" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S97" s="97"/>
+      <c r="T97" s="97"/>
+      <c r="Y97" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z97" s="97"/>
+      <c r="AA97" s="97"/>
+    </row>
+    <row r="98" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D98" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E98">
+        <f>Z86-D96</f>
+        <v>2.2711749999999986</v>
+      </c>
+      <c r="F98">
+        <v>1.323062</v>
+      </c>
+      <c r="K98" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L98">
+        <f>E117-K96</f>
+        <v>1.6825749999999986</v>
+      </c>
+      <c r="M98">
+        <v>1.323062</v>
+      </c>
+      <c r="R98" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S98">
+        <f>L117-R96</f>
+        <v>1.0939749999999988</v>
+      </c>
+      <c r="T98">
+        <v>1.323062</v>
+      </c>
+      <c r="Y98" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z98">
+        <f>S117-Y96</f>
+        <v>0.50537499999999869</v>
+      </c>
+      <c r="AA98">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="100" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>90</v>
+      </c>
+      <c r="C100" t="s">
+        <v>88</v>
+      </c>
+      <c r="D100" s="96">
+        <f>D98+F98</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E100" s="94"/>
+      <c r="G100" s="95"/>
+      <c r="H100" s="96"/>
+      <c r="I100" t="s">
+        <v>90</v>
+      </c>
+      <c r="J100" t="s">
+        <v>88</v>
+      </c>
+      <c r="K100" s="96">
+        <f>K98+M98</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L100" s="94"/>
+      <c r="N100" s="95"/>
+      <c r="P100" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>88</v>
+      </c>
+      <c r="R100" s="96">
+        <f>R98+T98</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S100" s="94"/>
+      <c r="U100" s="95"/>
+      <c r="W100" t="s">
+        <v>90</v>
+      </c>
+      <c r="X100" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y100" s="96">
+        <f>Y98+AA98</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z100" s="94"/>
+      <c r="AB100" s="95"/>
+    </row>
+    <row r="101" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>91</v>
+      </c>
+      <c r="C101" t="s">
+        <v>89</v>
+      </c>
+      <c r="D101" s="96">
+        <f>E98</f>
+        <v>2.2711749999999986</v>
+      </c>
+      <c r="I101" t="s">
+        <v>91</v>
+      </c>
+      <c r="J101" t="s">
+        <v>89</v>
+      </c>
+      <c r="K101" s="96">
+        <f>L98</f>
+        <v>1.6825749999999986</v>
+      </c>
+      <c r="P101" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>89</v>
+      </c>
+      <c r="R101" s="96">
+        <f>S98</f>
+        <v>1.0939749999999988</v>
+      </c>
+      <c r="W101" t="s">
+        <v>91</v>
+      </c>
+      <c r="X101" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y101" s="96">
+        <f>Z98</f>
+        <v>0.50537499999999869</v>
+      </c>
+    </row>
+    <row r="103" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>92</v>
+      </c>
+      <c r="D103" s="96">
+        <f>D101/D100</f>
+        <v>1.7166049241879462</v>
+      </c>
+      <c r="E103">
+        <f>D103*180</f>
+        <v>308.98888635383031</v>
+      </c>
+      <c r="F103" s="95"/>
+      <c r="G103" s="95">
+        <f>E103*C96</f>
+        <v>6.1797777270766066</v>
+      </c>
+      <c r="J103" t="s">
+        <v>92</v>
+      </c>
+      <c r="K103" s="96">
+        <f>K101/K100</f>
+        <v>1.2717278634695841</v>
+      </c>
+      <c r="L103">
+        <f>K103*180</f>
+        <v>228.91101542452515</v>
+      </c>
+      <c r="M103" s="95"/>
+      <c r="N103" s="95">
+        <f>L103*J96</f>
+        <v>4.5782203084905033</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>92</v>
+      </c>
+      <c r="R103" s="96">
+        <f>R101/R100</f>
+        <v>0.82685080275122236</v>
+      </c>
+      <c r="S103">
+        <f>R103*180</f>
+        <v>148.83314449522001</v>
+      </c>
+      <c r="T103" s="95"/>
+      <c r="U103" s="95">
+        <f>S103*Q96</f>
+        <v>2.9766628899044001</v>
+      </c>
+      <c r="X103" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y103" s="96">
+        <f>Y101/Y100</f>
+        <v>0.38197374203286033</v>
+      </c>
+      <c r="Z103">
+        <f>Y103*180</f>
+        <v>68.755273565914862</v>
+      </c>
+      <c r="AA103" s="95"/>
+      <c r="AB103" s="95">
+        <f>Z103*X96</f>
+        <v>1.3751054713182973</v>
+      </c>
+    </row>
+    <row r="104" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="G104" s="95"/>
+      <c r="N104" s="95"/>
+      <c r="U104" s="95"/>
+      <c r="AB104" s="95"/>
+    </row>
+    <row r="106" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D106" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E106" s="97"/>
+      <c r="F106" s="97"/>
+      <c r="K106" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L106" s="97"/>
+      <c r="M106" s="97"/>
+      <c r="R106" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S106" s="97"/>
+      <c r="T106" s="97"/>
+      <c r="Y106" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z106" s="97"/>
+      <c r="AA106" s="97"/>
+    </row>
+    <row r="107" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D107" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E107">
+        <f>E98-D96</f>
+        <v>2.0749749999999985</v>
+      </c>
+      <c r="F107">
+        <v>1.323062</v>
+      </c>
+      <c r="K107" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L107">
+        <f>L98-K96</f>
+        <v>1.4863749999999987</v>
+      </c>
+      <c r="M107">
+        <v>1.323062</v>
+      </c>
+      <c r="R107" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S107">
+        <f>S98-R96</f>
+        <v>0.89777499999999877</v>
+      </c>
+      <c r="T107">
+        <v>1.323062</v>
+      </c>
+      <c r="Y107" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z107">
+        <f>Z98-Y96</f>
+        <v>0.30917499999999865</v>
+      </c>
+      <c r="AA107">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="109" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>90</v>
+      </c>
+      <c r="C109" t="s">
+        <v>88</v>
+      </c>
+      <c r="D109" s="96">
+        <f>D107+F107</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E109" s="94"/>
+      <c r="I109" t="s">
+        <v>90</v>
+      </c>
+      <c r="J109" t="s">
+        <v>88</v>
+      </c>
+      <c r="K109" s="96">
+        <f>K107+M107</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L109" s="94"/>
+      <c r="P109" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>88</v>
+      </c>
+      <c r="R109" s="96">
+        <f>R107+T107</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S109" s="94"/>
+      <c r="W109" t="s">
+        <v>90</v>
+      </c>
+      <c r="X109" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y109" s="96">
+        <f>Y107+AA107</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z109" s="94"/>
+    </row>
+    <row r="110" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>91</v>
+      </c>
+      <c r="C110" t="s">
+        <v>89</v>
+      </c>
+      <c r="D110" s="96">
+        <f>E107</f>
+        <v>2.0749749999999985</v>
+      </c>
+      <c r="G110" s="95"/>
+      <c r="H110" s="96"/>
+      <c r="I110" t="s">
+        <v>91</v>
+      </c>
+      <c r="J110" t="s">
+        <v>89</v>
+      </c>
+      <c r="K110" s="96">
+        <f>L107</f>
+        <v>1.4863749999999987</v>
+      </c>
+      <c r="N110" s="95"/>
+      <c r="P110" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>89</v>
+      </c>
+      <c r="R110" s="96">
+        <f>S107</f>
+        <v>0.89777499999999877</v>
+      </c>
+      <c r="U110" s="95"/>
+      <c r="W110" t="s">
+        <v>91</v>
+      </c>
+      <c r="X110" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y110" s="96">
+        <f>Z107</f>
+        <v>0.30917499999999865</v>
+      </c>
+      <c r="AB110" s="95"/>
+    </row>
+    <row r="112" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>92</v>
+      </c>
+      <c r="D112" s="96">
+        <f>D110/D109</f>
+        <v>1.5683125706151588</v>
+      </c>
+      <c r="E112">
+        <f>D112*180</f>
+        <v>282.29626271072857</v>
+      </c>
+      <c r="F112" s="95"/>
+      <c r="G112" s="95">
+        <f>E112*C96</f>
+        <v>5.6459252542145713</v>
+      </c>
+      <c r="J112" t="s">
+        <v>92</v>
+      </c>
+      <c r="K112" s="96">
+        <f>K110/K109</f>
+        <v>1.123435509896797</v>
+      </c>
+      <c r="L112">
+        <f>K112*180</f>
+        <v>202.21839178142346</v>
+      </c>
+      <c r="M112" s="95"/>
+      <c r="N112" s="95">
+        <f>L112*J96</f>
+        <v>4.0443678356284689</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>92</v>
+      </c>
+      <c r="R112" s="96">
+        <f>R110/R109</f>
+        <v>0.678558449178435</v>
+      </c>
+      <c r="S112">
+        <f>R112*180</f>
+        <v>122.1405208521183</v>
+      </c>
+      <c r="T112" s="95"/>
+      <c r="U112" s="95">
+        <f>S112*Q96</f>
+        <v>2.4428104170423661</v>
+      </c>
+      <c r="X112" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y112" s="96">
+        <f>Y110/Y109</f>
+        <v>0.233681388460073</v>
+      </c>
+      <c r="Z112">
+        <f>Y112*180</f>
+        <v>42.062649922813137</v>
+      </c>
+      <c r="AA112" s="95"/>
+      <c r="AB112" s="95">
+        <f>Z112*X96</f>
+        <v>0.84125299845626278</v>
+      </c>
+    </row>
+    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D113" s="94"/>
+      <c r="F113" s="95"/>
+      <c r="G113" s="95"/>
+      <c r="K113" s="94"/>
+      <c r="M113" s="95"/>
+      <c r="N113" s="95"/>
+      <c r="R113" s="94"/>
+      <c r="T113" s="95"/>
+      <c r="U113" s="95"/>
+      <c r="Y113" s="94"/>
+      <c r="AA113" s="95"/>
+      <c r="AB113" s="95"/>
+    </row>
+    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G114" s="95"/>
+      <c r="N114" s="95"/>
+      <c r="U114" s="95"/>
+      <c r="AB114" s="95"/>
+    </row>
+    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D116" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="E116" s="97"/>
+      <c r="F116" s="97"/>
+      <c r="K116" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="L116" s="97"/>
+      <c r="M116" s="97"/>
+      <c r="R116" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S116" s="97"/>
+      <c r="T116" s="97"/>
+      <c r="Y116" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z116" s="97"/>
+      <c r="AA116" s="97"/>
+    </row>
+    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D117" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="E117">
+        <f>E107-D96</f>
+        <v>1.8787749999999985</v>
+      </c>
+      <c r="F117">
+        <v>1.323062</v>
+      </c>
+      <c r="K117" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="L117">
+        <f>L107-K96</f>
+        <v>1.2901749999999987</v>
+      </c>
+      <c r="M117">
+        <v>1.323062</v>
+      </c>
+      <c r="R117" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="S117">
+        <f>S107-R96</f>
+        <v>0.70157499999999873</v>
+      </c>
+      <c r="T117">
+        <v>1.323062</v>
+      </c>
+      <c r="Y117" s="93">
+        <v>1.4901159999999999E-7</v>
+      </c>
+      <c r="Z117">
+        <f>Z107-Y96</f>
+        <v>0.11297499999999863</v>
+      </c>
+      <c r="AA117">
+        <v>1.323062</v>
+      </c>
+    </row>
+    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>90</v>
+      </c>
+      <c r="C119" t="s">
+        <v>88</v>
+      </c>
+      <c r="D119" s="96">
+        <f>D117+F117</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="E119" s="94"/>
+      <c r="I119" t="s">
+        <v>90</v>
+      </c>
+      <c r="J119" t="s">
+        <v>88</v>
+      </c>
+      <c r="K119" s="96">
+        <f>K117+M117</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="L119" s="94"/>
+      <c r="P119" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>88</v>
+      </c>
+      <c r="R119" s="96">
+        <f>R117+T117</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="S119" s="94"/>
+      <c r="W119" t="s">
+        <v>90</v>
+      </c>
+      <c r="X119" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y119" s="96">
+        <f>Y117+AA117</f>
+        <v>1.3230621490115999</v>
+      </c>
+      <c r="Z119" s="94"/>
+    </row>
+    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>91</v>
+      </c>
+      <c r="C120" t="s">
+        <v>89</v>
+      </c>
+      <c r="D120" s="96">
+        <f>E117</f>
+        <v>1.8787749999999985</v>
+      </c>
+      <c r="I120" t="s">
+        <v>91</v>
+      </c>
+      <c r="J120" t="s">
+        <v>89</v>
+      </c>
+      <c r="K120" s="96">
+        <f>L117</f>
+        <v>1.2901749999999987</v>
+      </c>
+      <c r="P120" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>89</v>
+      </c>
+      <c r="R120" s="96">
+        <f>S117</f>
+        <v>0.70157499999999873</v>
+      </c>
+      <c r="W120" t="s">
+        <v>91</v>
+      </c>
+      <c r="X120" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y120" s="96">
+        <f>Z117</f>
+        <v>0.11297499999999863</v>
+      </c>
+    </row>
+    <row r="122" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>92</v>
+      </c>
+      <c r="D122" s="96">
+        <f>D120/D119</f>
+        <v>1.4200202170423715</v>
+      </c>
+      <c r="E122">
+        <f>D122*180</f>
+        <v>255.60363906762686</v>
+      </c>
+      <c r="F122" s="95"/>
+      <c r="G122" s="95">
+        <f>E122*C96</f>
+        <v>5.1120727813525368</v>
+      </c>
+      <c r="J122" t="s">
+        <v>92</v>
+      </c>
+      <c r="K122" s="96">
+        <f>K120/K119</f>
+        <v>0.97514315632400972</v>
+      </c>
+      <c r="L122">
+        <f>K122*180</f>
+        <v>175.52576813832175</v>
+      </c>
+      <c r="M122" s="95"/>
+      <c r="N122" s="95">
+        <f>L122*J96</f>
+        <v>3.5105153627664349</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>92</v>
+      </c>
+      <c r="R122" s="96">
+        <f>R120/R119</f>
+        <v>0.53026609560564764</v>
+      </c>
+      <c r="S122">
+        <f>R122*180</f>
+        <v>95.447897209016574</v>
+      </c>
+      <c r="T122" s="95"/>
+      <c r="U122" s="95">
+        <f>S122*Q96</f>
+        <v>1.9089579441803315</v>
+      </c>
+      <c r="X122" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y122" s="96">
+        <f>Y120/Y119</f>
+        <v>8.538903488728565E-2</v>
+      </c>
+      <c r="Z122">
+        <f>Y122*180</f>
+        <v>15.370026279711418</v>
+      </c>
+      <c r="AA122" s="95"/>
+      <c r="AB122" s="95">
+        <f>Z122*X96</f>
+        <v>0.30740052559422837</v>
+      </c>
+    </row>
+    <row r="124" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="G124" s="95">
+        <f>G122+G112+G103</f>
+        <v>16.937775762643717</v>
+      </c>
+      <c r="N124" s="95">
+        <f>N122+N112+N103</f>
+        <v>12.133103506885409</v>
+      </c>
+      <c r="U124" s="95">
+        <f>U122+U112+U103</f>
+        <v>7.3284312511270979</v>
+      </c>
+      <c r="AB124" s="95">
+        <f>AB122+AB112+AB103</f>
+        <v>2.5237589953687882</v>
+      </c>
+      <c r="AC124" s="95">
+        <f>SUM(G124:AB124)</f>
+        <v>38.923069516025009</v>
+      </c>
+    </row>
+    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A125" s="98"/>
+      <c r="B125" s="98"/>
+      <c r="C125" s="98"/>
+      <c r="D125" s="98"/>
+      <c r="E125" s="98"/>
+      <c r="F125" s="98"/>
+      <c r="G125" s="98"/>
+      <c r="H125" s="98"/>
+      <c r="I125" s="98"/>
+      <c r="J125" s="98"/>
+      <c r="K125" s="98"/>
+      <c r="L125" s="98"/>
+      <c r="M125" s="98"/>
+      <c r="N125" s="98"/>
+      <c r="O125" s="98"/>
+      <c r="P125" s="98"/>
+      <c r="Q125" s="98"/>
+      <c r="R125" s="98"/>
+      <c r="S125" s="98"/>
+      <c r="T125" s="98"/>
+      <c r="U125" s="98"/>
+      <c r="V125" s="98"/>
+      <c r="W125" s="98"/>
+      <c r="X125" s="98"/>
+      <c r="Y125" s="98"/>
+      <c r="Z125" s="98"/>
+      <c r="AA125" s="98"/>
+      <c r="AB125" s="98"/>
+      <c r="AC125" s="98"/>
+    </row>
+  </sheetData>
+  <mergeCells count="64">
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="K106:M106"/>
+    <mergeCell ref="R106:T106"/>
+    <mergeCell ref="Y106:AA106"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="K116:M116"/>
+    <mergeCell ref="R116:T116"/>
+    <mergeCell ref="Y116:AA116"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="I95:K95"/>
+    <mergeCell ref="P95:R95"/>
+    <mergeCell ref="W95:Y95"/>
+    <mergeCell ref="D97:F97"/>
+    <mergeCell ref="K97:M97"/>
+    <mergeCell ref="R97:T97"/>
+    <mergeCell ref="Y97:AA97"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="K75:M75"/>
+    <mergeCell ref="R75:T75"/>
+    <mergeCell ref="Y75:AA75"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="K85:M85"/>
+    <mergeCell ref="R85:T85"/>
+    <mergeCell ref="Y85:AA85"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="I64:K64"/>
+    <mergeCell ref="P64:R64"/>
+    <mergeCell ref="W64:Y64"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="K66:M66"/>
+    <mergeCell ref="R66:T66"/>
+    <mergeCell ref="Y66:AA66"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="Y44:AA44"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="K54:M54"/>
+    <mergeCell ref="R54:T54"/>
+    <mergeCell ref="Y54:AA54"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="W33:Y33"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="R35:T35"/>
+    <mergeCell ref="Y35:AA35"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="R23:T23"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K23:M23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed rotation again :S
</commit_message>
<xml_diff>
--- a/TODO altCtrlPancake.xlsx
+++ b/TODO altCtrlPancake.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ashley Sands\Amstrike Games\SimPancake3000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1542D288-9E38-453D-BB91-44C6AC4F9DE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EBF4E1-9A34-454B-858C-14810FB5F758}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6732AF01-4E77-4178-A282-B4B033BA40EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6732AF01-4E77-4178-A282-B4B033BA40EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="105">
   <si>
     <t>Project Sheet - Summary</t>
   </si>
@@ -342,16 +342,38 @@
   <si>
     <t>Level out pancake once below rotate thresshold</t>
   </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>x*z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight the pancake joints </t>
+  </si>
+  <si>
+    <t>I think this is caused during the pan changes, if shaky with the jug.</t>
+  </si>
+  <si>
+    <t>Fix TransformToUpforce excepting every value.</t>
+  </si>
+  <si>
+    <t>it should only except the first and any that are thurther away from the center</t>
+  </si>
+  <si>
+    <t>?? Maybe. This seams to of fixed since fixing other bugs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.000E+00"/>
+    <numFmt numFmtId="178" formatCode="0.0000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -758,7 +780,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -934,12 +956,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1195,16 +1228,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1219,32 +1242,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B2D132A-8E44-48F1-BBB2-2C53A683D787}" name="Main" displayName="Main" ref="A3:G50" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B2D132A-8E44-48F1-BBB2-2C53A683D787}" name="Main" displayName="Main" ref="A3:G50" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A3:G50" xr:uid="{041E981F-6BC0-4FDE-ACBA-E530F1EEC1B5}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{824F3C5E-1D9A-43A1-B8C9-BD326514D302}" name="ID" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{1150AD6D-6BBD-4CBF-9E9A-9902A96F9F82}" name="Task Name" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{F083697A-B89D-45BD-9721-20A038AAB4B0}" name="Task Details" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{85C72231-B520-4C6B-9B33-80C7B98FAEAF}" name="Status" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{4B87CB35-1B38-4C75-BBE3-CA245029C4B8}" name="Group" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{B40BFB71-0609-470A-9EAD-D610C0B87C75}" name="Sub Group" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{23817CE4-D3E3-4F39-ABA0-28388712A836}" name="Notes" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{824F3C5E-1D9A-43A1-B8C9-BD326514D302}" name="ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{1150AD6D-6BBD-4CBF-9E9A-9902A96F9F82}" name="Task Name" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{F083697A-B89D-45BD-9721-20A038AAB4B0}" name="Task Details" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{85C72231-B520-4C6B-9B33-80C7B98FAEAF}" name="Status" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{4B87CB35-1B38-4C75-BBE3-CA245029C4B8}" name="Group" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{B40BFB71-0609-470A-9EAD-D610C0B87C75}" name="Sub Group" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{23817CE4-D3E3-4F39-ABA0-28388712A836}" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60864319-97C2-48A4-B74F-713E907C5D25}" name="Arduino" displayName="Arduino" ref="A3:G50" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60864319-97C2-48A4-B74F-713E907C5D25}" name="Arduino" displayName="Arduino" ref="A3:G50" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A3:G50" xr:uid="{041E981F-6BC0-4FDE-ACBA-E530F1EEC1B5}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{12C5545D-8B1E-4FB2-8748-F7DBD896D325}" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{8D4C031C-DE34-4573-B782-3D586DEEE833}" name="Task Name" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{A2A6B64D-29D1-48FF-A65C-BA0EBD121B5B}" name="Task Details" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{45A6DF31-36F1-4C08-B878-330C15541E2C}" name="Status" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E20DE365-0A63-46A6-B55D-5E36FCC83D00}" name="Group" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{A90C5265-ADB6-421D-9C00-5E9716201C56}" name="Sub Group" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{92972826-2FDE-4271-B1AE-3D18F97AB66D}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{12C5545D-8B1E-4FB2-8748-F7DBD896D325}" name="ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8D4C031C-DE34-4573-B782-3D586DEEE833}" name="Task Name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{A2A6B64D-29D1-48FF-A65C-BA0EBD121B5B}" name="Task Details" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{45A6DF31-36F1-4C08-B878-330C15541E2C}" name="Status" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E20DE365-0A63-46A6-B55D-5E36FCC83D00}" name="Group" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A90C5265-ADB6-421D-9C00-5E9716201C56}" name="Sub Group" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{92972826-2FDE-4271-B1AE-3D18F97AB66D}" name="Notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1668,7 +1691,7 @@
       </c>
       <c r="C9" s="14">
         <f>C17+C18+C19+G17+G18+G19</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>11</v>
@@ -1682,14 +1705,14 @@
       </c>
       <c r="G9" s="14">
         <f>C9+E9</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="17">
         <f>C15+G15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1698,14 +1721,14 @@
       </c>
       <c r="C10" s="18">
         <f>C9/G9</f>
-        <v>0.12903225806451613</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="19">
         <f>E9/G9</f>
-        <v>0.87096774193548387</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>14</v>
@@ -1719,7 +1742,7 @@
       </c>
       <c r="I10" s="21">
         <f>I9/G9</f>
-        <v>3.2258064516129031E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1759,11 +1782,11 @@
       </c>
       <c r="C14" s="24">
         <f>COUNTIF(Main[Status], "-")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="25">
         <f>C14/C20</f>
-        <v>0.95652173913043481</v>
+        <v>0.92</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="23" t="s">
@@ -1775,7 +1798,7 @@
       </c>
       <c r="H14" s="25">
         <f>G14/G20</f>
-        <v>0.17391304347826086</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1784,11 +1807,11 @@
       </c>
       <c r="C15" s="24">
         <f>COUNTIF(Main[Status], "wip")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="25">
         <f>C15/C20</f>
-        <v>4.3478260869565216E-2</v>
+        <v>0</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="23" t="s">
@@ -1850,7 +1873,7 @@
       </c>
       <c r="H17" s="25">
         <f>G17/G20</f>
-        <v>0.17391304347826086</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1884,11 +1907,11 @@
       </c>
       <c r="C19" s="24">
         <f>COUNTIF(Main[Status], "fixed")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19" s="26">
         <f>C19/C20</f>
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="23" t="s">
@@ -1909,7 +1932,7 @@
       </c>
       <c r="C20" s="28">
         <f>COUNTA(Main[Status])</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D20" s="29">
         <f>SUM(D14:D19)</f>
@@ -1921,11 +1944,11 @@
       </c>
       <c r="G20" s="28">
         <f>COUNTA(Main[Status])</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H20" s="29">
         <f>SUM(H14:H19)</f>
-        <v>0.34782608695652173</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1934,14 +1957,14 @@
       </c>
       <c r="C21" s="30">
         <f>D14+D15+D16</f>
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="30">
         <f>H14+H15+H16</f>
-        <v>0.17391304347826086</v>
+        <v>0.16</v>
       </c>
       <c r="S21" s="67"/>
     </row>
@@ -1951,14 +1974,14 @@
       </c>
       <c r="C22" s="32">
         <f>D17+D18+D19</f>
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="F22" s="31" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="32">
         <f>H17+H18+H19</f>
-        <v>0.17391304347826086</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2389,7 +2412,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>$C$10</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2423,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BDFBF0-BDE3-48CD-9C74-022AECEC1124}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2534,7 +2557,7 @@
       </c>
       <c r="G7" s="74"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="73">
         <v>4</v>
       </c>
@@ -2545,7 +2568,9 @@
       <c r="D8" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="74"/>
+      <c r="G8" s="74" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="73">
@@ -2625,7 +2650,9 @@
       <c r="D14" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="74"/>
+      <c r="G14" s="74" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="73">
@@ -2748,7 +2775,7 @@
       </c>
       <c r="C23" s="74"/>
       <c r="D23" s="73" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G23" s="74"/>
     </row>
@@ -2795,16 +2822,28 @@
       <c r="A27" s="73">
         <v>23</v>
       </c>
-      <c r="B27" s="74"/>
+      <c r="B27" s="74" t="s">
+        <v>100</v>
+      </c>
       <c r="C27" s="74"/>
+      <c r="D27" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G27" s="74"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="73">
         <v>24</v>
       </c>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
+      <c r="B28" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="73" t="s">
+        <v>22</v>
+      </c>
       <c r="G28" s="74"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -3121,37 +3160,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A58165-66D3-4FDC-A087-9321E2B81B62}">
-  <dimension ref="A2:AC125"/>
+  <dimension ref="A1:AC125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <v>629.29999999999995</v>
+      </c>
+    </row>
     <row r="2" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B2" s="97" t="s">
         <v>86</v>
       </c>
       <c r="C2" s="97"/>
       <c r="D2" s="97"/>
-      <c r="I2" s="97" t="s">
+      <c r="J2" s="97" t="s">
         <v>86</v>
       </c>
-      <c r="J2" s="97"/>
       <c r="K2" s="97"/>
+      <c r="L2" s="97"/>
       <c r="P2" s="97" t="s">
         <v>86</v>
       </c>
       <c r="Q2" s="97"/>
       <c r="R2" s="97"/>
-      <c r="W2" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="T2" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2">
+        <v>90</v>
+      </c>
+      <c r="W2" s="97"/>
       <c r="X2" s="97"/>
       <c r="Y2" s="97"/>
     </row>
@@ -3167,15 +3217,15 @@
         <f>B3*C3</f>
         <v>0.19620000000000001</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>9.81</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f>1/50</f>
         <v>0.02</v>
       </c>
-      <c r="K3">
-        <f>I3*J3</f>
+      <c r="L3">
+        <f>J3*K3</f>
         <v>0.19620000000000001</v>
       </c>
       <c r="P3">
@@ -3189,17 +3239,6 @@
         <f>P3*Q3</f>
         <v>0.19620000000000001</v>
       </c>
-      <c r="W3">
-        <v>9.81</v>
-      </c>
-      <c r="X3">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="Y3">
-        <f>W3*X3</f>
-        <v>0.19620000000000001</v>
-      </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D4" s="97" t="s">
@@ -3207,62 +3246,49 @@
       </c>
       <c r="E4" s="97"/>
       <c r="F4" s="97"/>
-      <c r="K4" s="97" t="s">
+      <c r="L4" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="L4" s="97"/>
       <c r="M4" s="97"/>
+      <c r="N4" s="97"/>
       <c r="R4" s="97" t="s">
         <v>87</v>
       </c>
       <c r="S4" s="97"/>
       <c r="T4" s="97"/>
-      <c r="Y4" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y4" s="97"/>
       <c r="Z4" s="97"/>
       <c r="AA4" s="97"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D5" s="93">
-        <v>1.4901159999999999E-7</v>
+        <v>-1.3187679999999999</v>
       </c>
       <c r="E5">
+        <v>7.2</v>
+      </c>
+      <c r="F5">
+        <v>2.7384539999999999</v>
+      </c>
+      <c r="L5" s="93">
+        <v>1.3187679999999999</v>
+      </c>
+      <c r="M5">
+        <v>7.2</v>
+      </c>
+      <c r="N5">
+        <v>2.7384539999999999</v>
+      </c>
+      <c r="R5" s="93">
+        <v>1.49E-7</v>
+      </c>
+      <c r="S5">
         <v>4.6255750000000004</v>
-      </c>
-      <c r="F5">
-        <v>1.323062</v>
-      </c>
-      <c r="K5" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L5">
-        <f>E24-K3</f>
-        <v>4.036975</v>
-      </c>
-      <c r="M5">
-        <v>1.323062</v>
-      </c>
-      <c r="R5" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S5">
-        <f>L24-R3</f>
-        <v>3.4483749999999995</v>
       </c>
       <c r="T5">
         <v>1.323062</v>
       </c>
-      <c r="Y5" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z5">
-        <f>S24-Y3</f>
-        <v>2.8597749999999991</v>
-      </c>
-      <c r="AA5">
-        <v>1.323062</v>
-      </c>
+      <c r="Y5" s="93"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -3273,45 +3299,36 @@
       </c>
       <c r="D7" s="96">
         <f>D5+F5</f>
-        <v>1.3230621490115999</v>
+        <v>1.419686</v>
       </c>
       <c r="E7" s="94"/>
       <c r="G7" s="95"/>
       <c r="H7" s="96"/>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>90</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>88</v>
       </c>
-      <c r="K7" s="96">
-        <f>K5+M5</f>
-        <v>1.3230621490115999</v>
-      </c>
-      <c r="L7" s="94"/>
-      <c r="N7" s="95"/>
+      <c r="L7" s="96">
+        <f>(L5+N5)/2</f>
+        <v>2.0286109999999997</v>
+      </c>
+      <c r="M7" s="94"/>
+      <c r="O7" s="95"/>
       <c r="P7" t="s">
         <v>90</v>
       </c>
       <c r="Q7" t="s">
         <v>88</v>
       </c>
-      <c r="R7" s="96">
-        <f>R5+T5</f>
-        <v>1.3230621490115999</v>
+      <c r="R7" s="93">
+        <f>(R5+T5)/2</f>
+        <v>0.66153107449999993</v>
       </c>
       <c r="S7" s="94"/>
       <c r="U7" s="95"/>
-      <c r="W7" t="s">
-        <v>90</v>
-      </c>
-      <c r="X7" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y7" s="96">
-        <f>Y5+AA5</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y7" s="96"/>
       <c r="Z7" s="94"/>
       <c r="AB7" s="95"/>
     </row>
@@ -3324,17 +3341,17 @@
       </c>
       <c r="D8" s="96">
         <f>E5</f>
-        <v>4.6255750000000004</v>
-      </c>
-      <c r="I8" t="s">
+        <v>7.2</v>
+      </c>
+      <c r="J8" t="s">
         <v>91</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>89</v>
       </c>
-      <c r="K8" s="96">
-        <f>L5</f>
-        <v>4.036975</v>
+      <c r="L8" s="96">
+        <f>M5</f>
+        <v>7.2</v>
       </c>
       <c r="P8" t="s">
         <v>91</v>
@@ -3344,18 +3361,9 @@
       </c>
       <c r="R8" s="96">
         <f>S5</f>
-        <v>3.4483749999999995</v>
-      </c>
-      <c r="W8" t="s">
-        <v>91</v>
-      </c>
-      <c r="X8" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y8" s="96">
-        <f>Z5</f>
-        <v>2.8597749999999991</v>
-      </c>
+        <v>4.6255750000000004</v>
+      </c>
+      <c r="Y8" s="96"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
@@ -3363,846 +3371,384 @@
       </c>
       <c r="D10" s="96">
         <f>D8/D7</f>
-        <v>3.4961131670613956</v>
+        <v>5.0715439893046774</v>
       </c>
       <c r="E10">
         <f>D10*180</f>
-        <v>629.30037007105125</v>
+        <v>912.87791807484189</v>
       </c>
       <c r="F10" s="95"/>
       <c r="G10" s="95">
         <f>E10*C3</f>
-        <v>12.586007401421025</v>
-      </c>
-      <c r="J10" t="s">
+        <v>18.257558361496837</v>
+      </c>
+      <c r="K10" t="s">
         <v>92</v>
       </c>
-      <c r="K10" s="96">
-        <f>K8/K7</f>
-        <v>3.0512361063430333</v>
-      </c>
-      <c r="L10">
-        <f>K10*180</f>
-        <v>549.22249914174597</v>
-      </c>
-      <c r="M10" s="95"/>
-      <c r="N10" s="95">
-        <f>L10*J3</f>
-        <v>10.984449982834919</v>
+      <c r="L10" s="96">
+        <f>L8*L7</f>
+        <v>14.605999199999998</v>
+      </c>
+      <c r="M10">
+        <f>L10*U2</f>
+        <v>1314.5399279999997</v>
+      </c>
+      <c r="N10" s="95"/>
+      <c r="O10" s="95">
+        <f>M10*K3</f>
+        <v>26.290798559999995</v>
       </c>
       <c r="Q10" t="s">
         <v>92</v>
       </c>
       <c r="R10" s="96">
-        <f>R8/R7</f>
-        <v>2.606359045624671</v>
+        <f>R8*R7</f>
+        <v>3.0599615999303373</v>
       </c>
       <c r="S10">
-        <f>R10*180</f>
-        <v>469.14462821244081</v>
+        <f>R10*U2</f>
+        <v>275.39654399373035</v>
       </c>
       <c r="T10" s="95"/>
       <c r="U10" s="95">
         <f>S10*Q3</f>
-        <v>9.3828925642488166</v>
-      </c>
-      <c r="X10" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y10" s="96">
-        <f>Y8/Y7</f>
-        <v>2.1614819849063083</v>
-      </c>
-      <c r="Z10">
-        <f>Y10*180</f>
-        <v>389.06675728313547</v>
-      </c>
+        <v>5.5079308798746069</v>
+      </c>
+      <c r="Y10" s="96"/>
       <c r="AA10" s="95"/>
-      <c r="AB10" s="95">
-        <f>Z10*X3</f>
-        <v>7.7813351456627098</v>
-      </c>
+      <c r="AB10" s="95"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="G11" s="95"/>
-      <c r="N11" s="95"/>
+      <c r="L11">
+        <f>L7/L8</f>
+        <v>0.28175152777777773</v>
+      </c>
+      <c r="O11" s="95"/>
+      <c r="R11" s="95">
+        <f>R7/R8</f>
+        <v>0.14301596547456261</v>
+      </c>
       <c r="U11" s="95"/>
       <c r="AB11" s="95"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D13" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="D13" s="97"/>
       <c r="E13" s="97"/>
       <c r="F13" s="97"/>
-      <c r="K13" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="J13" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="K13" s="97"/>
       <c r="L13" s="97"/>
-      <c r="M13" s="97"/>
-      <c r="R13" s="97" t="s">
-        <v>87</v>
-      </c>
-      <c r="S13" s="97"/>
-      <c r="T13" s="97"/>
-      <c r="Y13" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="P13" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q13" s="97"/>
+      <c r="R13" s="97"/>
+      <c r="T13" t="s">
+        <v>98</v>
+      </c>
+      <c r="U13">
+        <v>90</v>
+      </c>
+      <c r="Y13" s="97"/>
       <c r="Z13" s="97"/>
       <c r="AA13" s="97"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D14" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E14">
-        <f>E5-D3</f>
-        <v>4.4293750000000003</v>
-      </c>
-      <c r="F14">
+      <c r="D14" s="93"/>
+      <c r="J14">
+        <v>9.81</v>
+      </c>
+      <c r="K14">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="L14">
+        <f>J14*K14</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="P14">
+        <v>9.81</v>
+      </c>
+      <c r="Q14">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="R14">
+        <f>P14*Q14</f>
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="Y14" s="93"/>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="L15" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="M15" s="97"/>
+      <c r="N15" s="97"/>
+      <c r="R15" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="S15" s="97"/>
+      <c r="T15" s="97"/>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="D16" s="96"/>
+      <c r="E16" s="94"/>
+      <c r="L16" s="93">
+        <v>1.3187679999999999</v>
+      </c>
+      <c r="M16">
+        <v>7.2</v>
+      </c>
+      <c r="N16">
+        <v>2.7384539999999999</v>
+      </c>
+      <c r="R16" s="99">
+        <v>1.49E-7</v>
+      </c>
+      <c r="S16">
+        <v>4.6255750000000004</v>
+      </c>
+      <c r="T16">
         <v>1.323062</v>
       </c>
-      <c r="K14" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L14">
-        <f>L5-K3</f>
-        <v>3.8407749999999998</v>
-      </c>
-      <c r="M14">
-        <v>1.323062</v>
-      </c>
-      <c r="R14" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S14">
-        <f>S5-R3</f>
-        <v>3.2521749999999994</v>
-      </c>
-      <c r="T14">
-        <v>1.323062</v>
-      </c>
-      <c r="Y14" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z14">
-        <f>Z5-Y3</f>
-        <v>2.6635749999999989</v>
-      </c>
-      <c r="AA14">
-        <v>1.323062</v>
-      </c>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="96">
-        <f>D14+F14</f>
-        <v>1.3230621490115999</v>
-      </c>
-      <c r="E16" s="94"/>
-      <c r="I16" t="s">
-        <v>90</v>
-      </c>
-      <c r="J16" t="s">
-        <v>88</v>
-      </c>
-      <c r="K16" s="96">
-        <f>K14+M14</f>
-        <v>1.3230621490115999</v>
-      </c>
-      <c r="L16" s="94"/>
-      <c r="P16" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>88</v>
-      </c>
-      <c r="R16" s="96">
-        <f>R14+T14</f>
-        <v>1.3230621490115999</v>
-      </c>
-      <c r="S16" s="94"/>
-      <c r="W16" t="s">
-        <v>90</v>
-      </c>
-      <c r="X16" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y16" s="96">
-        <f>Y14+AA14</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y16" s="96"/>
       <c r="Z16" s="94"/>
     </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="96">
-        <f>E14</f>
-        <v>4.4293750000000003</v>
-      </c>
+    <row r="17" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D17" s="96"/>
       <c r="G17" s="95"/>
       <c r="H17" s="96"/>
-      <c r="I17" t="s">
+      <c r="Y17" s="96"/>
+      <c r="AB17" s="95"/>
+    </row>
+    <row r="18" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" t="s">
+        <v>99</v>
+      </c>
+      <c r="L18" s="96">
+        <f>L16*N16</f>
+        <v>3.6113855046719996</v>
+      </c>
+      <c r="M18" s="94"/>
+      <c r="O18" s="95"/>
+      <c r="P18" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>99</v>
+      </c>
+      <c r="R18" s="96">
+        <f>R16*T16</f>
+        <v>1.9713623799999999E-7</v>
+      </c>
+      <c r="S18" s="94"/>
+      <c r="U18" s="95"/>
+    </row>
+    <row r="19" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D19" s="96"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="95"/>
+      <c r="J19" t="s">
         <v>91</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K19" t="s">
         <v>89</v>
       </c>
-      <c r="K17" s="96">
-        <f>L14</f>
-        <v>3.8407749999999998</v>
-      </c>
-      <c r="N17" s="95"/>
-      <c r="P17" t="s">
+      <c r="L19" s="96">
+        <f>M16</f>
+        <v>7.2</v>
+      </c>
+      <c r="P19" t="s">
         <v>91</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q19" t="s">
         <v>89</v>
       </c>
-      <c r="R17" s="96">
-        <f>S14</f>
-        <v>3.2521749999999994</v>
-      </c>
-      <c r="U17" s="95"/>
-      <c r="W17" t="s">
-        <v>91</v>
-      </c>
-      <c r="X17" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y17" s="96">
-        <f>Z14</f>
-        <v>2.6635749999999989</v>
-      </c>
-      <c r="AB17" s="95"/>
-    </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="96">
-        <f>D17/D16</f>
-        <v>3.347820813488608</v>
-      </c>
-      <c r="E19">
-        <f>D19*180</f>
-        <v>602.60774642794945</v>
-      </c>
-      <c r="F19" s="95"/>
-      <c r="G19" s="95">
-        <f>E19*C3</f>
-        <v>12.05215492855899</v>
-      </c>
-      <c r="J19" t="s">
-        <v>92</v>
-      </c>
-      <c r="K19" s="96">
-        <f>K17/K16</f>
-        <v>2.9029437527702457</v>
-      </c>
-      <c r="L19">
-        <f>K19*180</f>
-        <v>522.52987549864429</v>
-      </c>
-      <c r="M19" s="95"/>
-      <c r="N19" s="95">
-        <f>L19*J3</f>
-        <v>10.450597509972885</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>92</v>
-      </c>
       <c r="R19" s="96">
-        <f>R17/R16</f>
-        <v>2.4580666920518834</v>
-      </c>
-      <c r="S19">
-        <f>R19*180</f>
-        <v>442.45200456933901</v>
-      </c>
-      <c r="T19" s="95"/>
-      <c r="U19" s="95">
-        <f>S19*Q3</f>
-        <v>8.8490400913867813</v>
-      </c>
-      <c r="X19" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y19" s="96">
-        <f>Y17/Y16</f>
-        <v>2.0131896313335211</v>
-      </c>
-      <c r="Z19">
-        <f>Y19*180</f>
-        <v>362.37413364003379</v>
-      </c>
+        <f>S16</f>
+        <v>4.6255750000000004</v>
+      </c>
+      <c r="Y19" s="96"/>
       <c r="AA19" s="95"/>
-      <c r="AB19" s="95">
-        <f>Z19*X3</f>
-        <v>7.2474826728006763</v>
-      </c>
-    </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="AB19" s="95"/>
+    </row>
+    <row r="20" spans="4:29" x14ac:dyDescent="0.25">
       <c r="D20" s="94"/>
       <c r="F20" s="95"/>
       <c r="G20" s="95"/>
-      <c r="K20" s="94"/>
-      <c r="M20" s="95"/>
-      <c r="N20" s="95"/>
-      <c r="R20" s="94"/>
-      <c r="T20" s="95"/>
-      <c r="U20" s="95"/>
       <c r="Y20" s="94"/>
       <c r="AA20" s="95"/>
       <c r="AB20" s="95"/>
     </row>
-    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:29" x14ac:dyDescent="0.25">
       <c r="G21" s="95"/>
+      <c r="K21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="96">
+        <f>L19*L18</f>
+        <v>26.001975633638398</v>
+      </c>
+      <c r="M21">
+        <f>L21*U13</f>
+        <v>2340.1778070274559</v>
+      </c>
       <c r="N21" s="95"/>
-      <c r="U21" s="95"/>
+      <c r="O21" s="95">
+        <f>M21*K14</f>
+        <v>46.803556140549119</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>92</v>
+      </c>
+      <c r="R21" s="96">
+        <f>R19/R18</f>
+        <v>23463849.401447952</v>
+      </c>
+      <c r="S21" s="95">
+        <f>R21*U13</f>
+        <v>2111746446.1303158</v>
+      </c>
+      <c r="T21" s="95"/>
+      <c r="U21" s="95">
+        <f>S21*Q14</f>
+        <v>42234928.922606319</v>
+      </c>
       <c r="AB21" s="95"/>
     </row>
-    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="D23" s="97" t="s">
-        <v>87</v>
-      </c>
+    <row r="23" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D23" s="97"/>
       <c r="E23" s="97"/>
       <c r="F23" s="97"/>
-      <c r="K23" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K23" s="97"/>
       <c r="L23" s="97"/>
       <c r="M23" s="97"/>
-      <c r="R23" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R23" s="97"/>
       <c r="S23" s="97"/>
       <c r="T23" s="97"/>
-      <c r="Y23" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y23" s="97"/>
       <c r="Z23" s="97"/>
       <c r="AA23" s="97"/>
     </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="D24" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E24">
-        <f>E14-D3</f>
-        <v>4.2331750000000001</v>
-      </c>
-      <c r="F24">
-        <v>1.323062</v>
-      </c>
-      <c r="K24" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L24">
-        <f>L14-K3</f>
-        <v>3.6445749999999997</v>
-      </c>
-      <c r="M24">
-        <v>1.323062</v>
-      </c>
-      <c r="R24" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S24">
-        <f>S14-R3</f>
-        <v>3.0559749999999992</v>
-      </c>
-      <c r="T24">
-        <v>1.323062</v>
-      </c>
-      <c r="Y24" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z24">
-        <f>Z14-Y3</f>
-        <v>2.4673749999999988</v>
-      </c>
-      <c r="AA24">
-        <v>1.323062</v>
-      </c>
-    </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="96">
-        <f>D24+F24</f>
-        <v>1.3230621490115999</v>
-      </c>
+    <row r="24" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D24" s="93"/>
+      <c r="K24" s="93"/>
+      <c r="R24" s="93"/>
+      <c r="Y24" s="93"/>
+    </row>
+    <row r="26" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D26" s="96"/>
       <c r="E26" s="94"/>
-      <c r="I26" t="s">
-        <v>90</v>
-      </c>
-      <c r="J26" t="s">
-        <v>88</v>
-      </c>
-      <c r="K26" s="96">
-        <f>K24+M24</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K26" s="96"/>
       <c r="L26" s="94"/>
-      <c r="P26" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>88</v>
-      </c>
-      <c r="R26" s="96">
-        <f>R24+T24</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R26" s="96"/>
       <c r="S26" s="94"/>
-      <c r="W26" t="s">
-        <v>90</v>
-      </c>
-      <c r="X26" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y26" s="96">
-        <f>Y24+AA24</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y26" s="96"/>
       <c r="Z26" s="94"/>
     </row>
-    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="96">
-        <f>E24</f>
-        <v>4.2331750000000001</v>
-      </c>
-      <c r="I27" t="s">
-        <v>91</v>
-      </c>
-      <c r="J27" t="s">
-        <v>89</v>
-      </c>
-      <c r="K27" s="96">
-        <f>L24</f>
-        <v>3.6445749999999997</v>
-      </c>
-      <c r="P27" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>89</v>
-      </c>
-      <c r="R27" s="96">
-        <f>S24</f>
-        <v>3.0559749999999992</v>
-      </c>
-      <c r="W27" t="s">
-        <v>91</v>
-      </c>
-      <c r="X27" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y27" s="96">
-        <f>Z24</f>
-        <v>2.4673749999999988</v>
-      </c>
-    </row>
-    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="96">
-        <f>D27/D26</f>
-        <v>3.1995284599158205</v>
-      </c>
-      <c r="E29">
-        <f>D29*180</f>
-        <v>575.91512278484765</v>
-      </c>
+    <row r="27" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D27" s="96"/>
+      <c r="K27" s="96"/>
+      <c r="R27" s="96"/>
+      <c r="Y27" s="96"/>
+    </row>
+    <row r="29" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D29" s="96"/>
       <c r="F29" s="95"/>
-      <c r="G29" s="95">
-        <f>E29*C3</f>
-        <v>11.518302455696952</v>
-      </c>
-      <c r="J29" t="s">
-        <v>92</v>
-      </c>
-      <c r="K29" s="96">
-        <f>K27/K26</f>
-        <v>2.7546513991974582</v>
-      </c>
-      <c r="L29">
-        <f>K29*180</f>
-        <v>495.83725185554249</v>
-      </c>
+      <c r="G29" s="95"/>
+      <c r="K29" s="96"/>
       <c r="M29" s="95"/>
-      <c r="N29" s="95">
-        <f>L29*J3</f>
-        <v>9.9167450371108501</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>92</v>
-      </c>
-      <c r="R29" s="96">
-        <f>R27/R26</f>
-        <v>2.3097743384790959</v>
-      </c>
-      <c r="S29">
-        <f>R29*180</f>
-        <v>415.75938092623727</v>
-      </c>
+      <c r="N29" s="95"/>
+      <c r="R29" s="96"/>
       <c r="T29" s="95"/>
-      <c r="U29" s="95">
-        <f>S29*Q3</f>
-        <v>8.315187618524746</v>
-      </c>
-      <c r="X29" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y29" s="96">
-        <f>Y27/Y26</f>
-        <v>1.8648972777607336</v>
-      </c>
-      <c r="Z29">
-        <f>Y29*180</f>
-        <v>335.68150999693205</v>
-      </c>
+      <c r="U29" s="95"/>
+      <c r="Y29" s="96"/>
       <c r="AA29" s="95"/>
-      <c r="AB29" s="95">
-        <f>Z29*X3</f>
-        <v>6.713630199938641</v>
-      </c>
-    </row>
-    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G31" s="95">
-        <f>G29+G19+G10</f>
-        <v>36.156464785676967</v>
-      </c>
-      <c r="N31" s="95">
-        <f>N29+N19+N10</f>
-        <v>31.351792529918654</v>
-      </c>
-      <c r="U31" s="95">
-        <f>U29+U19+U10</f>
-        <v>26.547120274160346</v>
-      </c>
-      <c r="AB31" s="95">
-        <f>AB29+AB19+AB10</f>
-        <v>21.742448018402026</v>
-      </c>
-      <c r="AC31" s="95">
-        <f>SUM(G31:AB31)</f>
-        <v>115.79782560815799</v>
-      </c>
-    </row>
-    <row r="32" spans="2:29" s="98" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="AB29" s="95"/>
+    </row>
+    <row r="31" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="G31" s="95"/>
+      <c r="N31" s="95"/>
+      <c r="U31" s="95"/>
+      <c r="AB31" s="95"/>
+      <c r="AC31" s="95"/>
+    </row>
+    <row r="32" spans="4:29" s="98" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B33" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="B33" s="97"/>
       <c r="C33" s="97"/>
       <c r="D33" s="97"/>
-      <c r="I33" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="I33" s="97"/>
       <c r="J33" s="97"/>
       <c r="K33" s="97"/>
-      <c r="P33" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="P33" s="97"/>
       <c r="Q33" s="97"/>
       <c r="R33" s="97"/>
-      <c r="W33" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="W33" s="97"/>
       <c r="X33" s="97"/>
       <c r="Y33" s="97"/>
     </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>9.81</v>
-      </c>
-      <c r="C34">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="D34">
-        <f>B34*C34</f>
-        <v>0.19620000000000001</v>
-      </c>
-      <c r="I34">
-        <v>9.81</v>
-      </c>
-      <c r="J34">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="K34">
-        <f>I34*J34</f>
-        <v>0.19620000000000001</v>
-      </c>
-      <c r="P34">
-        <v>9.81</v>
-      </c>
-      <c r="Q34">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="R34">
-        <f>P34*Q34</f>
-        <v>0.19620000000000001</v>
-      </c>
-      <c r="W34">
-        <v>9.81</v>
-      </c>
-      <c r="X34">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="Y34">
-        <f>W34*X34</f>
-        <v>0.19620000000000001</v>
-      </c>
-    </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D35" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="D35" s="97"/>
       <c r="E35" s="97"/>
       <c r="F35" s="97"/>
-      <c r="K35" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K35" s="97"/>
       <c r="L35" s="97"/>
       <c r="M35" s="97"/>
-      <c r="R35" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R35" s="97"/>
       <c r="S35" s="97"/>
       <c r="T35" s="97"/>
-      <c r="Y35" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y35" s="97"/>
       <c r="Z35" s="97"/>
       <c r="AA35" s="97"/>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D36" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E36">
-        <f>Z24-D34</f>
-        <v>2.2711749999999986</v>
-      </c>
-      <c r="F36">
-        <v>1.323062</v>
-      </c>
-      <c r="K36" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L36">
-        <f>E55-K34</f>
-        <v>1.6825749999999986</v>
-      </c>
-      <c r="M36">
-        <v>1.323062</v>
-      </c>
-      <c r="R36" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S36">
-        <f>L55-R34</f>
-        <v>1.0939749999999988</v>
-      </c>
-      <c r="T36">
-        <v>1.323062</v>
-      </c>
-      <c r="Y36" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z36">
-        <f>S55-Y34</f>
-        <v>0.50537499999999869</v>
-      </c>
-      <c r="AA36">
-        <v>1.323062</v>
-      </c>
+      <c r="D36" s="93"/>
+      <c r="K36" s="93"/>
+      <c r="R36" s="93"/>
+      <c r="Y36" s="93"/>
     </row>
     <row r="38" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="96">
-        <f>D36+F36</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="D38" s="96"/>
       <c r="E38" s="94"/>
       <c r="G38" s="95"/>
       <c r="H38" s="96"/>
-      <c r="I38" t="s">
-        <v>90</v>
-      </c>
-      <c r="J38" t="s">
-        <v>88</v>
-      </c>
-      <c r="K38" s="96">
-        <f>K36+M36</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K38" s="96"/>
       <c r="L38" s="94"/>
       <c r="N38" s="95"/>
-      <c r="P38" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>88</v>
-      </c>
-      <c r="R38" s="96">
-        <f>R36+T36</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R38" s="96"/>
       <c r="S38" s="94"/>
       <c r="U38" s="95"/>
-      <c r="W38" t="s">
-        <v>90</v>
-      </c>
-      <c r="X38" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y38" s="96">
-        <f>Y36+AA36</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y38" s="96"/>
       <c r="Z38" s="94"/>
       <c r="AB38" s="95"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="96">
-        <f>E36</f>
-        <v>2.2711749999999986</v>
-      </c>
-      <c r="I39" t="s">
-        <v>91</v>
-      </c>
-      <c r="J39" t="s">
-        <v>89</v>
-      </c>
-      <c r="K39" s="96">
-        <f>L36</f>
-        <v>1.6825749999999986</v>
-      </c>
-      <c r="P39" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>89</v>
-      </c>
-      <c r="R39" s="96">
-        <f>S36</f>
-        <v>1.0939749999999988</v>
-      </c>
-      <c r="W39" t="s">
-        <v>91</v>
-      </c>
-      <c r="X39" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y39" s="96">
-        <f>Z36</f>
-        <v>0.50537499999999869</v>
-      </c>
+      <c r="D39" s="96"/>
+      <c r="K39" s="96"/>
+      <c r="R39" s="96"/>
+      <c r="Y39" s="96"/>
     </row>
     <row r="41" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="96">
-        <f>D39/D38</f>
-        <v>1.7166049241879462</v>
-      </c>
-      <c r="E41">
-        <f>D41*180</f>
-        <v>308.98888635383031</v>
-      </c>
+      <c r="D41" s="96"/>
       <c r="F41" s="95"/>
-      <c r="G41" s="95">
-        <f>E41*C34</f>
-        <v>6.1797777270766066</v>
-      </c>
-      <c r="J41" t="s">
-        <v>92</v>
-      </c>
-      <c r="K41" s="96">
-        <f>K39/K38</f>
-        <v>1.2717278634695841</v>
-      </c>
-      <c r="L41">
-        <f>K41*180</f>
-        <v>228.91101542452515</v>
-      </c>
+      <c r="G41" s="95"/>
+      <c r="K41" s="96"/>
       <c r="M41" s="95"/>
-      <c r="N41" s="95">
-        <f>L41*J34</f>
-        <v>4.5782203084905033</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>92</v>
-      </c>
-      <c r="R41" s="96">
-        <f>R39/R38</f>
-        <v>0.82685080275122236</v>
-      </c>
-      <c r="S41">
-        <f>R41*180</f>
-        <v>148.83314449522001</v>
-      </c>
+      <c r="N41" s="95"/>
+      <c r="R41" s="96"/>
       <c r="T41" s="95"/>
-      <c r="U41" s="95">
-        <f>S41*Q34</f>
-        <v>2.9766628899044001</v>
-      </c>
-      <c r="X41" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y41" s="96">
-        <f>Y39/Y38</f>
-        <v>0.38197374203286033</v>
-      </c>
-      <c r="Z41">
-        <f>Y41*180</f>
-        <v>68.755273565914862</v>
-      </c>
+      <c r="U41" s="95"/>
+      <c r="Y41" s="96"/>
       <c r="AA41" s="95"/>
-      <c r="AB41" s="95">
-        <f>Z41*X34</f>
-        <v>1.3751054713182973</v>
-      </c>
+      <c r="AB41" s="95"/>
     </row>
     <row r="42" spans="2:28" x14ac:dyDescent="0.25">
       <c r="G42" s="95"/>
@@ -4211,227 +3757,59 @@
       <c r="AB42" s="95"/>
     </row>
     <row r="44" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D44" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="D44" s="97"/>
       <c r="E44" s="97"/>
       <c r="F44" s="97"/>
-      <c r="K44" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K44" s="97"/>
       <c r="L44" s="97"/>
       <c r="M44" s="97"/>
-      <c r="R44" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R44" s="97"/>
       <c r="S44" s="97"/>
       <c r="T44" s="97"/>
-      <c r="Y44" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y44" s="97"/>
       <c r="Z44" s="97"/>
       <c r="AA44" s="97"/>
     </row>
     <row r="45" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D45" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E45">
-        <f>E36-D34</f>
-        <v>2.0749749999999985</v>
-      </c>
-      <c r="F45">
-        <v>1.323062</v>
-      </c>
-      <c r="K45" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L45">
-        <f>L36-K34</f>
-        <v>1.4863749999999987</v>
-      </c>
-      <c r="M45">
-        <v>1.323062</v>
-      </c>
-      <c r="R45" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S45">
-        <f>S36-R34</f>
-        <v>0.89777499999999877</v>
-      </c>
-      <c r="T45">
-        <v>1.323062</v>
-      </c>
-      <c r="Y45" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z45">
-        <f>Z36-Y34</f>
-        <v>0.30917499999999865</v>
-      </c>
-      <c r="AA45">
-        <v>1.323062</v>
-      </c>
+      <c r="D45" s="93"/>
+      <c r="K45" s="93"/>
+      <c r="R45" s="93"/>
+      <c r="Y45" s="93"/>
     </row>
     <row r="47" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C47" t="s">
-        <v>88</v>
-      </c>
-      <c r="D47" s="96">
-        <f>D45+F45</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="D47" s="96"/>
       <c r="E47" s="94"/>
-      <c r="I47" t="s">
-        <v>90</v>
-      </c>
-      <c r="J47" t="s">
-        <v>88</v>
-      </c>
-      <c r="K47" s="96">
-        <f>K45+M45</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K47" s="96"/>
       <c r="L47" s="94"/>
-      <c r="P47" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>88</v>
-      </c>
-      <c r="R47" s="96">
-        <f>R45+T45</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R47" s="96"/>
       <c r="S47" s="94"/>
-      <c r="W47" t="s">
-        <v>90</v>
-      </c>
-      <c r="X47" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y47" s="96">
-        <f>Y45+AA45</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y47" s="96"/>
       <c r="Z47" s="94"/>
     </row>
     <row r="48" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48" s="96">
-        <f>E45</f>
-        <v>2.0749749999999985</v>
-      </c>
+      <c r="D48" s="96"/>
       <c r="G48" s="95"/>
       <c r="H48" s="96"/>
-      <c r="I48" t="s">
-        <v>91</v>
-      </c>
-      <c r="J48" t="s">
-        <v>89</v>
-      </c>
-      <c r="K48" s="96">
-        <f>L45</f>
-        <v>1.4863749999999987</v>
-      </c>
+      <c r="K48" s="96"/>
       <c r="N48" s="95"/>
-      <c r="P48" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>89</v>
-      </c>
-      <c r="R48" s="96">
-        <f>S45</f>
-        <v>0.89777499999999877</v>
-      </c>
+      <c r="R48" s="96"/>
       <c r="U48" s="95"/>
-      <c r="W48" t="s">
-        <v>91</v>
-      </c>
-      <c r="X48" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y48" s="96">
-        <f>Z45</f>
-        <v>0.30917499999999865</v>
-      </c>
+      <c r="Y48" s="96"/>
       <c r="AB48" s="95"/>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>92</v>
-      </c>
-      <c r="D50" s="96">
-        <f>D48/D47</f>
-        <v>1.5683125706151588</v>
-      </c>
-      <c r="E50">
-        <f>D50*180</f>
-        <v>282.29626271072857</v>
-      </c>
+      <c r="D50" s="96"/>
       <c r="F50" s="95"/>
-      <c r="G50" s="95">
-        <f>E50*C34</f>
-        <v>5.6459252542145713</v>
-      </c>
-      <c r="J50" t="s">
-        <v>92</v>
-      </c>
-      <c r="K50" s="96">
-        <f>K48/K47</f>
-        <v>1.123435509896797</v>
-      </c>
-      <c r="L50">
-        <f>K50*180</f>
-        <v>202.21839178142346</v>
-      </c>
+      <c r="G50" s="95"/>
+      <c r="K50" s="96"/>
       <c r="M50" s="95"/>
-      <c r="N50" s="95">
-        <f>L50*J34</f>
-        <v>4.0443678356284689</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>92</v>
-      </c>
-      <c r="R50" s="96">
-        <f>R48/R47</f>
-        <v>0.678558449178435</v>
-      </c>
-      <c r="S50">
-        <f>R50*180</f>
-        <v>122.1405208521183</v>
-      </c>
+      <c r="N50" s="95"/>
+      <c r="R50" s="96"/>
       <c r="T50" s="95"/>
-      <c r="U50" s="95">
-        <f>S50*Q34</f>
-        <v>2.4428104170423661</v>
-      </c>
-      <c r="X50" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y50" s="96">
-        <f>Y48/Y47</f>
-        <v>0.233681388460073</v>
-      </c>
-      <c r="Z50">
-        <f>Y50*180</f>
-        <v>42.062649922813137</v>
-      </c>
+      <c r="U50" s="95"/>
+      <c r="Y50" s="96"/>
       <c r="AA50" s="95"/>
-      <c r="AB50" s="95">
-        <f>Z50*X34</f>
-        <v>0.84125299845626278</v>
-      </c>
+      <c r="AB50" s="95"/>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D51" s="94"/>
@@ -4454,244 +3832,61 @@
       <c r="AB52" s="95"/>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D54" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="D54" s="97"/>
       <c r="E54" s="97"/>
       <c r="F54" s="97"/>
-      <c r="K54" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K54" s="97"/>
       <c r="L54" s="97"/>
       <c r="M54" s="97"/>
-      <c r="R54" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R54" s="97"/>
       <c r="S54" s="97"/>
       <c r="T54" s="97"/>
-      <c r="Y54" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y54" s="97"/>
       <c r="Z54" s="97"/>
       <c r="AA54" s="97"/>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D55" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E55">
-        <f>E45-D34</f>
-        <v>1.8787749999999985</v>
-      </c>
-      <c r="F55">
-        <v>1.323062</v>
-      </c>
-      <c r="K55" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L55">
-        <f>L45-K34</f>
-        <v>1.2901749999999987</v>
-      </c>
-      <c r="M55">
-        <v>1.323062</v>
-      </c>
-      <c r="R55" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S55">
-        <f>S45-R34</f>
-        <v>0.70157499999999873</v>
-      </c>
-      <c r="T55">
-        <v>1.323062</v>
-      </c>
-      <c r="Y55" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z55">
-        <f>Z45-Y34</f>
-        <v>0.11297499999999863</v>
-      </c>
-      <c r="AA55">
-        <v>1.323062</v>
-      </c>
+      <c r="D55" s="93"/>
+      <c r="K55" s="93"/>
+      <c r="R55" s="93"/>
+      <c r="Y55" s="93"/>
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" t="s">
-        <v>88</v>
-      </c>
-      <c r="D57" s="96">
-        <f>D55+F55</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="D57" s="96"/>
       <c r="E57" s="94"/>
-      <c r="I57" t="s">
-        <v>90</v>
-      </c>
-      <c r="J57" t="s">
-        <v>88</v>
-      </c>
-      <c r="K57" s="96">
-        <f>K55+M55</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K57" s="96"/>
       <c r="L57" s="94"/>
-      <c r="P57" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>88</v>
-      </c>
-      <c r="R57" s="96">
-        <f>R55+T55</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R57" s="96"/>
       <c r="S57" s="94"/>
-      <c r="W57" t="s">
-        <v>90</v>
-      </c>
-      <c r="X57" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y57" s="96">
-        <f>Y55+AA55</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y57" s="96"/>
       <c r="Z57" s="94"/>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>91</v>
-      </c>
-      <c r="C58" t="s">
-        <v>89</v>
-      </c>
-      <c r="D58" s="96">
-        <f>E55</f>
-        <v>1.8787749999999985</v>
-      </c>
-      <c r="I58" t="s">
-        <v>91</v>
-      </c>
-      <c r="J58" t="s">
-        <v>89</v>
-      </c>
-      <c r="K58" s="96">
-        <f>L55</f>
-        <v>1.2901749999999987</v>
-      </c>
-      <c r="P58" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>89</v>
-      </c>
-      <c r="R58" s="96">
-        <f>S55</f>
-        <v>0.70157499999999873</v>
-      </c>
-      <c r="W58" t="s">
-        <v>91</v>
-      </c>
-      <c r="X58" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y58" s="96">
-        <f>Z55</f>
-        <v>0.11297499999999863</v>
-      </c>
+      <c r="D58" s="96"/>
+      <c r="K58" s="96"/>
+      <c r="R58" s="96"/>
+      <c r="Y58" s="96"/>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>92</v>
-      </c>
-      <c r="D60" s="96">
-        <f>D58/D57</f>
-        <v>1.4200202170423715</v>
-      </c>
-      <c r="E60">
-        <f>D60*180</f>
-        <v>255.60363906762686</v>
-      </c>
+      <c r="D60" s="96"/>
       <c r="F60" s="95"/>
-      <c r="G60" s="95">
-        <f>E60*C34</f>
-        <v>5.1120727813525368</v>
-      </c>
-      <c r="J60" t="s">
-        <v>92</v>
-      </c>
-      <c r="K60" s="96">
-        <f>K58/K57</f>
-        <v>0.97514315632400972</v>
-      </c>
-      <c r="L60">
-        <f>K60*180</f>
-        <v>175.52576813832175</v>
-      </c>
+      <c r="G60" s="95"/>
+      <c r="K60" s="96"/>
       <c r="M60" s="95"/>
-      <c r="N60" s="95">
-        <f>L60*J34</f>
-        <v>3.5105153627664349</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>92</v>
-      </c>
-      <c r="R60" s="96">
-        <f>R58/R57</f>
-        <v>0.53026609560564764</v>
-      </c>
-      <c r="S60">
-        <f>R60*180</f>
-        <v>95.447897209016574</v>
-      </c>
+      <c r="N60" s="95"/>
+      <c r="R60" s="96"/>
       <c r="T60" s="95"/>
-      <c r="U60" s="95">
-        <f>S60*Q34</f>
-        <v>1.9089579441803315</v>
-      </c>
-      <c r="X60" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y60" s="96">
-        <f>Y58/Y57</f>
-        <v>8.538903488728565E-2</v>
-      </c>
-      <c r="Z60">
-        <f>Y60*180</f>
-        <v>15.370026279711418</v>
-      </c>
+      <c r="U60" s="95"/>
+      <c r="Y60" s="96"/>
       <c r="AA60" s="95"/>
-      <c r="AB60" s="95">
-        <f>Z60*X34</f>
-        <v>0.30740052559422837</v>
-      </c>
+      <c r="AB60" s="95"/>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G62" s="95">
-        <f>G60+G50+G41</f>
-        <v>16.937775762643717</v>
-      </c>
-      <c r="N62" s="95">
-        <f>N60+N50+N41</f>
-        <v>12.133103506885409</v>
-      </c>
-      <c r="U62" s="95">
-        <f>U60+U50+U41</f>
-        <v>7.3284312511270979</v>
-      </c>
-      <c r="AB62" s="95">
-        <f>AB60+AB50+AB41</f>
-        <v>2.5237589953687882</v>
-      </c>
-      <c r="AC62" s="95">
-        <f>SUM(G62:AB62)</f>
-        <v>38.923069516025009</v>
-      </c>
+      <c r="G62" s="95"/>
+      <c r="N62" s="95"/>
+      <c r="U62" s="95"/>
+      <c r="AB62" s="95"/>
+      <c r="AC62" s="95"/>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" s="98"/>
@@ -4725,523 +3920,134 @@
       <c r="AC63" s="98"/>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B64" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="B64" s="97"/>
       <c r="C64" s="97"/>
       <c r="D64" s="97"/>
-      <c r="I64" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="I64" s="97"/>
       <c r="J64" s="97"/>
       <c r="K64" s="97"/>
-      <c r="P64" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="P64" s="97"/>
       <c r="Q64" s="97"/>
       <c r="R64" s="97"/>
-      <c r="W64" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="W64" s="97"/>
       <c r="X64" s="97"/>
       <c r="Y64" s="97"/>
     </row>
-    <row r="65" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B65">
-        <v>9.81</v>
-      </c>
-      <c r="C65">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="D65">
-        <f>B65*C65</f>
-        <v>0.19620000000000001</v>
-      </c>
-      <c r="I65">
-        <v>9.81</v>
-      </c>
-      <c r="J65">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="K65">
-        <f>I65*J65</f>
-        <v>0.19620000000000001</v>
-      </c>
-      <c r="P65">
-        <v>9.81</v>
-      </c>
-      <c r="Q65">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="R65">
-        <f>P65*Q65</f>
-        <v>0.19620000000000001</v>
-      </c>
-      <c r="W65">
-        <v>9.81</v>
-      </c>
-      <c r="X65">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="Y65">
-        <f>W65*X65</f>
-        <v>0.19620000000000001</v>
-      </c>
-    </row>
-    <row r="66" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D66" s="97" t="s">
-        <v>87</v>
-      </c>
+    <row r="66" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D66" s="97"/>
       <c r="E66" s="97"/>
       <c r="F66" s="97"/>
-      <c r="K66" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K66" s="97"/>
       <c r="L66" s="97"/>
       <c r="M66" s="97"/>
-      <c r="R66" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R66" s="97"/>
       <c r="S66" s="97"/>
       <c r="T66" s="97"/>
-      <c r="Y66" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y66" s="97"/>
       <c r="Z66" s="97"/>
       <c r="AA66" s="97"/>
     </row>
-    <row r="67" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D67" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E67">
-        <v>4.6255750000000004</v>
-      </c>
-      <c r="F67">
-        <v>1.323062</v>
-      </c>
-      <c r="K67" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L67">
-        <f>E86-K65</f>
-        <v>4.036975</v>
-      </c>
-      <c r="M67">
-        <v>1.323062</v>
-      </c>
-      <c r="R67" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S67">
-        <f>L86-R65</f>
-        <v>3.4483749999999995</v>
-      </c>
-      <c r="T67">
-        <v>1.323062</v>
-      </c>
-      <c r="Y67" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z67">
-        <f>S86-Y65</f>
-        <v>2.8597749999999991</v>
-      </c>
-      <c r="AA67">
-        <v>1.323062</v>
-      </c>
-    </row>
-    <row r="69" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>90</v>
-      </c>
-      <c r="C69" t="s">
-        <v>88</v>
-      </c>
-      <c r="D69" s="96">
-        <f>D67+F67</f>
-        <v>1.3230621490115999</v>
-      </c>
+    <row r="67" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D67" s="93"/>
+      <c r="K67" s="93"/>
+      <c r="R67" s="93"/>
+      <c r="Y67" s="93"/>
+    </row>
+    <row r="69" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D69" s="96"/>
       <c r="E69" s="94"/>
       <c r="G69" s="95"/>
       <c r="H69" s="96"/>
-      <c r="I69" t="s">
-        <v>90</v>
-      </c>
-      <c r="J69" t="s">
-        <v>88</v>
-      </c>
-      <c r="K69" s="96">
-        <f>K67+M67</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K69" s="96"/>
       <c r="L69" s="94"/>
       <c r="N69" s="95"/>
-      <c r="P69" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>88</v>
-      </c>
-      <c r="R69" s="96">
-        <f>R67+T67</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R69" s="96"/>
       <c r="S69" s="94"/>
       <c r="U69" s="95"/>
-      <c r="W69" t="s">
-        <v>90</v>
-      </c>
-      <c r="X69" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y69" s="96">
-        <f>Y67+AA67</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y69" s="96"/>
       <c r="Z69" s="94"/>
       <c r="AB69" s="95"/>
     </row>
-    <row r="70" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C70" t="s">
-        <v>89</v>
-      </c>
-      <c r="D70" s="96">
-        <f>E67</f>
-        <v>4.6255750000000004</v>
-      </c>
-      <c r="I70" t="s">
-        <v>91</v>
-      </c>
-      <c r="J70" t="s">
-        <v>89</v>
-      </c>
-      <c r="K70" s="96">
-        <f>L67</f>
-        <v>4.036975</v>
-      </c>
-      <c r="P70" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>89</v>
-      </c>
-      <c r="R70" s="96">
-        <f>S67</f>
-        <v>3.4483749999999995</v>
-      </c>
-      <c r="W70" t="s">
-        <v>91</v>
-      </c>
-      <c r="X70" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y70" s="96">
-        <f>Z67</f>
-        <v>2.8597749999999991</v>
-      </c>
-    </row>
-    <row r="72" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="96">
-        <f>D70/D69</f>
-        <v>3.4961131670613956</v>
-      </c>
-      <c r="E72">
-        <f>D72*180</f>
-        <v>629.30037007105125</v>
-      </c>
+    <row r="70" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D70" s="96"/>
+      <c r="K70" s="96"/>
+      <c r="R70" s="96"/>
+      <c r="Y70" s="96"/>
+    </row>
+    <row r="72" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D72" s="96"/>
       <c r="F72" s="95"/>
-      <c r="G72" s="95">
-        <f>E72*C65</f>
-        <v>12.586007401421025</v>
-      </c>
-      <c r="J72" t="s">
-        <v>92</v>
-      </c>
-      <c r="K72" s="96">
-        <f>K70/K69</f>
-        <v>3.0512361063430333</v>
-      </c>
-      <c r="L72">
-        <f>K72*180</f>
-        <v>549.22249914174597</v>
-      </c>
+      <c r="G72" s="95"/>
+      <c r="K72" s="96"/>
       <c r="M72" s="95"/>
-      <c r="N72" s="95">
-        <f>L72*J65</f>
-        <v>10.984449982834919</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>92</v>
-      </c>
-      <c r="R72" s="96">
-        <f>R70/R69</f>
-        <v>2.606359045624671</v>
-      </c>
-      <c r="S72">
-        <f>R72*180</f>
-        <v>469.14462821244081</v>
-      </c>
+      <c r="N72" s="95"/>
+      <c r="R72" s="96"/>
       <c r="T72" s="95"/>
-      <c r="U72" s="95">
-        <f>S72*Q65</f>
-        <v>9.3828925642488166</v>
-      </c>
-      <c r="X72" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y72" s="96">
-        <f>Y70/Y69</f>
-        <v>2.1614819849063083</v>
-      </c>
-      <c r="Z72">
-        <f>Y72*180</f>
-        <v>389.06675728313547</v>
-      </c>
+      <c r="U72" s="95"/>
+      <c r="Y72" s="96"/>
       <c r="AA72" s="95"/>
-      <c r="AB72" s="95">
-        <f>Z72*X65</f>
-        <v>7.7813351456627098</v>
-      </c>
-    </row>
-    <row r="73" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AB72" s="95"/>
+    </row>
+    <row r="73" spans="4:28" x14ac:dyDescent="0.25">
       <c r="G73" s="95"/>
       <c r="N73" s="95"/>
       <c r="U73" s="95"/>
       <c r="AB73" s="95"/>
     </row>
-    <row r="75" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D75" s="97" t="s">
-        <v>87</v>
-      </c>
+    <row r="75" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D75" s="97"/>
       <c r="E75" s="97"/>
       <c r="F75" s="97"/>
-      <c r="K75" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K75" s="97"/>
       <c r="L75" s="97"/>
       <c r="M75" s="97"/>
-      <c r="R75" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R75" s="97"/>
       <c r="S75" s="97"/>
       <c r="T75" s="97"/>
-      <c r="Y75" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y75" s="97"/>
       <c r="Z75" s="97"/>
       <c r="AA75" s="97"/>
     </row>
-    <row r="76" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D76" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E76">
-        <f>E67-D65</f>
-        <v>4.4293750000000003</v>
-      </c>
-      <c r="F76">
-        <v>1.323062</v>
-      </c>
-      <c r="K76" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L76">
-        <f>L67-K65</f>
-        <v>3.8407749999999998</v>
-      </c>
-      <c r="M76">
-        <v>1.323062</v>
-      </c>
-      <c r="R76" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S76">
-        <f>S67-R65</f>
-        <v>3.2521749999999994</v>
-      </c>
-      <c r="T76">
-        <v>1.323062</v>
-      </c>
-      <c r="Y76" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z76">
-        <f>Z67-Y65</f>
-        <v>2.6635749999999989</v>
-      </c>
-      <c r="AA76">
-        <v>1.323062</v>
-      </c>
-    </row>
-    <row r="78" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>90</v>
-      </c>
-      <c r="C78" t="s">
-        <v>88</v>
-      </c>
-      <c r="D78" s="96">
-        <f>D76+F76</f>
-        <v>1.3230621490115999</v>
-      </c>
+    <row r="76" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D76" s="93"/>
+      <c r="K76" s="93"/>
+      <c r="R76" s="93"/>
+      <c r="Y76" s="93"/>
+    </row>
+    <row r="78" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D78" s="96"/>
       <c r="E78" s="94"/>
-      <c r="I78" t="s">
-        <v>90</v>
-      </c>
-      <c r="J78" t="s">
-        <v>88</v>
-      </c>
-      <c r="K78" s="96">
-        <f>K76+M76</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K78" s="96"/>
       <c r="L78" s="94"/>
-      <c r="P78" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>88</v>
-      </c>
-      <c r="R78" s="96">
-        <f>R76+T76</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R78" s="96"/>
       <c r="S78" s="94"/>
-      <c r="W78" t="s">
-        <v>90</v>
-      </c>
-      <c r="X78" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y78" s="96">
-        <f>Y76+AA76</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y78" s="96"/>
       <c r="Z78" s="94"/>
     </row>
-    <row r="79" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>91</v>
-      </c>
-      <c r="C79" t="s">
-        <v>89</v>
-      </c>
-      <c r="D79" s="96">
-        <f>E76</f>
-        <v>4.4293750000000003</v>
-      </c>
+    <row r="79" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D79" s="96"/>
       <c r="G79" s="95"/>
       <c r="H79" s="96"/>
-      <c r="I79" t="s">
-        <v>91</v>
-      </c>
-      <c r="J79" t="s">
-        <v>89</v>
-      </c>
-      <c r="K79" s="96">
-        <f>L76</f>
-        <v>3.8407749999999998</v>
-      </c>
+      <c r="K79" s="96"/>
       <c r="N79" s="95"/>
-      <c r="P79" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>89</v>
-      </c>
-      <c r="R79" s="96">
-        <f>S76</f>
-        <v>3.2521749999999994</v>
-      </c>
+      <c r="R79" s="96"/>
       <c r="U79" s="95"/>
-      <c r="W79" t="s">
-        <v>91</v>
-      </c>
-      <c r="X79" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y79" s="96">
-        <f>Z76</f>
-        <v>2.6635749999999989</v>
-      </c>
+      <c r="Y79" s="96"/>
       <c r="AB79" s="95"/>
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
-        <v>92</v>
-      </c>
-      <c r="D81" s="96">
-        <f>D79/D78</f>
-        <v>3.347820813488608</v>
-      </c>
-      <c r="E81">
-        <f>D81*180</f>
-        <v>602.60774642794945</v>
-      </c>
+      <c r="D81" s="96"/>
       <c r="F81" s="95"/>
-      <c r="G81" s="95">
-        <f>E81*C65</f>
-        <v>12.05215492855899</v>
-      </c>
-      <c r="J81" t="s">
-        <v>92</v>
-      </c>
-      <c r="K81" s="96">
-        <f>K79/K78</f>
-        <v>2.9029437527702457</v>
-      </c>
-      <c r="L81">
-        <f>K81*180</f>
-        <v>522.52987549864429</v>
-      </c>
+      <c r="G81" s="95"/>
+      <c r="K81" s="96"/>
       <c r="M81" s="95"/>
-      <c r="N81" s="95">
-        <f>L81*J65</f>
-        <v>10.450597509972885</v>
-      </c>
-      <c r="Q81" t="s">
-        <v>92</v>
-      </c>
-      <c r="R81" s="96">
-        <f>R79/R78</f>
-        <v>2.4580666920518834</v>
-      </c>
-      <c r="S81">
-        <f>R81*180</f>
-        <v>442.45200456933901</v>
-      </c>
+      <c r="N81" s="95"/>
+      <c r="R81" s="96"/>
       <c r="T81" s="95"/>
-      <c r="U81" s="95">
-        <f>S81*Q65</f>
-        <v>8.8490400913867813</v>
-      </c>
-      <c r="X81" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y81" s="96">
-        <f>Y79/Y78</f>
-        <v>2.0131896313335211</v>
-      </c>
-      <c r="Z81">
-        <f>Y81*180</f>
-        <v>362.37413364003379</v>
-      </c>
+      <c r="U81" s="95"/>
+      <c r="Y81" s="96"/>
       <c r="AA81" s="95"/>
-      <c r="AB81" s="95">
-        <f>Z81*X65</f>
-        <v>7.2474826728006763</v>
-      </c>
+      <c r="AB81" s="95"/>
     </row>
     <row r="82" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D82" s="94"/>
@@ -5264,244 +4070,61 @@
       <c r="AB83" s="95"/>
     </row>
     <row r="85" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D85" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="D85" s="97"/>
       <c r="E85" s="97"/>
       <c r="F85" s="97"/>
-      <c r="K85" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K85" s="97"/>
       <c r="L85" s="97"/>
       <c r="M85" s="97"/>
-      <c r="R85" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R85" s="97"/>
       <c r="S85" s="97"/>
       <c r="T85" s="97"/>
-      <c r="Y85" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y85" s="97"/>
       <c r="Z85" s="97"/>
       <c r="AA85" s="97"/>
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D86" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E86">
-        <f>E76-D65</f>
-        <v>4.2331750000000001</v>
-      </c>
-      <c r="F86">
-        <v>1.323062</v>
-      </c>
-      <c r="K86" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L86">
-        <f>L76-K65</f>
-        <v>3.6445749999999997</v>
-      </c>
-      <c r="M86">
-        <v>1.323062</v>
-      </c>
-      <c r="R86" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S86">
-        <f>S76-R65</f>
-        <v>3.0559749999999992</v>
-      </c>
-      <c r="T86">
-        <v>1.323062</v>
-      </c>
-      <c r="Y86" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z86">
-        <f>Z76-Y65</f>
-        <v>2.4673749999999988</v>
-      </c>
-      <c r="AA86">
-        <v>1.323062</v>
-      </c>
+      <c r="D86" s="93"/>
+      <c r="K86" s="93"/>
+      <c r="R86" s="93"/>
+      <c r="Y86" s="93"/>
     </row>
     <row r="88" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>90</v>
-      </c>
-      <c r="C88" t="s">
-        <v>88</v>
-      </c>
-      <c r="D88" s="96">
-        <f>D86+F86</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="D88" s="96"/>
       <c r="E88" s="94"/>
-      <c r="I88" t="s">
-        <v>90</v>
-      </c>
-      <c r="J88" t="s">
-        <v>88</v>
-      </c>
-      <c r="K88" s="96">
-        <f>K86+M86</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K88" s="96"/>
       <c r="L88" s="94"/>
-      <c r="P88" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q88" t="s">
-        <v>88</v>
-      </c>
-      <c r="R88" s="96">
-        <f>R86+T86</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R88" s="96"/>
       <c r="S88" s="94"/>
-      <c r="W88" t="s">
-        <v>90</v>
-      </c>
-      <c r="X88" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y88" s="96">
-        <f>Y86+AA86</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y88" s="96"/>
       <c r="Z88" s="94"/>
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>91</v>
-      </c>
-      <c r="C89" t="s">
-        <v>89</v>
-      </c>
-      <c r="D89" s="96">
-        <f>E86</f>
-        <v>4.2331750000000001</v>
-      </c>
-      <c r="I89" t="s">
-        <v>91</v>
-      </c>
-      <c r="J89" t="s">
-        <v>89</v>
-      </c>
-      <c r="K89" s="96">
-        <f>L86</f>
-        <v>3.6445749999999997</v>
-      </c>
-      <c r="P89" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q89" t="s">
-        <v>89</v>
-      </c>
-      <c r="R89" s="96">
-        <f>S86</f>
-        <v>3.0559749999999992</v>
-      </c>
-      <c r="W89" t="s">
-        <v>91</v>
-      </c>
-      <c r="X89" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y89" s="96">
-        <f>Z86</f>
-        <v>2.4673749999999988</v>
-      </c>
+      <c r="D89" s="96"/>
+      <c r="K89" s="96"/>
+      <c r="R89" s="96"/>
+      <c r="Y89" s="96"/>
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>92</v>
-      </c>
-      <c r="D91" s="96">
-        <f>D89/D88</f>
-        <v>3.1995284599158205</v>
-      </c>
-      <c r="E91">
-        <f>D91*180</f>
-        <v>575.91512278484765</v>
-      </c>
+      <c r="D91" s="96"/>
       <c r="F91" s="95"/>
-      <c r="G91" s="95">
-        <f>E91*C65</f>
-        <v>11.518302455696952</v>
-      </c>
-      <c r="J91" t="s">
-        <v>92</v>
-      </c>
-      <c r="K91" s="96">
-        <f>K89/K88</f>
-        <v>2.7546513991974582</v>
-      </c>
-      <c r="L91">
-        <f>K91*180</f>
-        <v>495.83725185554249</v>
-      </c>
+      <c r="G91" s="95"/>
+      <c r="K91" s="96"/>
       <c r="M91" s="95"/>
-      <c r="N91" s="95">
-        <f>L91*J65</f>
-        <v>9.9167450371108501</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>92</v>
-      </c>
-      <c r="R91" s="96">
-        <f>R89/R88</f>
-        <v>2.3097743384790959</v>
-      </c>
-      <c r="S91">
-        <f>R91*180</f>
-        <v>415.75938092623727</v>
-      </c>
+      <c r="N91" s="95"/>
+      <c r="R91" s="96"/>
       <c r="T91" s="95"/>
-      <c r="U91" s="95">
-        <f>S91*Q65</f>
-        <v>8.315187618524746</v>
-      </c>
-      <c r="X91" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y91" s="96">
-        <f>Y89/Y88</f>
-        <v>1.8648972777607336</v>
-      </c>
-      <c r="Z91">
-        <f>Y91*180</f>
-        <v>335.68150999693205</v>
-      </c>
+      <c r="U91" s="95"/>
+      <c r="Y91" s="96"/>
       <c r="AA91" s="95"/>
-      <c r="AB91" s="95">
-        <f>Z91*X65</f>
-        <v>6.713630199938641</v>
-      </c>
+      <c r="AB91" s="95"/>
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G93" s="95">
-        <f>G91+G81+G72</f>
-        <v>36.156464785676967</v>
-      </c>
-      <c r="N93" s="95">
-        <f>N91+N81+N72</f>
-        <v>31.351792529918654</v>
-      </c>
-      <c r="U93" s="95">
-        <f>U91+U81+U72</f>
-        <v>26.547120274160346</v>
-      </c>
-      <c r="AB93" s="95">
-        <f>AB91+AB81+AB72</f>
-        <v>21.742448018402026</v>
-      </c>
-      <c r="AC93" s="95">
-        <f>SUM(G93:AB93)</f>
-        <v>115.79782560815799</v>
-      </c>
+      <c r="G93" s="95"/>
+      <c r="N93" s="95"/>
+      <c r="U93" s="95"/>
+      <c r="AB93" s="95"/>
+      <c r="AC93" s="95"/>
     </row>
     <row r="94" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A94" s="98"/>
@@ -5535,524 +4158,134 @@
       <c r="AC94" s="98"/>
     </row>
     <row r="95" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B95" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="B95" s="97"/>
       <c r="C95" s="97"/>
       <c r="D95" s="97"/>
-      <c r="I95" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="I95" s="97"/>
       <c r="J95" s="97"/>
       <c r="K95" s="97"/>
-      <c r="P95" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="P95" s="97"/>
       <c r="Q95" s="97"/>
       <c r="R95" s="97"/>
-      <c r="W95" s="97" t="s">
-        <v>86</v>
-      </c>
+      <c r="W95" s="97"/>
       <c r="X95" s="97"/>
       <c r="Y95" s="97"/>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B96">
-        <v>9.81</v>
-      </c>
-      <c r="C96">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="D96">
-        <f>B96*C96</f>
-        <v>0.19620000000000001</v>
-      </c>
-      <c r="I96">
-        <v>9.81</v>
-      </c>
-      <c r="J96">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="K96">
-        <f>I96*J96</f>
-        <v>0.19620000000000001</v>
-      </c>
-      <c r="P96">
-        <v>9.81</v>
-      </c>
-      <c r="Q96">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="R96">
-        <f>P96*Q96</f>
-        <v>0.19620000000000001</v>
-      </c>
-      <c r="W96">
-        <v>9.81</v>
-      </c>
-      <c r="X96">
-        <f>1/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="Y96">
-        <f>W96*X96</f>
-        <v>0.19620000000000001</v>
-      </c>
-    </row>
-    <row r="97" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D97" s="97" t="s">
-        <v>87</v>
-      </c>
+    <row r="97" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D97" s="97"/>
       <c r="E97" s="97"/>
       <c r="F97" s="97"/>
-      <c r="K97" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K97" s="97"/>
       <c r="L97" s="97"/>
       <c r="M97" s="97"/>
-      <c r="R97" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R97" s="97"/>
       <c r="S97" s="97"/>
       <c r="T97" s="97"/>
-      <c r="Y97" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y97" s="97"/>
       <c r="Z97" s="97"/>
       <c r="AA97" s="97"/>
     </row>
-    <row r="98" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D98" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E98">
-        <f>Z86-D96</f>
-        <v>2.2711749999999986</v>
-      </c>
-      <c r="F98">
-        <v>1.323062</v>
-      </c>
-      <c r="K98" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L98">
-        <f>E117-K96</f>
-        <v>1.6825749999999986</v>
-      </c>
-      <c r="M98">
-        <v>1.323062</v>
-      </c>
-      <c r="R98" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S98">
-        <f>L117-R96</f>
-        <v>1.0939749999999988</v>
-      </c>
-      <c r="T98">
-        <v>1.323062</v>
-      </c>
-      <c r="Y98" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z98">
-        <f>S117-Y96</f>
-        <v>0.50537499999999869</v>
-      </c>
-      <c r="AA98">
-        <v>1.323062</v>
-      </c>
-    </row>
-    <row r="100" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>90</v>
-      </c>
-      <c r="C100" t="s">
-        <v>88</v>
-      </c>
-      <c r="D100" s="96">
-        <f>D98+F98</f>
-        <v>1.3230621490115999</v>
-      </c>
+    <row r="98" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D98" s="93"/>
+      <c r="K98" s="93"/>
+      <c r="R98" s="93"/>
+      <c r="Y98" s="93"/>
+    </row>
+    <row r="100" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D100" s="96"/>
       <c r="E100" s="94"/>
       <c r="G100" s="95"/>
       <c r="H100" s="96"/>
-      <c r="I100" t="s">
-        <v>90</v>
-      </c>
-      <c r="J100" t="s">
-        <v>88</v>
-      </c>
-      <c r="K100" s="96">
-        <f>K98+M98</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K100" s="96"/>
       <c r="L100" s="94"/>
       <c r="N100" s="95"/>
-      <c r="P100" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>88</v>
-      </c>
-      <c r="R100" s="96">
-        <f>R98+T98</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R100" s="96"/>
       <c r="S100" s="94"/>
       <c r="U100" s="95"/>
-      <c r="W100" t="s">
-        <v>90</v>
-      </c>
-      <c r="X100" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y100" s="96">
-        <f>Y98+AA98</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y100" s="96"/>
       <c r="Z100" s="94"/>
       <c r="AB100" s="95"/>
     </row>
-    <row r="101" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>91</v>
-      </c>
-      <c r="C101" t="s">
-        <v>89</v>
-      </c>
-      <c r="D101" s="96">
-        <f>E98</f>
-        <v>2.2711749999999986</v>
-      </c>
-      <c r="I101" t="s">
-        <v>91</v>
-      </c>
-      <c r="J101" t="s">
-        <v>89</v>
-      </c>
-      <c r="K101" s="96">
-        <f>L98</f>
-        <v>1.6825749999999986</v>
-      </c>
-      <c r="P101" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>89</v>
-      </c>
-      <c r="R101" s="96">
-        <f>S98</f>
-        <v>1.0939749999999988</v>
-      </c>
-      <c r="W101" t="s">
-        <v>91</v>
-      </c>
-      <c r="X101" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y101" s="96">
-        <f>Z98</f>
-        <v>0.50537499999999869</v>
-      </c>
-    </row>
-    <row r="103" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
-        <v>92</v>
-      </c>
-      <c r="D103" s="96">
-        <f>D101/D100</f>
-        <v>1.7166049241879462</v>
-      </c>
-      <c r="E103">
-        <f>D103*180</f>
-        <v>308.98888635383031</v>
-      </c>
+    <row r="101" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D101" s="96"/>
+      <c r="K101" s="96"/>
+      <c r="R101" s="96"/>
+      <c r="Y101" s="96"/>
+    </row>
+    <row r="103" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D103" s="96"/>
       <c r="F103" s="95"/>
-      <c r="G103" s="95">
-        <f>E103*C96</f>
-        <v>6.1797777270766066</v>
-      </c>
-      <c r="J103" t="s">
-        <v>92</v>
-      </c>
-      <c r="K103" s="96">
-        <f>K101/K100</f>
-        <v>1.2717278634695841</v>
-      </c>
-      <c r="L103">
-        <f>K103*180</f>
-        <v>228.91101542452515</v>
-      </c>
+      <c r="G103" s="95"/>
+      <c r="K103" s="96"/>
       <c r="M103" s="95"/>
-      <c r="N103" s="95">
-        <f>L103*J96</f>
-        <v>4.5782203084905033</v>
-      </c>
-      <c r="Q103" t="s">
-        <v>92</v>
-      </c>
-      <c r="R103" s="96">
-        <f>R101/R100</f>
-        <v>0.82685080275122236</v>
-      </c>
-      <c r="S103">
-        <f>R103*180</f>
-        <v>148.83314449522001</v>
-      </c>
+      <c r="N103" s="95"/>
+      <c r="R103" s="96"/>
       <c r="T103" s="95"/>
-      <c r="U103" s="95">
-        <f>S103*Q96</f>
-        <v>2.9766628899044001</v>
-      </c>
-      <c r="X103" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y103" s="96">
-        <f>Y101/Y100</f>
-        <v>0.38197374203286033</v>
-      </c>
-      <c r="Z103">
-        <f>Y103*180</f>
-        <v>68.755273565914862</v>
-      </c>
+      <c r="U103" s="95"/>
+      <c r="Y103" s="96"/>
       <c r="AA103" s="95"/>
-      <c r="AB103" s="95">
-        <f>Z103*X96</f>
-        <v>1.3751054713182973</v>
-      </c>
-    </row>
-    <row r="104" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AB103" s="95"/>
+    </row>
+    <row r="104" spans="4:28" x14ac:dyDescent="0.25">
       <c r="G104" s="95"/>
       <c r="N104" s="95"/>
       <c r="U104" s="95"/>
       <c r="AB104" s="95"/>
     </row>
-    <row r="106" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D106" s="97" t="s">
-        <v>87</v>
-      </c>
+    <row r="106" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D106" s="97"/>
       <c r="E106" s="97"/>
       <c r="F106" s="97"/>
-      <c r="K106" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K106" s="97"/>
       <c r="L106" s="97"/>
       <c r="M106" s="97"/>
-      <c r="R106" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R106" s="97"/>
       <c r="S106" s="97"/>
       <c r="T106" s="97"/>
-      <c r="Y106" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y106" s="97"/>
       <c r="Z106" s="97"/>
       <c r="AA106" s="97"/>
     </row>
-    <row r="107" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D107" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E107">
-        <f>E98-D96</f>
-        <v>2.0749749999999985</v>
-      </c>
-      <c r="F107">
-        <v>1.323062</v>
-      </c>
-      <c r="K107" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L107">
-        <f>L98-K96</f>
-        <v>1.4863749999999987</v>
-      </c>
-      <c r="M107">
-        <v>1.323062</v>
-      </c>
-      <c r="R107" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S107">
-        <f>S98-R96</f>
-        <v>0.89777499999999877</v>
-      </c>
-      <c r="T107">
-        <v>1.323062</v>
-      </c>
-      <c r="Y107" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z107">
-        <f>Z98-Y96</f>
-        <v>0.30917499999999865</v>
-      </c>
-      <c r="AA107">
-        <v>1.323062</v>
-      </c>
-    </row>
-    <row r="109" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>90</v>
-      </c>
-      <c r="C109" t="s">
-        <v>88</v>
-      </c>
-      <c r="D109" s="96">
-        <f>D107+F107</f>
-        <v>1.3230621490115999</v>
-      </c>
+    <row r="107" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D107" s="93"/>
+      <c r="K107" s="93"/>
+      <c r="R107" s="93"/>
+      <c r="Y107" s="93"/>
+    </row>
+    <row r="109" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D109" s="96"/>
       <c r="E109" s="94"/>
-      <c r="I109" t="s">
-        <v>90</v>
-      </c>
-      <c r="J109" t="s">
-        <v>88</v>
-      </c>
-      <c r="K109" s="96">
-        <f>K107+M107</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K109" s="96"/>
       <c r="L109" s="94"/>
-      <c r="P109" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q109" t="s">
-        <v>88</v>
-      </c>
-      <c r="R109" s="96">
-        <f>R107+T107</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R109" s="96"/>
       <c r="S109" s="94"/>
-      <c r="W109" t="s">
-        <v>90</v>
-      </c>
-      <c r="X109" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y109" s="96">
-        <f>Y107+AA107</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y109" s="96"/>
       <c r="Z109" s="94"/>
     </row>
-    <row r="110" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>91</v>
-      </c>
-      <c r="C110" t="s">
-        <v>89</v>
-      </c>
-      <c r="D110" s="96">
-        <f>E107</f>
-        <v>2.0749749999999985</v>
-      </c>
+    <row r="110" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D110" s="96"/>
       <c r="G110" s="95"/>
       <c r="H110" s="96"/>
-      <c r="I110" t="s">
-        <v>91</v>
-      </c>
-      <c r="J110" t="s">
-        <v>89</v>
-      </c>
-      <c r="K110" s="96">
-        <f>L107</f>
-        <v>1.4863749999999987</v>
-      </c>
+      <c r="K110" s="96"/>
       <c r="N110" s="95"/>
-      <c r="P110" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q110" t="s">
-        <v>89</v>
-      </c>
-      <c r="R110" s="96">
-        <f>S107</f>
-        <v>0.89777499999999877</v>
-      </c>
+      <c r="R110" s="96"/>
       <c r="U110" s="95"/>
-      <c r="W110" t="s">
-        <v>91</v>
-      </c>
-      <c r="X110" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y110" s="96">
-        <f>Z107</f>
-        <v>0.30917499999999865</v>
-      </c>
+      <c r="Y110" s="96"/>
       <c r="AB110" s="95"/>
     </row>
-    <row r="112" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
-        <v>92</v>
-      </c>
-      <c r="D112" s="96">
-        <f>D110/D109</f>
-        <v>1.5683125706151588</v>
-      </c>
-      <c r="E112">
-        <f>D112*180</f>
-        <v>282.29626271072857</v>
-      </c>
+    <row r="112" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D112" s="96"/>
       <c r="F112" s="95"/>
-      <c r="G112" s="95">
-        <f>E112*C96</f>
-        <v>5.6459252542145713</v>
-      </c>
-      <c r="J112" t="s">
-        <v>92</v>
-      </c>
-      <c r="K112" s="96">
-        <f>K110/K109</f>
-        <v>1.123435509896797</v>
-      </c>
-      <c r="L112">
-        <f>K112*180</f>
-        <v>202.21839178142346</v>
-      </c>
+      <c r="G112" s="95"/>
+      <c r="K112" s="96"/>
       <c r="M112" s="95"/>
-      <c r="N112" s="95">
-        <f>L112*J96</f>
-        <v>4.0443678356284689</v>
-      </c>
-      <c r="Q112" t="s">
-        <v>92</v>
-      </c>
-      <c r="R112" s="96">
-        <f>R110/R109</f>
-        <v>0.678558449178435</v>
-      </c>
-      <c r="S112">
-        <f>R112*180</f>
-        <v>122.1405208521183</v>
-      </c>
+      <c r="N112" s="95"/>
+      <c r="R112" s="96"/>
       <c r="T112" s="95"/>
-      <c r="U112" s="95">
-        <f>S112*Q96</f>
-        <v>2.4428104170423661</v>
-      </c>
-      <c r="X112" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y112" s="96">
-        <f>Y110/Y109</f>
-        <v>0.233681388460073</v>
-      </c>
-      <c r="Z112">
-        <f>Y112*180</f>
-        <v>42.062649922813137</v>
-      </c>
+      <c r="U112" s="95"/>
+      <c r="Y112" s="96"/>
       <c r="AA112" s="95"/>
-      <c r="AB112" s="95">
-        <f>Z112*X96</f>
-        <v>0.84125299845626278</v>
-      </c>
+      <c r="AB112" s="95"/>
     </row>
     <row r="113" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D113" s="94"/>
@@ -6075,244 +4308,61 @@
       <c r="AB114" s="95"/>
     </row>
     <row r="116" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D116" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="D116" s="97"/>
       <c r="E116" s="97"/>
       <c r="F116" s="97"/>
-      <c r="K116" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="K116" s="97"/>
       <c r="L116" s="97"/>
       <c r="M116" s="97"/>
-      <c r="R116" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="R116" s="97"/>
       <c r="S116" s="97"/>
       <c r="T116" s="97"/>
-      <c r="Y116" s="97" t="s">
-        <v>87</v>
-      </c>
+      <c r="Y116" s="97"/>
       <c r="Z116" s="97"/>
       <c r="AA116" s="97"/>
     </row>
     <row r="117" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D117" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="E117">
-        <f>E107-D96</f>
-        <v>1.8787749999999985</v>
-      </c>
-      <c r="F117">
-        <v>1.323062</v>
-      </c>
-      <c r="K117" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="L117">
-        <f>L107-K96</f>
-        <v>1.2901749999999987</v>
-      </c>
-      <c r="M117">
-        <v>1.323062</v>
-      </c>
-      <c r="R117" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="S117">
-        <f>S107-R96</f>
-        <v>0.70157499999999873</v>
-      </c>
-      <c r="T117">
-        <v>1.323062</v>
-      </c>
-      <c r="Y117" s="93">
-        <v>1.4901159999999999E-7</v>
-      </c>
-      <c r="Z117">
-        <f>Z107-Y96</f>
-        <v>0.11297499999999863</v>
-      </c>
-      <c r="AA117">
-        <v>1.323062</v>
-      </c>
+      <c r="D117" s="93"/>
+      <c r="K117" s="93"/>
+      <c r="R117" s="93"/>
+      <c r="Y117" s="93"/>
     </row>
     <row r="119" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>90</v>
-      </c>
-      <c r="C119" t="s">
-        <v>88</v>
-      </c>
-      <c r="D119" s="96">
-        <f>D117+F117</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="D119" s="96"/>
       <c r="E119" s="94"/>
-      <c r="I119" t="s">
-        <v>90</v>
-      </c>
-      <c r="J119" t="s">
-        <v>88</v>
-      </c>
-      <c r="K119" s="96">
-        <f>K117+M117</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="K119" s="96"/>
       <c r="L119" s="94"/>
-      <c r="P119" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q119" t="s">
-        <v>88</v>
-      </c>
-      <c r="R119" s="96">
-        <f>R117+T117</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="R119" s="96"/>
       <c r="S119" s="94"/>
-      <c r="W119" t="s">
-        <v>90</v>
-      </c>
-      <c r="X119" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y119" s="96">
-        <f>Y117+AA117</f>
-        <v>1.3230621490115999</v>
-      </c>
+      <c r="Y119" s="96"/>
       <c r="Z119" s="94"/>
     </row>
     <row r="120" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
-        <v>91</v>
-      </c>
-      <c r="C120" t="s">
-        <v>89</v>
-      </c>
-      <c r="D120" s="96">
-        <f>E117</f>
-        <v>1.8787749999999985</v>
-      </c>
-      <c r="I120" t="s">
-        <v>91</v>
-      </c>
-      <c r="J120" t="s">
-        <v>89</v>
-      </c>
-      <c r="K120" s="96">
-        <f>L117</f>
-        <v>1.2901749999999987</v>
-      </c>
-      <c r="P120" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q120" t="s">
-        <v>89</v>
-      </c>
-      <c r="R120" s="96">
-        <f>S117</f>
-        <v>0.70157499999999873</v>
-      </c>
-      <c r="W120" t="s">
-        <v>91</v>
-      </c>
-      <c r="X120" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y120" s="96">
-        <f>Z117</f>
-        <v>0.11297499999999863</v>
-      </c>
+      <c r="D120" s="96"/>
+      <c r="K120" s="96"/>
+      <c r="R120" s="96"/>
+      <c r="Y120" s="96"/>
     </row>
     <row r="122" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C122" t="s">
-        <v>92</v>
-      </c>
-      <c r="D122" s="96">
-        <f>D120/D119</f>
-        <v>1.4200202170423715</v>
-      </c>
-      <c r="E122">
-        <f>D122*180</f>
-        <v>255.60363906762686</v>
-      </c>
+      <c r="D122" s="96"/>
       <c r="F122" s="95"/>
-      <c r="G122" s="95">
-        <f>E122*C96</f>
-        <v>5.1120727813525368</v>
-      </c>
-      <c r="J122" t="s">
-        <v>92</v>
-      </c>
-      <c r="K122" s="96">
-        <f>K120/K119</f>
-        <v>0.97514315632400972</v>
-      </c>
-      <c r="L122">
-        <f>K122*180</f>
-        <v>175.52576813832175</v>
-      </c>
+      <c r="G122" s="95"/>
+      <c r="K122" s="96"/>
       <c r="M122" s="95"/>
-      <c r="N122" s="95">
-        <f>L122*J96</f>
-        <v>3.5105153627664349</v>
-      </c>
-      <c r="Q122" t="s">
-        <v>92</v>
-      </c>
-      <c r="R122" s="96">
-        <f>R120/R119</f>
-        <v>0.53026609560564764</v>
-      </c>
-      <c r="S122">
-        <f>R122*180</f>
-        <v>95.447897209016574</v>
-      </c>
+      <c r="N122" s="95"/>
+      <c r="R122" s="96"/>
       <c r="T122" s="95"/>
-      <c r="U122" s="95">
-        <f>S122*Q96</f>
-        <v>1.9089579441803315</v>
-      </c>
-      <c r="X122" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y122" s="96">
-        <f>Y120/Y119</f>
-        <v>8.538903488728565E-2</v>
-      </c>
-      <c r="Z122">
-        <f>Y122*180</f>
-        <v>15.370026279711418</v>
-      </c>
+      <c r="U122" s="95"/>
+      <c r="Y122" s="96"/>
       <c r="AA122" s="95"/>
-      <c r="AB122" s="95">
-        <f>Z122*X96</f>
-        <v>0.30740052559422837</v>
-      </c>
+      <c r="AB122" s="95"/>
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G124" s="95">
-        <f>G122+G112+G103</f>
-        <v>16.937775762643717</v>
-      </c>
-      <c r="N124" s="95">
-        <f>N122+N112+N103</f>
-        <v>12.133103506885409</v>
-      </c>
-      <c r="U124" s="95">
-        <f>U122+U112+U103</f>
-        <v>7.3284312511270979</v>
-      </c>
-      <c r="AB124" s="95">
-        <f>AB122+AB112+AB103</f>
-        <v>2.5237589953687882</v>
-      </c>
-      <c r="AC124" s="95">
-        <f>SUM(G124:AB124)</f>
-        <v>38.923069516025009</v>
-      </c>
+      <c r="G124" s="95"/>
+      <c r="N124" s="95"/>
+      <c r="U124" s="95"/>
+      <c r="AB124" s="95"/>
+      <c r="AC124" s="95"/>
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A125" s="98"/>
@@ -6346,7 +4396,11 @@
       <c r="AC125" s="98"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="66">
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="R15:T15"/>
     <mergeCell ref="D106:F106"/>
     <mergeCell ref="K106:M106"/>
     <mergeCell ref="R106:T106"/>
@@ -6397,7 +4451,6 @@
     <mergeCell ref="Y35:AA35"/>
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R13:T13"/>
     <mergeCell ref="R23:T23"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="Y4:AA4"/>
@@ -6407,10 +4460,9 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="D23:F23"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K13:M13"/>
     <mergeCell ref="K23:M23"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed typos i comments and added a comment :)
</commit_message>
<xml_diff>
--- a/TODO altCtrlPancake.xlsx
+++ b/TODO altCtrlPancake.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ashley Sands\Amstrike Games\SimPancake3000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EBF4E1-9A34-454B-858C-14810FB5F758}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B8FD29-BEFD-4207-BD4C-61439380DBB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6732AF01-4E77-4178-A282-B4B033BA40EA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6732AF01-4E77-4178-A282-B4B033BA40EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="140">
   <si>
     <t>Project Sheet - Summary</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Even move fucking task stats</t>
   </si>
   <si>
-    <t xml:space="preserve">Task </t>
-  </si>
-  <si>
     <t>Task Compleat</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>Add pancake fire</t>
   </si>
   <si>
-    <t>Add room smoke</t>
-  </si>
-  <si>
     <t>Add a lil bit of force to the pancake to make shore it comes back to the player. IE a bit of backfroce form the force point</t>
   </si>
   <si>
@@ -362,6 +356,118 @@
   </si>
   <si>
     <t>?? Maybe. This seams to of fixed since fixing other bugs</t>
+  </si>
+  <si>
+    <t>Add Mass to pancakes</t>
+  </si>
+  <si>
+    <t>Fixed pancaked turning into bird like shapes</t>
+  </si>
+  <si>
+    <t>wip</t>
+  </si>
+  <si>
+    <t>Make pancakes slide a lil in the fryingPan :)</t>
+  </si>
+  <si>
+    <t>Ok I belive this is happen cus all the joints at hiting max distance at the same time, I think. So I need to either correct the position befor we update the joints or we need temp update the max distance. TBF I think that correcting the position will be better. but is sounds like a pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add destroy pancake </t>
+  </si>
+  <si>
+    <t>Fixed Pancake rising up when its position is being corrected</t>
+  </si>
+  <si>
+    <t>Fix incorrect flip rotation</t>
+  </si>
+  <si>
+    <t>the flip rotation need to be alined with its velocity</t>
+  </si>
+  <si>
+    <t>Add pan smoke</t>
+  </si>
+  <si>
+    <t>Trigger fire alarm and fire fx</t>
+  </si>
+  <si>
+    <t>So when pan reach burnt state it should slowly cook the other side (say x0.25) and once at fire state x0.5 cook speed ??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pan temp need to be more dynamic </t>
+  </si>
+  <si>
+    <t>pancake cook timer need to reset when batter is added to mixture</t>
+  </si>
+  <si>
+    <t>Fix stateTimer not updateing with the remaining time from the last state</t>
+  </si>
+  <si>
+    <t>When pancake go to a fire state the pan should not catch fire untill the other side is at least perfect</t>
+  </si>
+  <si>
+    <t>Make pancake keep the rotation when they land in the pan</t>
+  </si>
+  <si>
+    <t>side up</t>
+  </si>
+  <si>
+    <t>side down</t>
+  </si>
+  <si>
+    <t>Make fire and smake FX more dynamic</t>
+  </si>
+  <si>
+    <t>so its more inline with the pancake</t>
+  </si>
+  <si>
+    <t>Fixed spwaning pancakes and faliing through pan instatly</t>
+  </si>
+  <si>
+    <t>Add pan steam</t>
+  </si>
+  <si>
+    <t>Make pan steam dynamic based on pan temp</t>
+  </si>
+  <si>
+    <t>Improve the heat up / cool down of pan temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currently it heats up far to fast. I think it might be worth take some form of conductive value into account
+</t>
+  </si>
+  <si>
+    <t>Fix pancake force being inverted when on the flip side (side 1 face down)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is causing the pancake to go fling down streat throught the pan. This might be what is causing (ID 38) since for some resason when it is spwaned it starts on face one. </t>
+  </si>
+  <si>
+    <t>Fix pancakes starting on face 1 rater than face 2.</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>Task  Added</t>
+  </si>
+  <si>
+    <t>Fixed pancake be able to flip when in mixture state and sticking when no mixture state</t>
+  </si>
+  <si>
+    <t>It should be the opersit you tit</t>
+  </si>
+  <si>
+    <t>Fixed pancake roating in the opersit direction when face one is down</t>
+  </si>
+  <si>
+    <t>See ID 42, that might fix this.</t>
+  </si>
+  <si>
+    <t>or 43 might of fixed this</t>
+  </si>
+  <si>
+    <t>Im think that I might just scale the object negative when fliped, so that will alow this, we shell see…</t>
   </si>
 </sst>
 </file>
@@ -373,7 +479,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.000E+00"/>
-    <numFmt numFmtId="178" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -894,6 +1000,12 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -948,31 +1060,15 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1228,6 +1324,16 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1242,32 +1348,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B2D132A-8E44-48F1-BBB2-2C53A683D787}" name="Main" displayName="Main" ref="A3:G50" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A3:G50" xr:uid="{041E981F-6BC0-4FDE-ACBA-E530F1EEC1B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B2D132A-8E44-48F1-BBB2-2C53A683D787}" name="Main" displayName="Main" ref="A3:G85" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A3:G85" xr:uid="{041E981F-6BC0-4FDE-ACBA-E530F1EEC1B5}">
+    <filterColumn colId="3">
+      <filters blank="1">
+        <filter val="-"/>
+        <filter val="wip"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{824F3C5E-1D9A-43A1-B8C9-BD326514D302}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{1150AD6D-6BBD-4CBF-9E9A-9902A96F9F82}" name="Task Name" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{F083697A-B89D-45BD-9721-20A038AAB4B0}" name="Task Details" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{85C72231-B520-4C6B-9B33-80C7B98FAEAF}" name="Status" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{4B87CB35-1B38-4C75-BBE3-CA245029C4B8}" name="Group" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{B40BFB71-0609-470A-9EAD-D610C0B87C75}" name="Sub Group" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{23817CE4-D3E3-4F39-ABA0-28388712A836}" name="Notes" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{824F3C5E-1D9A-43A1-B8C9-BD326514D302}" name="ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{1150AD6D-6BBD-4CBF-9E9A-9902A96F9F82}" name="Task Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{F083697A-B89D-45BD-9721-20A038AAB4B0}" name="Task Details" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{85C72231-B520-4C6B-9B33-80C7B98FAEAF}" name="Status" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{4B87CB35-1B38-4C75-BBE3-CA245029C4B8}" name="Group" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{B40BFB71-0609-470A-9EAD-D610C0B87C75}" name="Sub Group" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{23817CE4-D3E3-4F39-ABA0-28388712A836}" name="Notes" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60864319-97C2-48A4-B74F-713E907C5D25}" name="Arduino" displayName="Arduino" ref="A3:G50" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60864319-97C2-48A4-B74F-713E907C5D25}" name="Arduino" displayName="Arduino" ref="A3:G50" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A3:G50" xr:uid="{041E981F-6BC0-4FDE-ACBA-E530F1EEC1B5}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{12C5545D-8B1E-4FB2-8748-F7DBD896D325}" name="ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8D4C031C-DE34-4573-B782-3D586DEEE833}" name="Task Name" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{A2A6B64D-29D1-48FF-A65C-BA0EBD121B5B}" name="Task Details" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{45A6DF31-36F1-4C08-B878-330C15541E2C}" name="Status" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{E20DE365-0A63-46A6-B55D-5E36FCC83D00}" name="Group" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{A90C5265-ADB6-421D-9C00-5E9716201C56}" name="Sub Group" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{92972826-2FDE-4271-B1AE-3D18F97AB66D}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{12C5545D-8B1E-4FB2-8748-F7DBD896D325}" name="ID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{8D4C031C-DE34-4573-B782-3D586DEEE833}" name="Task Name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A2A6B64D-29D1-48FF-A65C-BA0EBD121B5B}" name="Task Details" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{45A6DF31-36F1-4C08-B878-330C15541E2C}" name="Status" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E20DE365-0A63-46A6-B55D-5E36FCC83D00}" name="Group" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{A90C5265-ADB6-421D-9C00-5E9716201C56}" name="Sub Group" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{92972826-2FDE-4271-B1AE-3D18F97AB66D}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1572,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30403D6D-C9A3-4C64-B0D0-8C03B84E3440}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,17 +1704,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
       <c r="J1" s="33"/>
       <c r="K1" s="33"/>
       <c r="L1" s="33"/>
@@ -1619,13 +1732,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="70" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1640,7 +1753,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="5">
-        <v>43651</v>
+        <v>43658</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1649,14 +1762,14 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">_xlfn.DAYS(E4,NOW())</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="9">
         <f>_xlfn.DAYS(E4,C4)</f>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -1666,24 +1779,24 @@
       </c>
       <c r="C6" s="12">
         <f ca="1">1-IF(E5&lt;&gt;0,(C5/E5),0)</f>
-        <v>0.2142857142857143</v>
-      </c>
-      <c r="D6" s="76" t="s">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="D6" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="76"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="8" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -1691,7 +1804,7 @@
       </c>
       <c r="C9" s="14">
         <f>C17+C18+C19+G17+G18+G19</f>
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>11</v>
@@ -1705,14 +1818,14 @@
       </c>
       <c r="G9" s="14">
         <f>C9+E9</f>
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="17">
         <f>C15+G15</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1721,14 +1834,14 @@
       </c>
       <c r="C10" s="18">
         <f>C9/G9</f>
-        <v>0.18181818181818182</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="19">
         <f>E9/G9</f>
-        <v>0.81818181818181823</v>
+        <v>0.5</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>14</v>
@@ -1742,7 +1855,7 @@
       </c>
       <c r="I10" s="21">
         <f>I9/G9</f>
-        <v>0</v>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1754,27 +1867,27 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="82"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="88"/>
       <c r="E13" s="22"/>
-      <c r="F13" s="80" t="s">
+      <c r="F13" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="81"/>
-      <c r="H13" s="82"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="88"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
@@ -1782,11 +1895,11 @@
       </c>
       <c r="C14" s="24">
         <f>COUNTIF(Main[Status], "-")</f>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" s="25">
         <f>C14/C20</f>
-        <v>0.92</v>
+        <v>0.43478260869565216</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="23" t="s">
@@ -1798,7 +1911,7 @@
       </c>
       <c r="H14" s="25">
         <f>G14/G20</f>
-        <v>0.16</v>
+        <v>8.6956521739130432E-2</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1807,11 +1920,11 @@
       </c>
       <c r="C15" s="24">
         <f>COUNTIF(Main[Status], "wip")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="25">
         <f>C15/C20</f>
-        <v>0</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="23" t="s">
@@ -1832,11 +1945,11 @@
       </c>
       <c r="C16" s="24">
         <f>COUNTIF(Main[Status], "testing")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="25">
         <f>C16/C20</f>
-        <v>0</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="23" t="s">
@@ -1857,11 +1970,11 @@
       </c>
       <c r="C17" s="24">
         <f>COUNTIF(Main[Status], "c")</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D17" s="25">
         <f>C17/C20</f>
-        <v>0</v>
+        <v>0.30434782608695654</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="23" t="s">
@@ -1873,7 +1986,7 @@
       </c>
       <c r="H17" s="25">
         <f>G17/G20</f>
-        <v>0.16</v>
+        <v>8.6956521739130432E-2</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1907,11 +2020,11 @@
       </c>
       <c r="C19" s="24">
         <f>COUNTIF(Main[Status], "fixed")</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D19" s="26">
         <f>C19/C20</f>
-        <v>0.08</v>
+        <v>0.19565217391304349</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="23" t="s">
@@ -1932,7 +2045,7 @@
       </c>
       <c r="C20" s="28">
         <f>COUNTA(Main[Status])</f>
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D20" s="29">
         <f>SUM(D14:D19)</f>
@@ -1944,11 +2057,11 @@
       </c>
       <c r="G20" s="28">
         <f>COUNTA(Main[Status])</f>
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H20" s="29">
         <f>SUM(H14:H19)</f>
-        <v>0.32</v>
+        <v>0.17391304347826086</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1957,14 +2070,14 @@
       </c>
       <c r="C21" s="30">
         <f>D14+D15+D16</f>
-        <v>0.92</v>
+        <v>0.5</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="30">
         <f>H14+H15+H16</f>
-        <v>0.16</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="S21" s="67"/>
     </row>
@@ -1974,39 +2087,39 @@
       </c>
       <c r="C22" s="32">
         <f>D17+D18+D19</f>
-        <v>0.08</v>
+        <v>0.5</v>
       </c>
       <c r="F22" s="31" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="32">
         <f>H17+H18+H19</f>
-        <v>0.16</v>
+        <v>8.6956521739130432E-2</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="84" t="s">
+      <c r="A25" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="85"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="86" t="s">
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="86"/>
-      <c r="K25" s="86"/>
-      <c r="L25" s="87" t="s">
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="M25" s="88"/>
-      <c r="N25" s="89"/>
+      <c r="M25" s="94"/>
+      <c r="N25" s="95"/>
       <c r="O25" s="63"/>
     </row>
     <row r="26" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
@@ -2016,61 +2129,61 @@
       <c r="D26" s="35"/>
       <c r="E26" s="35"/>
       <c r="F26" s="35"/>
-      <c r="G26" s="90" t="s">
+      <c r="G26" s="96" t="s">
+        <v>133</v>
+      </c>
+      <c r="H26" s="96" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="90" t="s">
+      <c r="J26" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="I26" s="90" t="s">
+      <c r="K26" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="J26" s="90" t="s">
-        <v>14</v>
-      </c>
-      <c r="K26" s="83" t="s">
+      <c r="L26" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="L26" s="91" t="s">
+      <c r="M26" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="M26" s="92" t="s">
+      <c r="N26" s="89" t="s">
         <v>42</v>
-      </c>
-      <c r="N26" s="83" t="s">
-        <v>43</v>
       </c>
       <c r="O26" s="64"/>
     </row>
     <row r="27" spans="1:19" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="C27" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="D27" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="36" t="s">
         <v>46</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="36" t="s">
-        <v>47</v>
       </c>
       <c r="F27" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="83"/>
-      <c r="L27" s="91"/>
-      <c r="M27" s="92"/>
-      <c r="N27" s="83"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="96"/>
+      <c r="J27" s="96"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="98"/>
+      <c r="N27" s="89"/>
       <c r="O27" s="64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2078,48 +2191,55 @@
         <v>0</v>
       </c>
       <c r="B28" s="40">
-        <v>180</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="43" t="e">
+        <v>43644</v>
+      </c>
+      <c r="C28" s="41">
+        <v>42</v>
+      </c>
+      <c r="D28" s="42">
+        <v>14</v>
+      </c>
+      <c r="E28" s="42">
+        <f>C28-D28</f>
+        <v>28</v>
+      </c>
+      <c r="F28" s="43">
         <f>D28/C28</f>
-        <v>#DIV/0!</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G28" s="44">
         <f>C28</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="H28" s="45">
         <v>0</v>
       </c>
       <c r="I28" s="44">
         <f>D28</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J28" s="46">
         <v>0</v>
       </c>
-      <c r="K28" s="47" t="e">
+      <c r="K28" s="47">
         <f>I28/G28</f>
-        <v>#DIV/0!</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="L28" s="48">
         <f ca="1">IF(NOW()&lt;B28, G28/_xlfn.DAYS(NOW(),C4), G28/_xlfn.DAYS(B28,C4))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M28" s="49">
         <f ca="1">IF(NOW()&lt;B28, I28/_xlfn.DAYS(NOW(),C4), I28/_xlfn.DAYS(B28,C4))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N28" s="50">
         <f>D28/G9</f>
-        <v>0</v>
+        <v>0.25925925925925924</v>
       </c>
       <c r="O28" s="65">
         <f>N28</f>
-        <v>0</v>
+        <v>0.25925925925925924</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2129,48 +2249,57 @@
       <c r="B29" s="40">
         <v>43651</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43" t="e">
-        <f t="shared" ref="F29" si="0">D29/C29</f>
-        <v>#DIV/0!</v>
+      <c r="C29" s="41">
+        <f>G9</f>
+        <v>54</v>
+      </c>
+      <c r="D29" s="42">
+        <f>C9</f>
+        <v>27</v>
+      </c>
+      <c r="E29" s="42">
+        <f>C29-D29</f>
+        <v>27</v>
+      </c>
+      <c r="F29" s="43">
+        <f>D29/C29</f>
+        <v>0.5</v>
       </c>
       <c r="G29" s="44">
         <f>C29-C28</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="45" t="e">
+        <v>12</v>
+      </c>
+      <c r="H29" s="45">
         <f>(G29-G28)/G28</f>
-        <v>#DIV/0!</v>
+        <v>-0.7142857142857143</v>
       </c>
       <c r="I29" s="44">
         <f>D29-D28</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="46" t="e">
+        <v>13</v>
+      </c>
+      <c r="J29" s="46">
         <f>(I29-I28)/I28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K29" s="47" t="e">
-        <f t="shared" ref="K29" si="1">I29/G29</f>
-        <v>#DIV/0!</v>
+        <v>-7.1428571428571425E-2</v>
+      </c>
+      <c r="K29" s="47">
+        <f t="shared" ref="K29" si="0">I29/G29</f>
+        <v>1.0833333333333333</v>
       </c>
       <c r="L29" s="48">
         <f ca="1">IF(NOW()&lt;B29, G29/_xlfn.DAYS(NOW(),B28), G29/_xlfn.DAYS(B29,B28))</f>
-        <v>0</v>
+        <v>1.7142857142857142</v>
       </c>
       <c r="M29" s="49">
         <f ca="1">IF(NOW()&lt;B29, I29/_xlfn.DAYS(NOW(),B28), I29/_xlfn.DAYS(B29,B28))</f>
-        <v>0</v>
+        <v>1.8571428571428572</v>
       </c>
       <c r="N29" s="50">
         <f>D29/G9</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O29" s="65">
         <f>N29-O28</f>
-        <v>0</v>
+        <v>0.24074074074074076</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -2412,7 +2541,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
       <formula>$C$10</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2444,10 +2573,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BDFBF0-BDE3-48CD-9C74-022AECEC1124}">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2464,15 +2593,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
       <c r="H1" s="72"/>
       <c r="I1" s="72"/>
     </row>
@@ -2499,34 +2628,34 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="73">
         <v>0</v>
       </c>
       <c r="B4" s="74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="74"/>
       <c r="D4" s="73" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="G4" s="74"/>
     </row>
-    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="73">
         <v>1</v>
       </c>
       <c r="B5" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="74" t="s">
-        <v>62</v>
-      </c>
       <c r="D5" s="73" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
@@ -2534,10 +2663,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="74" t="s">
         <v>63</v>
-      </c>
-      <c r="C6" s="74" t="s">
-        <v>64</v>
       </c>
       <c r="D6" s="73" t="s">
         <v>32</v>
@@ -2549,7 +2678,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="74"/>
       <c r="D7" s="73" t="s">
@@ -2562,41 +2691,41 @@
         <v>4</v>
       </c>
       <c r="B8" s="74" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="74"/>
       <c r="D8" s="73" t="s">
         <v>32</v>
       </c>
       <c r="G8" s="74" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="73">
         <v>5</v>
       </c>
       <c r="B9" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="74" t="s">
-        <v>68</v>
-      </c>
       <c r="D9" s="73" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="G9" s="74"/>
     </row>
-    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="73">
         <v>6</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="74"/>
       <c r="D10" s="73" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="G10" s="74"/>
     </row>
@@ -2605,7 +2734,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="74"/>
       <c r="D11" s="73" t="s">
@@ -2613,16 +2742,16 @@
       </c>
       <c r="G11" s="74"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="73">
         <v>8</v>
       </c>
       <c r="B12" s="74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="74"/>
       <c r="D12" s="73" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="G12" s="74"/>
     </row>
@@ -2631,11 +2760,11 @@
         <v>9</v>
       </c>
       <c r="B13" s="74" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="C13" s="74"/>
       <c r="D13" s="73" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="G13" s="74"/>
     </row>
@@ -2644,28 +2773,28 @@
         <v>10</v>
       </c>
       <c r="B14" s="74" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" s="74"/>
       <c r="D14" s="73" t="s">
         <v>32</v>
       </c>
       <c r="G14" s="74" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="73">
         <v>11</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" s="74" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D15" s="73" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="G15" s="74"/>
     </row>
@@ -2674,7 +2803,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="74"/>
       <c r="D16" s="73" t="s">
@@ -2687,7 +2816,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="74" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C17" s="74"/>
       <c r="D17" s="73" t="s">
@@ -2700,11 +2829,11 @@
         <v>14</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="74"/>
       <c r="D18" s="73" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="G18" s="74"/>
     </row>
@@ -2713,7 +2842,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19" s="74"/>
       <c r="D19" s="73" t="s">
@@ -2726,10 +2855,10 @@
         <v>16</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C20" s="74" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D20" s="73" t="s">
         <v>32</v>
@@ -2741,10 +2870,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C21" s="74" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" s="73" t="s">
         <v>32</v>
@@ -2756,22 +2885,22 @@
         <v>18</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C22" s="74" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D22" s="73" t="s">
         <v>32</v>
       </c>
       <c r="G22" s="74"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="73">
         <v>19</v>
       </c>
       <c r="B23" s="74" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23" s="74"/>
       <c r="D23" s="73" t="s">
@@ -2784,7 +2913,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="74" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C24" s="74"/>
       <c r="D24" s="73" t="s">
@@ -2797,7 +2926,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="74" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C25" s="74"/>
       <c r="D25" s="73" t="s">
@@ -2810,7 +2939,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="74" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C26" s="74"/>
       <c r="D26" s="73" t="s">
@@ -2823,7 +2952,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="74" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C27" s="74"/>
       <c r="D27" s="73" t="s">
@@ -2831,15 +2960,15 @@
       </c>
       <c r="G27" s="74"/>
     </row>
-    <row r="28" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="73">
         <v>24</v>
       </c>
       <c r="B28" s="74" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C28" s="74" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D28" s="73" t="s">
         <v>22</v>
@@ -2850,129 +2979,523 @@
       <c r="A29" s="73">
         <v>25</v>
       </c>
-      <c r="B29" s="74"/>
+      <c r="B29" s="74" t="s">
+        <v>103</v>
+      </c>
       <c r="C29" s="74"/>
+      <c r="D29" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G29" s="74"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="76.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="73">
         <v>26</v>
       </c>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
+      <c r="B30" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="73" t="s">
+        <v>22</v>
+      </c>
       <c r="G30" s="74"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="73">
         <v>27</v>
       </c>
-      <c r="B31" s="74"/>
+      <c r="B31" s="74" t="s">
+        <v>106</v>
+      </c>
       <c r="C31" s="74"/>
+      <c r="D31" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G31" s="74"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="73">
         <v>28</v>
       </c>
-      <c r="B32" s="74"/>
+      <c r="B32" s="74" t="s">
+        <v>108</v>
+      </c>
       <c r="C32" s="74"/>
+      <c r="D32" s="73" t="s">
+        <v>51</v>
+      </c>
       <c r="G32" s="74"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="73">
         <v>29</v>
       </c>
-      <c r="B33" s="74"/>
+      <c r="B33" s="74" t="s">
+        <v>109</v>
+      </c>
       <c r="C33" s="74"/>
+      <c r="D33" s="73" t="s">
+        <v>22</v>
+      </c>
       <c r="G33" s="74"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="73">
         <v>30</v>
       </c>
-      <c r="B34" s="74"/>
-      <c r="C34" s="74"/>
+      <c r="B34" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="73" t="s">
+        <v>22</v>
+      </c>
       <c r="G34" s="74"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="74"/>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="73">
+        <v>31</v>
+      </c>
+      <c r="B35" s="74" t="s">
+        <v>113</v>
+      </c>
       <c r="C35" s="74"/>
+      <c r="D35" s="73" t="s">
+        <v>51</v>
+      </c>
       <c r="G35" s="74"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
+    <row r="36" spans="1:7" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="73">
+        <v>32</v>
+      </c>
+      <c r="B36" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="73" t="s">
+        <v>51</v>
+      </c>
       <c r="G36" s="74"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="74"/>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="73">
+        <v>33</v>
+      </c>
+      <c r="B37" s="74" t="s">
+        <v>115</v>
+      </c>
       <c r="C37" s="74"/>
+      <c r="D37" s="73" t="s">
+        <v>51</v>
+      </c>
       <c r="G37" s="74"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="74"/>
+    <row r="38" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="73">
+        <v>34</v>
+      </c>
+      <c r="B38" s="74" t="s">
+        <v>116</v>
+      </c>
       <c r="C38" s="74"/>
+      <c r="D38" s="73" t="s">
+        <v>51</v>
+      </c>
       <c r="G38" s="74"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="74"/>
+    <row r="39" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="73">
+        <v>35</v>
+      </c>
+      <c r="B39" s="74" t="s">
+        <v>117</v>
+      </c>
       <c r="C39" s="74"/>
+      <c r="D39" s="73" t="s">
+        <v>22</v>
+      </c>
       <c r="G39" s="74"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="74"/>
-      <c r="C40" s="74"/>
+    <row r="40" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="73">
+        <v>36</v>
+      </c>
+      <c r="B40" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="D40" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G40" s="74"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="74"/>
-      <c r="C41" s="74"/>
+      <c r="A41" s="73">
+        <f>A40+1</f>
+        <v>37</v>
+      </c>
+      <c r="B41" s="74" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G41" s="74"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="74"/>
-      <c r="C42" s="74"/>
-      <c r="G42" s="74"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B43" s="74"/>
+    <row r="42" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="73">
+        <f t="shared" ref="A42:A59" si="0">A41+1</f>
+        <v>38</v>
+      </c>
+      <c r="B42" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="G42" s="74" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="73">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B43" s="74" t="s">
+        <v>125</v>
+      </c>
       <c r="C43" s="74"/>
+      <c r="D43" s="73" t="s">
+        <v>51</v>
+      </c>
       <c r="G43" s="74"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B44" s="74"/>
+    <row r="44" spans="1:7" ht="25.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="73">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B44" s="74" t="s">
+        <v>126</v>
+      </c>
       <c r="C44" s="74"/>
+      <c r="D44" s="73" t="s">
+        <v>51</v>
+      </c>
       <c r="G44" s="74"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B45" s="74"/>
-      <c r="C45" s="74"/>
+    <row r="45" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" s="73">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B45" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="74" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="73" t="s">
+        <v>51</v>
+      </c>
       <c r="G45" s="74"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B46" s="74"/>
-      <c r="C46" s="74"/>
+    <row r="46" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="73">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B46" s="74" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="73" t="s">
+        <v>32</v>
+      </c>
       <c r="G46" s="74"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B47" s="74"/>
+    <row r="47" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="73">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B47" s="74" t="s">
+        <v>131</v>
+      </c>
       <c r="C47" s="74"/>
+      <c r="D47" s="73" t="s">
+        <v>22</v>
+      </c>
       <c r="G47" s="74"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B48" s="74"/>
+    <row r="48" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A48" s="73">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B48" s="74" t="s">
+        <v>136</v>
+      </c>
       <c r="C48" s="74"/>
+      <c r="D48" s="73" t="s">
+        <v>22</v>
+      </c>
       <c r="G48" s="74"/>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="74"/>
-      <c r="C49" s="74"/>
+    <row r="49" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="73">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B49" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" s="74" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="73" t="s">
+        <v>22</v>
+      </c>
       <c r="G49" s="74"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="73">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
       <c r="B50" s="74"/>
       <c r="C50" s="74"/>
       <c r="G50" s="74"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="73">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B51" s="74"/>
+      <c r="C51" s="74"/>
+      <c r="G51" s="74"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="73">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B52" s="74"/>
+      <c r="C52" s="74"/>
+      <c r="G52" s="74"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="73">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B53" s="74"/>
+      <c r="C53" s="74"/>
+      <c r="G53" s="74"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="73">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B54" s="74"/>
+      <c r="C54" s="74"/>
+      <c r="G54" s="74"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="73">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B55" s="74"/>
+      <c r="C55" s="74"/>
+      <c r="G55" s="74"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="73">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B56" s="74"/>
+      <c r="C56" s="74"/>
+      <c r="G56" s="74"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="73">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B57" s="74"/>
+      <c r="C57" s="74"/>
+      <c r="G57" s="74"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="73">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B58" s="74"/>
+      <c r="C58" s="74"/>
+      <c r="G58" s="74"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="73">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B59" s="74"/>
+      <c r="C59" s="74"/>
+      <c r="G59" s="74"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B60" s="74"/>
+      <c r="C60" s="74"/>
+      <c r="G60" s="74"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B61" s="74"/>
+      <c r="C61" s="74"/>
+      <c r="G61" s="74"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B62" s="74"/>
+      <c r="C62" s="74"/>
+      <c r="G62" s="74"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B63" s="74"/>
+      <c r="C63" s="74"/>
+      <c r="G63" s="74"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B64" s="74"/>
+      <c r="C64" s="74"/>
+      <c r="G64" s="74"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65" s="74"/>
+      <c r="C65" s="74"/>
+      <c r="G65" s="74"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B66" s="74"/>
+      <c r="C66" s="74"/>
+      <c r="G66" s="74"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="74"/>
+      <c r="C67" s="74"/>
+      <c r="G67" s="74"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B68" s="74"/>
+      <c r="C68" s="74"/>
+      <c r="G68" s="74"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B69" s="74"/>
+      <c r="C69" s="74"/>
+      <c r="G69" s="74"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B70" s="74"/>
+      <c r="C70" s="74"/>
+      <c r="G70" s="74"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B71" s="74"/>
+      <c r="C71" s="74"/>
+      <c r="G71" s="74"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B72" s="74"/>
+      <c r="C72" s="74"/>
+      <c r="G72" s="74"/>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B73" s="74"/>
+      <c r="C73" s="74"/>
+      <c r="G73" s="74"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B74" s="74"/>
+      <c r="C74" s="74"/>
+      <c r="G74" s="74"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B75" s="74"/>
+      <c r="C75" s="74"/>
+      <c r="G75" s="74"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B76" s="74"/>
+      <c r="C76" s="74"/>
+      <c r="G76" s="74"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B77" s="74"/>
+      <c r="C77" s="74"/>
+      <c r="G77" s="74"/>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B78" s="74"/>
+      <c r="C78" s="74"/>
+      <c r="G78" s="74"/>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B79" s="74"/>
+      <c r="C79" s="74"/>
+      <c r="G79" s="74"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B80" s="74"/>
+      <c r="C80" s="74"/>
+      <c r="G80" s="74"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B81" s="74"/>
+      <c r="C81" s="74"/>
+      <c r="G81" s="74"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B82" s="74"/>
+      <c r="C82" s="74"/>
+      <c r="G82" s="74"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B83" s="74"/>
+      <c r="C83" s="74"/>
+      <c r="G83" s="74"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B84" s="74"/>
+      <c r="C84" s="74"/>
+      <c r="G84" s="74"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B85" s="74"/>
+      <c r="C85" s="74"/>
+      <c r="G85" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2991,7 +3514,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B9" sqref="B7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3008,15 +3531,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
       <c r="H1" s="72"/>
       <c r="I1" s="72"/>
     </row>
@@ -3048,10 +3571,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="74" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -3059,7 +3582,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="73" t="s">
         <v>32</v>
@@ -3070,7 +3593,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="73" t="s">
         <v>32</v>
@@ -3081,10 +3604,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="73" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -3092,10 +3615,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3103,10 +3626,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -3114,7 +3637,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>32</v>
@@ -3125,7 +3648,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="73" t="s">
         <v>32</v>
@@ -3162,14 +3685,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A58165-66D3-4FDC-A087-9321E2B81B62}">
   <dimension ref="A1:AC125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3180,30 +3704,30 @@
       </c>
     </row>
     <row r="2" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B2" s="97" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="J2" s="97" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="P2" s="97" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97"/>
+      <c r="B2" s="99" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="J2" s="99" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="P2" s="99" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="99"/>
       <c r="T2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U2">
         <v>90</v>
       </c>
-      <c r="W2" s="97"/>
-      <c r="X2" s="97"/>
-      <c r="Y2" s="97"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3">
@@ -3241,27 +3765,27 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D4" s="97" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="L4" s="97" t="s">
-        <v>87</v>
-      </c>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="R4" s="97" t="s">
-        <v>87</v>
-      </c>
-      <c r="S4" s="97"/>
-      <c r="T4" s="97"/>
-      <c r="Y4" s="97"/>
-      <c r="Z4" s="97"/>
-      <c r="AA4" s="97"/>
+      <c r="D4" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="L4" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99"/>
+      <c r="R4" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="Y4" s="99"/>
+      <c r="Z4" s="99"/>
+      <c r="AA4" s="99"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D5" s="93">
+      <c r="D5" s="75">
         <v>-1.3187679999999999</v>
       </c>
       <c r="E5">
@@ -3270,7 +3794,7 @@
       <c r="F5">
         <v>2.7384539999999999</v>
       </c>
-      <c r="L5" s="93">
+      <c r="L5" s="75">
         <v>1.3187679999999999</v>
       </c>
       <c r="M5">
@@ -3279,7 +3803,7 @@
       <c r="N5">
         <v>2.7384539999999999</v>
       </c>
-      <c r="R5" s="93">
+      <c r="R5" s="75">
         <v>1.49E-7</v>
       </c>
       <c r="S5">
@@ -3288,88 +3812,88 @@
       <c r="T5">
         <v>1.323062</v>
       </c>
-      <c r="Y5" s="93"/>
+      <c r="Y5" s="75"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="96">
+        <v>86</v>
+      </c>
+      <c r="D7" s="78">
         <f>D5+F5</f>
         <v>1.419686</v>
       </c>
-      <c r="E7" s="94"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="96"/>
+      <c r="E7" s="76"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="78"/>
       <c r="J7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K7" t="s">
-        <v>88</v>
-      </c>
-      <c r="L7" s="96">
+        <v>86</v>
+      </c>
+      <c r="L7" s="78">
         <f>(L5+N5)/2</f>
         <v>2.0286109999999997</v>
       </c>
-      <c r="M7" s="94"/>
-      <c r="O7" s="95"/>
+      <c r="M7" s="76"/>
+      <c r="O7" s="77"/>
       <c r="P7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q7" t="s">
-        <v>88</v>
-      </c>
-      <c r="R7" s="93">
+        <v>86</v>
+      </c>
+      <c r="R7" s="75">
         <f>(R5+T5)/2</f>
         <v>0.66153107449999993</v>
       </c>
-      <c r="S7" s="94"/>
-      <c r="U7" s="95"/>
-      <c r="Y7" s="96"/>
-      <c r="Z7" s="94"/>
-      <c r="AB7" s="95"/>
+      <c r="S7" s="76"/>
+      <c r="U7" s="77"/>
+      <c r="Y7" s="78"/>
+      <c r="Z7" s="76"/>
+      <c r="AB7" s="77"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="96">
+        <v>87</v>
+      </c>
+      <c r="D8" s="78">
         <f>E5</f>
         <v>7.2</v>
       </c>
       <c r="J8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
-      </c>
-      <c r="L8" s="96">
+        <v>87</v>
+      </c>
+      <c r="L8" s="78">
         <f>M5</f>
         <v>7.2</v>
       </c>
       <c r="P8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q8" t="s">
-        <v>89</v>
-      </c>
-      <c r="R8" s="96">
+        <v>87</v>
+      </c>
+      <c r="R8" s="78">
         <f>S5</f>
         <v>4.6255750000000004</v>
       </c>
-      <c r="Y8" s="96"/>
+      <c r="Y8" s="78"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="96">
+        <v>90</v>
+      </c>
+      <c r="D10" s="78">
         <f>D8/D7</f>
         <v>5.0715439893046774</v>
       </c>
@@ -3377,15 +3901,15 @@
         <f>D10*180</f>
         <v>912.87791807484189</v>
       </c>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95">
+      <c r="F10" s="77"/>
+      <c r="G10" s="77">
         <f>E10*C3</f>
         <v>18.257558361496837</v>
       </c>
       <c r="K10" t="s">
-        <v>92</v>
-      </c>
-      <c r="L10" s="96">
+        <v>90</v>
+      </c>
+      <c r="L10" s="78">
         <f>L8*L7</f>
         <v>14.605999199999998</v>
       </c>
@@ -3393,15 +3917,15 @@
         <f>L10*U2</f>
         <v>1314.5399279999997</v>
       </c>
-      <c r="N10" s="95"/>
-      <c r="O10" s="95">
+      <c r="N10" s="77"/>
+      <c r="O10" s="77">
         <f>M10*K3</f>
         <v>26.290798559999995</v>
       </c>
       <c r="Q10" t="s">
-        <v>92</v>
-      </c>
-      <c r="R10" s="96">
+        <v>90</v>
+      </c>
+      <c r="R10" s="78">
         <f>R8*R7</f>
         <v>3.0599615999303373</v>
       </c>
@@ -3409,55 +3933,55 @@
         <f>R10*U2</f>
         <v>275.39654399373035</v>
       </c>
-      <c r="T10" s="95"/>
-      <c r="U10" s="95">
+      <c r="T10" s="77"/>
+      <c r="U10" s="77">
         <f>S10*Q3</f>
         <v>5.5079308798746069</v>
       </c>
-      <c r="Y10" s="96"/>
-      <c r="AA10" s="95"/>
-      <c r="AB10" s="95"/>
+      <c r="Y10" s="78"/>
+      <c r="AA10" s="77"/>
+      <c r="AB10" s="77"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="G11" s="95"/>
+      <c r="G11" s="77"/>
       <c r="L11">
         <f>L7/L8</f>
         <v>0.28175152777777773</v>
       </c>
-      <c r="O11" s="95"/>
-      <c r="R11" s="95">
+      <c r="O11" s="77"/>
+      <c r="R11" s="77">
         <f>R7/R8</f>
         <v>0.14301596547456261</v>
       </c>
-      <c r="U11" s="95"/>
-      <c r="AB11" s="95"/>
+      <c r="U11" s="77"/>
+      <c r="AB11" s="77"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="J13" s="97" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="P13" s="97" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q13" s="97"/>
-      <c r="R13" s="97"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="99"/>
+      <c r="J13" s="99" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="99"/>
+      <c r="L13" s="99"/>
+      <c r="P13" s="99" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q13" s="99"/>
+      <c r="R13" s="99"/>
       <c r="T13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U13">
         <v>90</v>
       </c>
-      <c r="Y13" s="97"/>
-      <c r="Z13" s="97"/>
-      <c r="AA13" s="97"/>
+      <c r="Y13" s="99"/>
+      <c r="Z13" s="99"/>
+      <c r="AA13" s="99"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D14" s="93"/>
+      <c r="D14" s="75"/>
       <c r="J14">
         <v>9.81</v>
       </c>
@@ -3480,24 +4004,24 @@
         <f>P14*Q14</f>
         <v>0.19620000000000001</v>
       </c>
-      <c r="Y14" s="93"/>
+      <c r="Y14" s="75"/>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="L15" s="97" t="s">
-        <v>87</v>
-      </c>
-      <c r="M15" s="97"/>
-      <c r="N15" s="97"/>
-      <c r="R15" s="97" t="s">
-        <v>87</v>
-      </c>
-      <c r="S15" s="97"/>
-      <c r="T15" s="97"/>
+      <c r="L15" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="M15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="R15" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="S15" s="99"/>
+      <c r="T15" s="99"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="96"/>
-      <c r="E16" s="94"/>
-      <c r="L16" s="93">
+      <c r="D16" s="78"/>
+      <c r="E16" s="76"/>
+      <c r="L16" s="75">
         <v>1.3187679999999999</v>
       </c>
       <c r="M16">
@@ -3506,7 +4030,7 @@
       <c r="N16">
         <v>2.7384539999999999</v>
       </c>
-      <c r="R16" s="99">
+      <c r="R16" s="80">
         <v>1.49E-7</v>
       </c>
       <c r="S16">
@@ -3515,84 +4039,84 @@
       <c r="T16">
         <v>1.323062</v>
       </c>
-      <c r="Y16" s="96"/>
-      <c r="Z16" s="94"/>
+      <c r="Y16" s="78"/>
+      <c r="Z16" s="76"/>
     </row>
     <row r="17" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="D17" s="96"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="96"/>
-      <c r="Y17" s="96"/>
-      <c r="AB17" s="95"/>
+      <c r="D17" s="78"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="78"/>
+      <c r="Y17" s="78"/>
+      <c r="AB17" s="77"/>
     </row>
     <row r="18" spans="4:29" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K18" t="s">
-        <v>99</v>
-      </c>
-      <c r="L18" s="96">
+        <v>97</v>
+      </c>
+      <c r="L18" s="78">
         <f>L16*N16</f>
         <v>3.6113855046719996</v>
       </c>
-      <c r="M18" s="94"/>
-      <c r="O18" s="95"/>
+      <c r="M18" s="76"/>
+      <c r="O18" s="77"/>
       <c r="P18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q18" t="s">
-        <v>99</v>
-      </c>
-      <c r="R18" s="96">
+        <v>97</v>
+      </c>
+      <c r="R18" s="78">
         <f>R16*T16</f>
         <v>1.9713623799999999E-7</v>
       </c>
-      <c r="S18" s="94"/>
-      <c r="U18" s="95"/>
+      <c r="S18" s="76"/>
+      <c r="U18" s="77"/>
     </row>
     <row r="19" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="D19" s="96"/>
-      <c r="F19" s="95"/>
-      <c r="G19" s="95"/>
+      <c r="D19" s="78"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
       <c r="J19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K19" t="s">
-        <v>89</v>
-      </c>
-      <c r="L19" s="96">
+        <v>87</v>
+      </c>
+      <c r="L19" s="78">
         <f>M16</f>
         <v>7.2</v>
       </c>
       <c r="P19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q19" t="s">
-        <v>89</v>
-      </c>
-      <c r="R19" s="96">
+        <v>87</v>
+      </c>
+      <c r="R19" s="78">
         <f>S16</f>
         <v>4.6255750000000004</v>
       </c>
-      <c r="Y19" s="96"/>
-      <c r="AA19" s="95"/>
-      <c r="AB19" s="95"/>
+      <c r="Y19" s="78"/>
+      <c r="AA19" s="77"/>
+      <c r="AB19" s="77"/>
     </row>
     <row r="20" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="D20" s="94"/>
-      <c r="F20" s="95"/>
-      <c r="G20" s="95"/>
-      <c r="Y20" s="94"/>
-      <c r="AA20" s="95"/>
-      <c r="AB20" s="95"/>
+      <c r="D20" s="76"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="Y20" s="76"/>
+      <c r="AA20" s="77"/>
+      <c r="AB20" s="77"/>
     </row>
     <row r="21" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="G21" s="95"/>
+      <c r="G21" s="77"/>
       <c r="K21" t="s">
-        <v>92</v>
-      </c>
-      <c r="L21" s="96">
+        <v>90</v>
+      </c>
+      <c r="L21" s="78">
         <f>L19*L18</f>
         <v>26.001975633638398</v>
       </c>
@@ -3600,839 +4124,846 @@
         <f>L21*U13</f>
         <v>2340.1778070274559</v>
       </c>
-      <c r="N21" s="95"/>
-      <c r="O21" s="95">
+      <c r="N21" s="77"/>
+      <c r="O21" s="77">
         <f>M21*K14</f>
         <v>46.803556140549119</v>
       </c>
       <c r="Q21" t="s">
-        <v>92</v>
-      </c>
-      <c r="R21" s="96">
+        <v>90</v>
+      </c>
+      <c r="R21" s="78">
         <f>R19/R18</f>
         <v>23463849.401447952</v>
       </c>
-      <c r="S21" s="95">
+      <c r="S21" s="77">
         <f>R21*U13</f>
         <v>2111746446.1303158</v>
       </c>
-      <c r="T21" s="95"/>
-      <c r="U21" s="95">
+      <c r="T21" s="77"/>
+      <c r="U21" s="77">
         <f>S21*Q14</f>
         <v>42234928.922606319</v>
       </c>
-      <c r="AB21" s="95"/>
+      <c r="AB21" s="77"/>
     </row>
     <row r="23" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="K23" s="97"/>
-      <c r="L23" s="97"/>
-      <c r="M23" s="97"/>
-      <c r="R23" s="97"/>
-      <c r="S23" s="97"/>
-      <c r="T23" s="97"/>
-      <c r="Y23" s="97"/>
-      <c r="Z23" s="97"/>
-      <c r="AA23" s="97"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="99"/>
+      <c r="K23" s="99"/>
+      <c r="L23" s="99"/>
+      <c r="M23" s="99"/>
+      <c r="R23" s="99"/>
+      <c r="S23" s="99"/>
+      <c r="T23" s="99"/>
+      <c r="Y23" s="99"/>
+      <c r="Z23" s="99"/>
+      <c r="AA23" s="99"/>
     </row>
     <row r="24" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="D24" s="93"/>
-      <c r="K24" s="93"/>
-      <c r="R24" s="93"/>
-      <c r="Y24" s="93"/>
+      <c r="D24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="R24" s="75"/>
+      <c r="Y24" s="75"/>
     </row>
     <row r="26" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="D26" s="96"/>
-      <c r="E26" s="94"/>
-      <c r="K26" s="96"/>
-      <c r="L26" s="94"/>
-      <c r="R26" s="96"/>
-      <c r="S26" s="94"/>
-      <c r="Y26" s="96"/>
-      <c r="Z26" s="94"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="76"/>
+      <c r="K26" s="78"/>
+      <c r="L26" s="76"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="76"/>
+      <c r="Y26" s="78"/>
+      <c r="Z26" s="76"/>
     </row>
     <row r="27" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="D27" s="96"/>
-      <c r="K27" s="96"/>
-      <c r="R27" s="96"/>
-      <c r="Y27" s="96"/>
+      <c r="D27" s="78"/>
+      <c r="K27" s="78"/>
+      <c r="R27" s="78"/>
+      <c r="Y27" s="78"/>
     </row>
     <row r="29" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="D29" s="96"/>
-      <c r="F29" s="95"/>
-      <c r="G29" s="95"/>
-      <c r="K29" s="96"/>
-      <c r="M29" s="95"/>
-      <c r="N29" s="95"/>
-      <c r="R29" s="96"/>
-      <c r="T29" s="95"/>
-      <c r="U29" s="95"/>
-      <c r="Y29" s="96"/>
-      <c r="AA29" s="95"/>
-      <c r="AB29" s="95"/>
+      <c r="D29" s="78"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="K29" s="78"/>
+      <c r="M29" s="77"/>
+      <c r="N29" s="77"/>
+      <c r="R29" s="78"/>
+      <c r="T29" s="77"/>
+      <c r="U29" s="77"/>
+      <c r="Y29" s="78"/>
+      <c r="AA29" s="77"/>
+      <c r="AB29" s="77"/>
     </row>
     <row r="31" spans="4:29" x14ac:dyDescent="0.25">
-      <c r="G31" s="95"/>
-      <c r="N31" s="95"/>
-      <c r="U31" s="95"/>
-      <c r="AB31" s="95"/>
-      <c r="AC31" s="95"/>
-    </row>
-    <row r="32" spans="4:29" s="98" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="G31" s="77"/>
+      <c r="N31" s="77"/>
+      <c r="U31" s="77"/>
+      <c r="AB31" s="77"/>
+      <c r="AC31" s="77"/>
+    </row>
+    <row r="32" spans="4:29" s="79" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B33" s="97"/>
-      <c r="C33" s="97"/>
-      <c r="D33" s="97"/>
-      <c r="I33" s="97"/>
-      <c r="J33" s="97"/>
-      <c r="K33" s="97"/>
-      <c r="P33" s="97"/>
-      <c r="Q33" s="97"/>
-      <c r="R33" s="97"/>
-      <c r="W33" s="97"/>
-      <c r="X33" s="97"/>
-      <c r="Y33" s="97"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="99"/>
+      <c r="I33" s="99"/>
+      <c r="J33" s="99"/>
+      <c r="K33" s="99"/>
+      <c r="P33" s="99"/>
+      <c r="Q33" s="99"/>
+      <c r="R33" s="99"/>
+      <c r="W33" s="99"/>
+      <c r="X33" s="99"/>
+      <c r="Y33" s="99"/>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D35" s="97"/>
-      <c r="E35" s="97"/>
-      <c r="F35" s="97"/>
-      <c r="K35" s="97"/>
-      <c r="L35" s="97"/>
-      <c r="M35" s="97"/>
-      <c r="R35" s="97"/>
-      <c r="S35" s="97"/>
-      <c r="T35" s="97"/>
-      <c r="Y35" s="97"/>
-      <c r="Z35" s="97"/>
-      <c r="AA35" s="97"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="99"/>
+      <c r="F35" s="99"/>
+      <c r="K35" s="99"/>
+      <c r="L35" s="99"/>
+      <c r="M35" s="99"/>
+      <c r="R35" s="99"/>
+      <c r="S35" s="99"/>
+      <c r="T35" s="99"/>
+      <c r="Y35" s="99"/>
+      <c r="Z35" s="99"/>
+      <c r="AA35" s="99"/>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D36" s="93"/>
-      <c r="K36" s="93"/>
-      <c r="R36" s="93"/>
-      <c r="Y36" s="93"/>
+      <c r="D36" s="75"/>
+      <c r="K36" s="75"/>
+      <c r="R36" s="75"/>
+      <c r="Y36" s="75"/>
     </row>
     <row r="38" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D38" s="96"/>
-      <c r="E38" s="94"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="96"/>
-      <c r="K38" s="96"/>
-      <c r="L38" s="94"/>
-      <c r="N38" s="95"/>
-      <c r="R38" s="96"/>
-      <c r="S38" s="94"/>
-      <c r="U38" s="95"/>
-      <c r="Y38" s="96"/>
-      <c r="Z38" s="94"/>
-      <c r="AB38" s="95"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="76"/>
+      <c r="G38" s="77"/>
+      <c r="H38" s="78"/>
+      <c r="J38" t="s">
+        <v>121</v>
+      </c>
+      <c r="K38" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="L38" s="76"/>
+      <c r="N38" s="77"/>
+      <c r="R38" s="78"/>
+      <c r="S38" s="76"/>
+      <c r="U38" s="77"/>
+      <c r="Y38" s="78"/>
+      <c r="Z38" s="76"/>
+      <c r="AB38" s="77"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D39" s="96"/>
-      <c r="K39" s="96"/>
-      <c r="R39" s="96"/>
-      <c r="Y39" s="96"/>
+      <c r="D39" s="78"/>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39" s="78">
+        <f>1-J39</f>
+        <v>1</v>
+      </c>
+      <c r="R39" s="78"/>
+      <c r="Y39" s="78"/>
     </row>
     <row r="41" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D41" s="96"/>
-      <c r="F41" s="95"/>
-      <c r="G41" s="95"/>
-      <c r="K41" s="96"/>
-      <c r="M41" s="95"/>
-      <c r="N41" s="95"/>
-      <c r="R41" s="96"/>
-      <c r="T41" s="95"/>
-      <c r="U41" s="95"/>
-      <c r="Y41" s="96"/>
-      <c r="AA41" s="95"/>
-      <c r="AB41" s="95"/>
+      <c r="D41" s="78"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="77"/>
+      <c r="K41" s="78"/>
+      <c r="M41" s="77"/>
+      <c r="N41" s="77"/>
+      <c r="R41" s="78"/>
+      <c r="T41" s="77"/>
+      <c r="U41" s="77"/>
+      <c r="Y41" s="78"/>
+      <c r="AA41" s="77"/>
+      <c r="AB41" s="77"/>
     </row>
     <row r="42" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="G42" s="95"/>
-      <c r="N42" s="95"/>
-      <c r="U42" s="95"/>
-      <c r="AB42" s="95"/>
+      <c r="G42" s="77"/>
+      <c r="N42" s="77"/>
+      <c r="U42" s="77"/>
+      <c r="AB42" s="77"/>
     </row>
     <row r="44" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D44" s="97"/>
-      <c r="E44" s="97"/>
-      <c r="F44" s="97"/>
-      <c r="K44" s="97"/>
-      <c r="L44" s="97"/>
-      <c r="M44" s="97"/>
-      <c r="R44" s="97"/>
-      <c r="S44" s="97"/>
-      <c r="T44" s="97"/>
-      <c r="Y44" s="97"/>
-      <c r="Z44" s="97"/>
-      <c r="AA44" s="97"/>
+      <c r="D44" s="99"/>
+      <c r="E44" s="99"/>
+      <c r="F44" s="99"/>
+      <c r="K44" s="99"/>
+      <c r="L44" s="99"/>
+      <c r="M44" s="99"/>
+      <c r="R44" s="99"/>
+      <c r="S44" s="99"/>
+      <c r="T44" s="99"/>
+      <c r="Y44" s="99"/>
+      <c r="Z44" s="99"/>
+      <c r="AA44" s="99"/>
     </row>
     <row r="45" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D45" s="93"/>
-      <c r="K45" s="93"/>
-      <c r="R45" s="93"/>
-      <c r="Y45" s="93"/>
+      <c r="D45" s="75"/>
+      <c r="K45" s="75"/>
+      <c r="R45" s="75"/>
+      <c r="Y45" s="75"/>
     </row>
     <row r="47" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D47" s="96"/>
-      <c r="E47" s="94"/>
-      <c r="K47" s="96"/>
-      <c r="L47" s="94"/>
-      <c r="R47" s="96"/>
-      <c r="S47" s="94"/>
-      <c r="Y47" s="96"/>
-      <c r="Z47" s="94"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="76"/>
+      <c r="K47" s="78"/>
+      <c r="L47" s="76"/>
+      <c r="R47" s="78"/>
+      <c r="S47" s="76"/>
+      <c r="Y47" s="78"/>
+      <c r="Z47" s="76"/>
     </row>
     <row r="48" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D48" s="96"/>
-      <c r="G48" s="95"/>
-      <c r="H48" s="96"/>
-      <c r="K48" s="96"/>
-      <c r="N48" s="95"/>
-      <c r="R48" s="96"/>
-      <c r="U48" s="95"/>
-      <c r="Y48" s="96"/>
-      <c r="AB48" s="95"/>
+      <c r="D48" s="78"/>
+      <c r="G48" s="77"/>
+      <c r="H48" s="78"/>
+      <c r="K48" s="78"/>
+      <c r="N48" s="77"/>
+      <c r="R48" s="78"/>
+      <c r="U48" s="77"/>
+      <c r="Y48" s="78"/>
+      <c r="AB48" s="77"/>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D50" s="96"/>
-      <c r="F50" s="95"/>
-      <c r="G50" s="95"/>
-      <c r="K50" s="96"/>
-      <c r="M50" s="95"/>
-      <c r="N50" s="95"/>
-      <c r="R50" s="96"/>
-      <c r="T50" s="95"/>
-      <c r="U50" s="95"/>
-      <c r="Y50" s="96"/>
-      <c r="AA50" s="95"/>
-      <c r="AB50" s="95"/>
+      <c r="D50" s="78"/>
+      <c r="F50" s="77"/>
+      <c r="G50" s="77"/>
+      <c r="K50" s="78"/>
+      <c r="M50" s="77"/>
+      <c r="N50" s="77"/>
+      <c r="R50" s="78"/>
+      <c r="T50" s="77"/>
+      <c r="U50" s="77"/>
+      <c r="Y50" s="78"/>
+      <c r="AA50" s="77"/>
+      <c r="AB50" s="77"/>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D51" s="94"/>
-      <c r="F51" s="95"/>
-      <c r="G51" s="95"/>
-      <c r="K51" s="94"/>
-      <c r="M51" s="95"/>
-      <c r="N51" s="95"/>
-      <c r="R51" s="94"/>
-      <c r="T51" s="95"/>
-      <c r="U51" s="95"/>
-      <c r="Y51" s="94"/>
-      <c r="AA51" s="95"/>
-      <c r="AB51" s="95"/>
+      <c r="D51" s="76"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="77"/>
+      <c r="K51" s="76"/>
+      <c r="M51" s="77"/>
+      <c r="N51" s="77"/>
+      <c r="R51" s="76"/>
+      <c r="T51" s="77"/>
+      <c r="U51" s="77"/>
+      <c r="Y51" s="76"/>
+      <c r="AA51" s="77"/>
+      <c r="AB51" s="77"/>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G52" s="95"/>
-      <c r="N52" s="95"/>
-      <c r="U52" s="95"/>
-      <c r="AB52" s="95"/>
+      <c r="G52" s="77"/>
+      <c r="N52" s="77"/>
+      <c r="U52" s="77"/>
+      <c r="AB52" s="77"/>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D54" s="97"/>
-      <c r="E54" s="97"/>
-      <c r="F54" s="97"/>
-      <c r="K54" s="97"/>
-      <c r="L54" s="97"/>
-      <c r="M54" s="97"/>
-      <c r="R54" s="97"/>
-      <c r="S54" s="97"/>
-      <c r="T54" s="97"/>
-      <c r="Y54" s="97"/>
-      <c r="Z54" s="97"/>
-      <c r="AA54" s="97"/>
+      <c r="D54" s="99"/>
+      <c r="E54" s="99"/>
+      <c r="F54" s="99"/>
+      <c r="K54" s="99"/>
+      <c r="L54" s="99"/>
+      <c r="M54" s="99"/>
+      <c r="R54" s="99"/>
+      <c r="S54" s="99"/>
+      <c r="T54" s="99"/>
+      <c r="Y54" s="99"/>
+      <c r="Z54" s="99"/>
+      <c r="AA54" s="99"/>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D55" s="93"/>
-      <c r="K55" s="93"/>
-      <c r="R55" s="93"/>
-      <c r="Y55" s="93"/>
+      <c r="D55" s="75"/>
+      <c r="K55" s="75"/>
+      <c r="R55" s="75"/>
+      <c r="Y55" s="75"/>
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D57" s="96"/>
-      <c r="E57" s="94"/>
-      <c r="K57" s="96"/>
-      <c r="L57" s="94"/>
-      <c r="R57" s="96"/>
-      <c r="S57" s="94"/>
-      <c r="Y57" s="96"/>
-      <c r="Z57" s="94"/>
+      <c r="D57" s="78"/>
+      <c r="E57" s="76"/>
+      <c r="K57" s="78"/>
+      <c r="L57" s="76"/>
+      <c r="R57" s="78"/>
+      <c r="S57" s="76"/>
+      <c r="Y57" s="78"/>
+      <c r="Z57" s="76"/>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D58" s="96"/>
-      <c r="K58" s="96"/>
-      <c r="R58" s="96"/>
-      <c r="Y58" s="96"/>
+      <c r="D58" s="78"/>
+      <c r="K58" s="78"/>
+      <c r="R58" s="78"/>
+      <c r="Y58" s="78"/>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D60" s="96"/>
-      <c r="F60" s="95"/>
-      <c r="G60" s="95"/>
-      <c r="K60" s="96"/>
-      <c r="M60" s="95"/>
-      <c r="N60" s="95"/>
-      <c r="R60" s="96"/>
-      <c r="T60" s="95"/>
-      <c r="U60" s="95"/>
-      <c r="Y60" s="96"/>
-      <c r="AA60" s="95"/>
-      <c r="AB60" s="95"/>
+      <c r="D60" s="78"/>
+      <c r="F60" s="77"/>
+      <c r="G60" s="77"/>
+      <c r="K60" s="78"/>
+      <c r="M60" s="77"/>
+      <c r="N60" s="77"/>
+      <c r="R60" s="78"/>
+      <c r="T60" s="77"/>
+      <c r="U60" s="77"/>
+      <c r="Y60" s="78"/>
+      <c r="AA60" s="77"/>
+      <c r="AB60" s="77"/>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G62" s="95"/>
-      <c r="N62" s="95"/>
-      <c r="U62" s="95"/>
-      <c r="AB62" s="95"/>
-      <c r="AC62" s="95"/>
+      <c r="G62" s="77"/>
+      <c r="N62" s="77"/>
+      <c r="U62" s="77"/>
+      <c r="AB62" s="77"/>
+      <c r="AC62" s="77"/>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A63" s="98"/>
-      <c r="B63" s="98"/>
-      <c r="C63" s="98"/>
-      <c r="D63" s="98"/>
-      <c r="E63" s="98"/>
-      <c r="F63" s="98"/>
-      <c r="G63" s="98"/>
-      <c r="H63" s="98"/>
-      <c r="I63" s="98"/>
-      <c r="J63" s="98"/>
-      <c r="K63" s="98"/>
-      <c r="L63" s="98"/>
-      <c r="M63" s="98"/>
-      <c r="N63" s="98"/>
-      <c r="O63" s="98"/>
-      <c r="P63" s="98"/>
-      <c r="Q63" s="98"/>
-      <c r="R63" s="98"/>
-      <c r="S63" s="98"/>
-      <c r="T63" s="98"/>
-      <c r="U63" s="98"/>
-      <c r="V63" s="98"/>
-      <c r="W63" s="98"/>
-      <c r="X63" s="98"/>
-      <c r="Y63" s="98"/>
-      <c r="Z63" s="98"/>
-      <c r="AA63" s="98"/>
-      <c r="AB63" s="98"/>
-      <c r="AC63" s="98"/>
+      <c r="A63" s="79"/>
+      <c r="B63" s="79"/>
+      <c r="C63" s="79"/>
+      <c r="D63" s="79"/>
+      <c r="E63" s="79"/>
+      <c r="F63" s="79"/>
+      <c r="G63" s="79"/>
+      <c r="H63" s="79"/>
+      <c r="I63" s="79"/>
+      <c r="J63" s="79"/>
+      <c r="K63" s="79"/>
+      <c r="L63" s="79"/>
+      <c r="M63" s="79"/>
+      <c r="N63" s="79"/>
+      <c r="O63" s="79"/>
+      <c r="P63" s="79"/>
+      <c r="Q63" s="79"/>
+      <c r="R63" s="79"/>
+      <c r="S63" s="79"/>
+      <c r="T63" s="79"/>
+      <c r="U63" s="79"/>
+      <c r="V63" s="79"/>
+      <c r="W63" s="79"/>
+      <c r="X63" s="79"/>
+      <c r="Y63" s="79"/>
+      <c r="Z63" s="79"/>
+      <c r="AA63" s="79"/>
+      <c r="AB63" s="79"/>
+      <c r="AC63" s="79"/>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B64" s="97"/>
-      <c r="C64" s="97"/>
-      <c r="D64" s="97"/>
-      <c r="I64" s="97"/>
-      <c r="J64" s="97"/>
-      <c r="K64" s="97"/>
-      <c r="P64" s="97"/>
-      <c r="Q64" s="97"/>
-      <c r="R64" s="97"/>
-      <c r="W64" s="97"/>
-      <c r="X64" s="97"/>
-      <c r="Y64" s="97"/>
+      <c r="B64" s="99"/>
+      <c r="C64" s="99"/>
+      <c r="D64" s="99"/>
+      <c r="I64" s="99"/>
+      <c r="J64" s="99"/>
+      <c r="K64" s="99"/>
+      <c r="P64" s="99"/>
+      <c r="Q64" s="99"/>
+      <c r="R64" s="99"/>
+      <c r="W64" s="99"/>
+      <c r="X64" s="99"/>
+      <c r="Y64" s="99"/>
     </row>
     <row r="66" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D66" s="97"/>
-      <c r="E66" s="97"/>
-      <c r="F66" s="97"/>
-      <c r="K66" s="97"/>
-      <c r="L66" s="97"/>
-      <c r="M66" s="97"/>
-      <c r="R66" s="97"/>
-      <c r="S66" s="97"/>
-      <c r="T66" s="97"/>
-      <c r="Y66" s="97"/>
-      <c r="Z66" s="97"/>
-      <c r="AA66" s="97"/>
+      <c r="D66" s="99"/>
+      <c r="E66" s="99"/>
+      <c r="F66" s="99"/>
+      <c r="K66" s="99"/>
+      <c r="L66" s="99"/>
+      <c r="M66" s="99"/>
+      <c r="R66" s="99"/>
+      <c r="S66" s="99"/>
+      <c r="T66" s="99"/>
+      <c r="Y66" s="99"/>
+      <c r="Z66" s="99"/>
+      <c r="AA66" s="99"/>
     </row>
     <row r="67" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D67" s="93"/>
-      <c r="K67" s="93"/>
-      <c r="R67" s="93"/>
-      <c r="Y67" s="93"/>
+      <c r="D67" s="75"/>
+      <c r="K67" s="75"/>
+      <c r="R67" s="75"/>
+      <c r="Y67" s="75"/>
     </row>
     <row r="69" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D69" s="96"/>
-      <c r="E69" s="94"/>
-      <c r="G69" s="95"/>
-      <c r="H69" s="96"/>
-      <c r="K69" s="96"/>
-      <c r="L69" s="94"/>
-      <c r="N69" s="95"/>
-      <c r="R69" s="96"/>
-      <c r="S69" s="94"/>
-      <c r="U69" s="95"/>
-      <c r="Y69" s="96"/>
-      <c r="Z69" s="94"/>
-      <c r="AB69" s="95"/>
+      <c r="D69" s="78"/>
+      <c r="E69" s="76"/>
+      <c r="G69" s="77"/>
+      <c r="H69" s="78"/>
+      <c r="K69" s="78"/>
+      <c r="L69" s="76"/>
+      <c r="N69" s="77"/>
+      <c r="R69" s="78"/>
+      <c r="S69" s="76"/>
+      <c r="U69" s="77"/>
+      <c r="Y69" s="78"/>
+      <c r="Z69" s="76"/>
+      <c r="AB69" s="77"/>
     </row>
     <row r="70" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D70" s="96"/>
-      <c r="K70" s="96"/>
-      <c r="R70" s="96"/>
-      <c r="Y70" s="96"/>
+      <c r="D70" s="78"/>
+      <c r="K70" s="78"/>
+      <c r="R70" s="78"/>
+      <c r="Y70" s="78"/>
     </row>
     <row r="72" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D72" s="96"/>
-      <c r="F72" s="95"/>
-      <c r="G72" s="95"/>
-      <c r="K72" s="96"/>
-      <c r="M72" s="95"/>
-      <c r="N72" s="95"/>
-      <c r="R72" s="96"/>
-      <c r="T72" s="95"/>
-      <c r="U72" s="95"/>
-      <c r="Y72" s="96"/>
-      <c r="AA72" s="95"/>
-      <c r="AB72" s="95"/>
+      <c r="D72" s="78"/>
+      <c r="F72" s="77"/>
+      <c r="G72" s="77"/>
+      <c r="K72" s="78"/>
+      <c r="M72" s="77"/>
+      <c r="N72" s="77"/>
+      <c r="R72" s="78"/>
+      <c r="T72" s="77"/>
+      <c r="U72" s="77"/>
+      <c r="Y72" s="78"/>
+      <c r="AA72" s="77"/>
+      <c r="AB72" s="77"/>
     </row>
     <row r="73" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G73" s="95"/>
-      <c r="N73" s="95"/>
-      <c r="U73" s="95"/>
-      <c r="AB73" s="95"/>
+      <c r="G73" s="77"/>
+      <c r="N73" s="77"/>
+      <c r="U73" s="77"/>
+      <c r="AB73" s="77"/>
     </row>
     <row r="75" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D75" s="97"/>
-      <c r="E75" s="97"/>
-      <c r="F75" s="97"/>
-      <c r="K75" s="97"/>
-      <c r="L75" s="97"/>
-      <c r="M75" s="97"/>
-      <c r="R75" s="97"/>
-      <c r="S75" s="97"/>
-      <c r="T75" s="97"/>
-      <c r="Y75" s="97"/>
-      <c r="Z75" s="97"/>
-      <c r="AA75" s="97"/>
+      <c r="D75" s="99"/>
+      <c r="E75" s="99"/>
+      <c r="F75" s="99"/>
+      <c r="K75" s="99"/>
+      <c r="L75" s="99"/>
+      <c r="M75" s="99"/>
+      <c r="R75" s="99"/>
+      <c r="S75" s="99"/>
+      <c r="T75" s="99"/>
+      <c r="Y75" s="99"/>
+      <c r="Z75" s="99"/>
+      <c r="AA75" s="99"/>
     </row>
     <row r="76" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D76" s="93"/>
-      <c r="K76" s="93"/>
-      <c r="R76" s="93"/>
-      <c r="Y76" s="93"/>
+      <c r="D76" s="75"/>
+      <c r="K76" s="75"/>
+      <c r="R76" s="75"/>
+      <c r="Y76" s="75"/>
     </row>
     <row r="78" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D78" s="96"/>
-      <c r="E78" s="94"/>
-      <c r="K78" s="96"/>
-      <c r="L78" s="94"/>
-      <c r="R78" s="96"/>
-      <c r="S78" s="94"/>
-      <c r="Y78" s="96"/>
-      <c r="Z78" s="94"/>
+      <c r="D78" s="78"/>
+      <c r="E78" s="76"/>
+      <c r="K78" s="78"/>
+      <c r="L78" s="76"/>
+      <c r="R78" s="78"/>
+      <c r="S78" s="76"/>
+      <c r="Y78" s="78"/>
+      <c r="Z78" s="76"/>
     </row>
     <row r="79" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D79" s="96"/>
-      <c r="G79" s="95"/>
-      <c r="H79" s="96"/>
-      <c r="K79" s="96"/>
-      <c r="N79" s="95"/>
-      <c r="R79" s="96"/>
-      <c r="U79" s="95"/>
-      <c r="Y79" s="96"/>
-      <c r="AB79" s="95"/>
+      <c r="D79" s="78"/>
+      <c r="G79" s="77"/>
+      <c r="H79" s="78"/>
+      <c r="K79" s="78"/>
+      <c r="N79" s="77"/>
+      <c r="R79" s="78"/>
+      <c r="U79" s="77"/>
+      <c r="Y79" s="78"/>
+      <c r="AB79" s="77"/>
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D81" s="96"/>
-      <c r="F81" s="95"/>
-      <c r="G81" s="95"/>
-      <c r="K81" s="96"/>
-      <c r="M81" s="95"/>
-      <c r="N81" s="95"/>
-      <c r="R81" s="96"/>
-      <c r="T81" s="95"/>
-      <c r="U81" s="95"/>
-      <c r="Y81" s="96"/>
-      <c r="AA81" s="95"/>
-      <c r="AB81" s="95"/>
+      <c r="D81" s="78"/>
+      <c r="F81" s="77"/>
+      <c r="G81" s="77"/>
+      <c r="K81" s="78"/>
+      <c r="M81" s="77"/>
+      <c r="N81" s="77"/>
+      <c r="R81" s="78"/>
+      <c r="T81" s="77"/>
+      <c r="U81" s="77"/>
+      <c r="Y81" s="78"/>
+      <c r="AA81" s="77"/>
+      <c r="AB81" s="77"/>
     </row>
     <row r="82" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D82" s="94"/>
-      <c r="F82" s="95"/>
-      <c r="G82" s="95"/>
-      <c r="K82" s="94"/>
-      <c r="M82" s="95"/>
-      <c r="N82" s="95"/>
-      <c r="R82" s="94"/>
-      <c r="T82" s="95"/>
-      <c r="U82" s="95"/>
-      <c r="Y82" s="94"/>
-      <c r="AA82" s="95"/>
-      <c r="AB82" s="95"/>
+      <c r="D82" s="76"/>
+      <c r="F82" s="77"/>
+      <c r="G82" s="77"/>
+      <c r="K82" s="76"/>
+      <c r="M82" s="77"/>
+      <c r="N82" s="77"/>
+      <c r="R82" s="76"/>
+      <c r="T82" s="77"/>
+      <c r="U82" s="77"/>
+      <c r="Y82" s="76"/>
+      <c r="AA82" s="77"/>
+      <c r="AB82" s="77"/>
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G83" s="95"/>
-      <c r="N83" s="95"/>
-      <c r="U83" s="95"/>
-      <c r="AB83" s="95"/>
+      <c r="G83" s="77"/>
+      <c r="N83" s="77"/>
+      <c r="U83" s="77"/>
+      <c r="AB83" s="77"/>
     </row>
     <row r="85" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D85" s="97"/>
-      <c r="E85" s="97"/>
-      <c r="F85" s="97"/>
-      <c r="K85" s="97"/>
-      <c r="L85" s="97"/>
-      <c r="M85" s="97"/>
-      <c r="R85" s="97"/>
-      <c r="S85" s="97"/>
-      <c r="T85" s="97"/>
-      <c r="Y85" s="97"/>
-      <c r="Z85" s="97"/>
-      <c r="AA85" s="97"/>
+      <c r="D85" s="99"/>
+      <c r="E85" s="99"/>
+      <c r="F85" s="99"/>
+      <c r="K85" s="99"/>
+      <c r="L85" s="99"/>
+      <c r="M85" s="99"/>
+      <c r="R85" s="99"/>
+      <c r="S85" s="99"/>
+      <c r="T85" s="99"/>
+      <c r="Y85" s="99"/>
+      <c r="Z85" s="99"/>
+      <c r="AA85" s="99"/>
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D86" s="93"/>
-      <c r="K86" s="93"/>
-      <c r="R86" s="93"/>
-      <c r="Y86" s="93"/>
+      <c r="D86" s="75"/>
+      <c r="K86" s="75"/>
+      <c r="R86" s="75"/>
+      <c r="Y86" s="75"/>
     </row>
     <row r="88" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D88" s="96"/>
-      <c r="E88" s="94"/>
-      <c r="K88" s="96"/>
-      <c r="L88" s="94"/>
-      <c r="R88" s="96"/>
-      <c r="S88" s="94"/>
-      <c r="Y88" s="96"/>
-      <c r="Z88" s="94"/>
+      <c r="D88" s="78"/>
+      <c r="E88" s="76"/>
+      <c r="K88" s="78"/>
+      <c r="L88" s="76"/>
+      <c r="R88" s="78"/>
+      <c r="S88" s="76"/>
+      <c r="Y88" s="78"/>
+      <c r="Z88" s="76"/>
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D89" s="96"/>
-      <c r="K89" s="96"/>
-      <c r="R89" s="96"/>
-      <c r="Y89" s="96"/>
+      <c r="D89" s="78"/>
+      <c r="K89" s="78"/>
+      <c r="R89" s="78"/>
+      <c r="Y89" s="78"/>
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D91" s="96"/>
-      <c r="F91" s="95"/>
-      <c r="G91" s="95"/>
-      <c r="K91" s="96"/>
-      <c r="M91" s="95"/>
-      <c r="N91" s="95"/>
-      <c r="R91" s="96"/>
-      <c r="T91" s="95"/>
-      <c r="U91" s="95"/>
-      <c r="Y91" s="96"/>
-      <c r="AA91" s="95"/>
-      <c r="AB91" s="95"/>
+      <c r="D91" s="78"/>
+      <c r="F91" s="77"/>
+      <c r="G91" s="77"/>
+      <c r="K91" s="78"/>
+      <c r="M91" s="77"/>
+      <c r="N91" s="77"/>
+      <c r="R91" s="78"/>
+      <c r="T91" s="77"/>
+      <c r="U91" s="77"/>
+      <c r="Y91" s="78"/>
+      <c r="AA91" s="77"/>
+      <c r="AB91" s="77"/>
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G93" s="95"/>
-      <c r="N93" s="95"/>
-      <c r="U93" s="95"/>
-      <c r="AB93" s="95"/>
-      <c r="AC93" s="95"/>
+      <c r="G93" s="77"/>
+      <c r="N93" s="77"/>
+      <c r="U93" s="77"/>
+      <c r="AB93" s="77"/>
+      <c r="AC93" s="77"/>
     </row>
     <row r="94" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A94" s="98"/>
-      <c r="B94" s="98"/>
-      <c r="C94" s="98"/>
-      <c r="D94" s="98"/>
-      <c r="E94" s="98"/>
-      <c r="F94" s="98"/>
-      <c r="G94" s="98"/>
-      <c r="H94" s="98"/>
-      <c r="I94" s="98"/>
-      <c r="J94" s="98"/>
-      <c r="K94" s="98"/>
-      <c r="L94" s="98"/>
-      <c r="M94" s="98"/>
-      <c r="N94" s="98"/>
-      <c r="O94" s="98"/>
-      <c r="P94" s="98"/>
-      <c r="Q94" s="98"/>
-      <c r="R94" s="98"/>
-      <c r="S94" s="98"/>
-      <c r="T94" s="98"/>
-      <c r="U94" s="98"/>
-      <c r="V94" s="98"/>
-      <c r="W94" s="98"/>
-      <c r="X94" s="98"/>
-      <c r="Y94" s="98"/>
-      <c r="Z94" s="98"/>
-      <c r="AA94" s="98"/>
-      <c r="AB94" s="98"/>
-      <c r="AC94" s="98"/>
+      <c r="A94" s="79"/>
+      <c r="B94" s="79"/>
+      <c r="C94" s="79"/>
+      <c r="D94" s="79"/>
+      <c r="E94" s="79"/>
+      <c r="F94" s="79"/>
+      <c r="G94" s="79"/>
+      <c r="H94" s="79"/>
+      <c r="I94" s="79"/>
+      <c r="J94" s="79"/>
+      <c r="K94" s="79"/>
+      <c r="L94" s="79"/>
+      <c r="M94" s="79"/>
+      <c r="N94" s="79"/>
+      <c r="O94" s="79"/>
+      <c r="P94" s="79"/>
+      <c r="Q94" s="79"/>
+      <c r="R94" s="79"/>
+      <c r="S94" s="79"/>
+      <c r="T94" s="79"/>
+      <c r="U94" s="79"/>
+      <c r="V94" s="79"/>
+      <c r="W94" s="79"/>
+      <c r="X94" s="79"/>
+      <c r="Y94" s="79"/>
+      <c r="Z94" s="79"/>
+      <c r="AA94" s="79"/>
+      <c r="AB94" s="79"/>
+      <c r="AC94" s="79"/>
     </row>
     <row r="95" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B95" s="97"/>
-      <c r="C95" s="97"/>
-      <c r="D95" s="97"/>
-      <c r="I95" s="97"/>
-      <c r="J95" s="97"/>
-      <c r="K95" s="97"/>
-      <c r="P95" s="97"/>
-      <c r="Q95" s="97"/>
-      <c r="R95" s="97"/>
-      <c r="W95" s="97"/>
-      <c r="X95" s="97"/>
-      <c r="Y95" s="97"/>
+      <c r="B95" s="99"/>
+      <c r="C95" s="99"/>
+      <c r="D95" s="99"/>
+      <c r="I95" s="99"/>
+      <c r="J95" s="99"/>
+      <c r="K95" s="99"/>
+      <c r="P95" s="99"/>
+      <c r="Q95" s="99"/>
+      <c r="R95" s="99"/>
+      <c r="W95" s="99"/>
+      <c r="X95" s="99"/>
+      <c r="Y95" s="99"/>
     </row>
     <row r="97" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D97" s="97"/>
-      <c r="E97" s="97"/>
-      <c r="F97" s="97"/>
-      <c r="K97" s="97"/>
-      <c r="L97" s="97"/>
-      <c r="M97" s="97"/>
-      <c r="R97" s="97"/>
-      <c r="S97" s="97"/>
-      <c r="T97" s="97"/>
-      <c r="Y97" s="97"/>
-      <c r="Z97" s="97"/>
-      <c r="AA97" s="97"/>
+      <c r="D97" s="99"/>
+      <c r="E97" s="99"/>
+      <c r="F97" s="99"/>
+      <c r="K97" s="99"/>
+      <c r="L97" s="99"/>
+      <c r="M97" s="99"/>
+      <c r="R97" s="99"/>
+      <c r="S97" s="99"/>
+      <c r="T97" s="99"/>
+      <c r="Y97" s="99"/>
+      <c r="Z97" s="99"/>
+      <c r="AA97" s="99"/>
     </row>
     <row r="98" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D98" s="93"/>
-      <c r="K98" s="93"/>
-      <c r="R98" s="93"/>
-      <c r="Y98" s="93"/>
+      <c r="D98" s="75"/>
+      <c r="K98" s="75"/>
+      <c r="R98" s="75"/>
+      <c r="Y98" s="75"/>
     </row>
     <row r="100" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D100" s="96"/>
-      <c r="E100" s="94"/>
-      <c r="G100" s="95"/>
-      <c r="H100" s="96"/>
-      <c r="K100" s="96"/>
-      <c r="L100" s="94"/>
-      <c r="N100" s="95"/>
-      <c r="R100" s="96"/>
-      <c r="S100" s="94"/>
-      <c r="U100" s="95"/>
-      <c r="Y100" s="96"/>
-      <c r="Z100" s="94"/>
-      <c r="AB100" s="95"/>
+      <c r="D100" s="78"/>
+      <c r="E100" s="76"/>
+      <c r="G100" s="77"/>
+      <c r="H100" s="78"/>
+      <c r="K100" s="78"/>
+      <c r="L100" s="76"/>
+      <c r="N100" s="77"/>
+      <c r="R100" s="78"/>
+      <c r="S100" s="76"/>
+      <c r="U100" s="77"/>
+      <c r="Y100" s="78"/>
+      <c r="Z100" s="76"/>
+      <c r="AB100" s="77"/>
     </row>
     <row r="101" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D101" s="96"/>
-      <c r="K101" s="96"/>
-      <c r="R101" s="96"/>
-      <c r="Y101" s="96"/>
+      <c r="D101" s="78"/>
+      <c r="K101" s="78"/>
+      <c r="R101" s="78"/>
+      <c r="Y101" s="78"/>
     </row>
     <row r="103" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D103" s="96"/>
-      <c r="F103" s="95"/>
-      <c r="G103" s="95"/>
-      <c r="K103" s="96"/>
-      <c r="M103" s="95"/>
-      <c r="N103" s="95"/>
-      <c r="R103" s="96"/>
-      <c r="T103" s="95"/>
-      <c r="U103" s="95"/>
-      <c r="Y103" s="96"/>
-      <c r="AA103" s="95"/>
-      <c r="AB103" s="95"/>
+      <c r="D103" s="78"/>
+      <c r="F103" s="77"/>
+      <c r="G103" s="77"/>
+      <c r="K103" s="78"/>
+      <c r="M103" s="77"/>
+      <c r="N103" s="77"/>
+      <c r="R103" s="78"/>
+      <c r="T103" s="77"/>
+      <c r="U103" s="77"/>
+      <c r="Y103" s="78"/>
+      <c r="AA103" s="77"/>
+      <c r="AB103" s="77"/>
     </row>
     <row r="104" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G104" s="95"/>
-      <c r="N104" s="95"/>
-      <c r="U104" s="95"/>
-      <c r="AB104" s="95"/>
+      <c r="G104" s="77"/>
+      <c r="N104" s="77"/>
+      <c r="U104" s="77"/>
+      <c r="AB104" s="77"/>
     </row>
     <row r="106" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D106" s="97"/>
-      <c r="E106" s="97"/>
-      <c r="F106" s="97"/>
-      <c r="K106" s="97"/>
-      <c r="L106" s="97"/>
-      <c r="M106" s="97"/>
-      <c r="R106" s="97"/>
-      <c r="S106" s="97"/>
-      <c r="T106" s="97"/>
-      <c r="Y106" s="97"/>
-      <c r="Z106" s="97"/>
-      <c r="AA106" s="97"/>
+      <c r="D106" s="99"/>
+      <c r="E106" s="99"/>
+      <c r="F106" s="99"/>
+      <c r="K106" s="99"/>
+      <c r="L106" s="99"/>
+      <c r="M106" s="99"/>
+      <c r="R106" s="99"/>
+      <c r="S106" s="99"/>
+      <c r="T106" s="99"/>
+      <c r="Y106" s="99"/>
+      <c r="Z106" s="99"/>
+      <c r="AA106" s="99"/>
     </row>
     <row r="107" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D107" s="93"/>
-      <c r="K107" s="93"/>
-      <c r="R107" s="93"/>
-      <c r="Y107" s="93"/>
+      <c r="D107" s="75"/>
+      <c r="K107" s="75"/>
+      <c r="R107" s="75"/>
+      <c r="Y107" s="75"/>
     </row>
     <row r="109" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D109" s="96"/>
-      <c r="E109" s="94"/>
-      <c r="K109" s="96"/>
-      <c r="L109" s="94"/>
-      <c r="R109" s="96"/>
-      <c r="S109" s="94"/>
-      <c r="Y109" s="96"/>
-      <c r="Z109" s="94"/>
+      <c r="D109" s="78"/>
+      <c r="E109" s="76"/>
+      <c r="K109" s="78"/>
+      <c r="L109" s="76"/>
+      <c r="R109" s="78"/>
+      <c r="S109" s="76"/>
+      <c r="Y109" s="78"/>
+      <c r="Z109" s="76"/>
     </row>
     <row r="110" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D110" s="96"/>
-      <c r="G110" s="95"/>
-      <c r="H110" s="96"/>
-      <c r="K110" s="96"/>
-      <c r="N110" s="95"/>
-      <c r="R110" s="96"/>
-      <c r="U110" s="95"/>
-      <c r="Y110" s="96"/>
-      <c r="AB110" s="95"/>
+      <c r="D110" s="78"/>
+      <c r="G110" s="77"/>
+      <c r="H110" s="78"/>
+      <c r="K110" s="78"/>
+      <c r="N110" s="77"/>
+      <c r="R110" s="78"/>
+      <c r="U110" s="77"/>
+      <c r="Y110" s="78"/>
+      <c r="AB110" s="77"/>
     </row>
     <row r="112" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D112" s="96"/>
-      <c r="F112" s="95"/>
-      <c r="G112" s="95"/>
-      <c r="K112" s="96"/>
-      <c r="M112" s="95"/>
-      <c r="N112" s="95"/>
-      <c r="R112" s="96"/>
-      <c r="T112" s="95"/>
-      <c r="U112" s="95"/>
-      <c r="Y112" s="96"/>
-      <c r="AA112" s="95"/>
-      <c r="AB112" s="95"/>
+      <c r="D112" s="78"/>
+      <c r="F112" s="77"/>
+      <c r="G112" s="77"/>
+      <c r="K112" s="78"/>
+      <c r="M112" s="77"/>
+      <c r="N112" s="77"/>
+      <c r="R112" s="78"/>
+      <c r="T112" s="77"/>
+      <c r="U112" s="77"/>
+      <c r="Y112" s="78"/>
+      <c r="AA112" s="77"/>
+      <c r="AB112" s="77"/>
     </row>
     <row r="113" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D113" s="94"/>
-      <c r="F113" s="95"/>
-      <c r="G113" s="95"/>
-      <c r="K113" s="94"/>
-      <c r="M113" s="95"/>
-      <c r="N113" s="95"/>
-      <c r="R113" s="94"/>
-      <c r="T113" s="95"/>
-      <c r="U113" s="95"/>
-      <c r="Y113" s="94"/>
-      <c r="AA113" s="95"/>
-      <c r="AB113" s="95"/>
+      <c r="D113" s="76"/>
+      <c r="F113" s="77"/>
+      <c r="G113" s="77"/>
+      <c r="K113" s="76"/>
+      <c r="M113" s="77"/>
+      <c r="N113" s="77"/>
+      <c r="R113" s="76"/>
+      <c r="T113" s="77"/>
+      <c r="U113" s="77"/>
+      <c r="Y113" s="76"/>
+      <c r="AA113" s="77"/>
+      <c r="AB113" s="77"/>
     </row>
     <row r="114" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G114" s="95"/>
-      <c r="N114" s="95"/>
-      <c r="U114" s="95"/>
-      <c r="AB114" s="95"/>
+      <c r="G114" s="77"/>
+      <c r="N114" s="77"/>
+      <c r="U114" s="77"/>
+      <c r="AB114" s="77"/>
     </row>
     <row r="116" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D116" s="97"/>
-      <c r="E116" s="97"/>
-      <c r="F116" s="97"/>
-      <c r="K116" s="97"/>
-      <c r="L116" s="97"/>
-      <c r="M116" s="97"/>
-      <c r="R116" s="97"/>
-      <c r="S116" s="97"/>
-      <c r="T116" s="97"/>
-      <c r="Y116" s="97"/>
-      <c r="Z116" s="97"/>
-      <c r="AA116" s="97"/>
+      <c r="D116" s="99"/>
+      <c r="E116" s="99"/>
+      <c r="F116" s="99"/>
+      <c r="K116" s="99"/>
+      <c r="L116" s="99"/>
+      <c r="M116" s="99"/>
+      <c r="R116" s="99"/>
+      <c r="S116" s="99"/>
+      <c r="T116" s="99"/>
+      <c r="Y116" s="99"/>
+      <c r="Z116" s="99"/>
+      <c r="AA116" s="99"/>
     </row>
     <row r="117" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D117" s="93"/>
-      <c r="K117" s="93"/>
-      <c r="R117" s="93"/>
-      <c r="Y117" s="93"/>
+      <c r="D117" s="75"/>
+      <c r="K117" s="75"/>
+      <c r="R117" s="75"/>
+      <c r="Y117" s="75"/>
     </row>
     <row r="119" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D119" s="96"/>
-      <c r="E119" s="94"/>
-      <c r="K119" s="96"/>
-      <c r="L119" s="94"/>
-      <c r="R119" s="96"/>
-      <c r="S119" s="94"/>
-      <c r="Y119" s="96"/>
-      <c r="Z119" s="94"/>
+      <c r="D119" s="78"/>
+      <c r="E119" s="76"/>
+      <c r="K119" s="78"/>
+      <c r="L119" s="76"/>
+      <c r="R119" s="78"/>
+      <c r="S119" s="76"/>
+      <c r="Y119" s="78"/>
+      <c r="Z119" s="76"/>
     </row>
     <row r="120" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D120" s="96"/>
-      <c r="K120" s="96"/>
-      <c r="R120" s="96"/>
-      <c r="Y120" s="96"/>
+      <c r="D120" s="78"/>
+      <c r="K120" s="78"/>
+      <c r="R120" s="78"/>
+      <c r="Y120" s="78"/>
     </row>
     <row r="122" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D122" s="96"/>
-      <c r="F122" s="95"/>
-      <c r="G122" s="95"/>
-      <c r="K122" s="96"/>
-      <c r="M122" s="95"/>
-      <c r="N122" s="95"/>
-      <c r="R122" s="96"/>
-      <c r="T122" s="95"/>
-      <c r="U122" s="95"/>
-      <c r="Y122" s="96"/>
-      <c r="AA122" s="95"/>
-      <c r="AB122" s="95"/>
+      <c r="D122" s="78"/>
+      <c r="F122" s="77"/>
+      <c r="G122" s="77"/>
+      <c r="K122" s="78"/>
+      <c r="M122" s="77"/>
+      <c r="N122" s="77"/>
+      <c r="R122" s="78"/>
+      <c r="T122" s="77"/>
+      <c r="U122" s="77"/>
+      <c r="Y122" s="78"/>
+      <c r="AA122" s="77"/>
+      <c r="AB122" s="77"/>
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="G124" s="95"/>
-      <c r="N124" s="95"/>
-      <c r="U124" s="95"/>
-      <c r="AB124" s="95"/>
-      <c r="AC124" s="95"/>
+      <c r="G124" s="77"/>
+      <c r="N124" s="77"/>
+      <c r="U124" s="77"/>
+      <c r="AB124" s="77"/>
+      <c r="AC124" s="77"/>
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A125" s="98"/>
-      <c r="B125" s="98"/>
-      <c r="C125" s="98"/>
-      <c r="D125" s="98"/>
-      <c r="E125" s="98"/>
-      <c r="F125" s="98"/>
-      <c r="G125" s="98"/>
-      <c r="H125" s="98"/>
-      <c r="I125" s="98"/>
-      <c r="J125" s="98"/>
-      <c r="K125" s="98"/>
-      <c r="L125" s="98"/>
-      <c r="M125" s="98"/>
-      <c r="N125" s="98"/>
-      <c r="O125" s="98"/>
-      <c r="P125" s="98"/>
-      <c r="Q125" s="98"/>
-      <c r="R125" s="98"/>
-      <c r="S125" s="98"/>
-      <c r="T125" s="98"/>
-      <c r="U125" s="98"/>
-      <c r="V125" s="98"/>
-      <c r="W125" s="98"/>
-      <c r="X125" s="98"/>
-      <c r="Y125" s="98"/>
-      <c r="Z125" s="98"/>
-      <c r="AA125" s="98"/>
-      <c r="AB125" s="98"/>
-      <c r="AC125" s="98"/>
+      <c r="A125" s="79"/>
+      <c r="B125" s="79"/>
+      <c r="C125" s="79"/>
+      <c r="D125" s="79"/>
+      <c r="E125" s="79"/>
+      <c r="F125" s="79"/>
+      <c r="G125" s="79"/>
+      <c r="H125" s="79"/>
+      <c r="I125" s="79"/>
+      <c r="J125" s="79"/>
+      <c r="K125" s="79"/>
+      <c r="L125" s="79"/>
+      <c r="M125" s="79"/>
+      <c r="N125" s="79"/>
+      <c r="O125" s="79"/>
+      <c r="P125" s="79"/>
+      <c r="Q125" s="79"/>
+      <c r="R125" s="79"/>
+      <c r="S125" s="79"/>
+      <c r="T125" s="79"/>
+      <c r="U125" s="79"/>
+      <c r="V125" s="79"/>
+      <c r="W125" s="79"/>
+      <c r="X125" s="79"/>
+      <c r="Y125" s="79"/>
+      <c r="Z125" s="79"/>
+      <c r="AA125" s="79"/>
+      <c r="AB125" s="79"/>
+      <c r="AC125" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="K106:M106"/>
-    <mergeCell ref="R106:T106"/>
     <mergeCell ref="Y106:AA106"/>
     <mergeCell ref="D116:F116"/>
     <mergeCell ref="K116:M116"/>
     <mergeCell ref="R116:T116"/>
     <mergeCell ref="Y116:AA116"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="I95:K95"/>
-    <mergeCell ref="P95:R95"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="K106:M106"/>
+    <mergeCell ref="R106:T106"/>
     <mergeCell ref="W95:Y95"/>
     <mergeCell ref="D97:F97"/>
     <mergeCell ref="K97:M97"/>
     <mergeCell ref="R97:T97"/>
     <mergeCell ref="Y97:AA97"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="K75:M75"/>
-    <mergeCell ref="R75:T75"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="I95:K95"/>
+    <mergeCell ref="P95:R95"/>
     <mergeCell ref="Y75:AA75"/>
     <mergeCell ref="D85:F85"/>
     <mergeCell ref="K85:M85"/>
     <mergeCell ref="R85:T85"/>
     <mergeCell ref="Y85:AA85"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="I64:K64"/>
-    <mergeCell ref="P64:R64"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="K75:M75"/>
+    <mergeCell ref="R75:T75"/>
     <mergeCell ref="W64:Y64"/>
     <mergeCell ref="D66:F66"/>
     <mergeCell ref="K66:M66"/>
     <mergeCell ref="R66:T66"/>
     <mergeCell ref="Y66:AA66"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="I64:K64"/>
+    <mergeCell ref="P64:R64"/>
     <mergeCell ref="D44:F44"/>
     <mergeCell ref="K44:M44"/>
     <mergeCell ref="R44:T44"/>
@@ -4456,6 +4987,8 @@
     <mergeCell ref="Y4:AA4"/>
     <mergeCell ref="Y13:AA13"/>
     <mergeCell ref="Y23:AA23"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="R15:T15"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D13:F13"/>
@@ -4463,6 +4996,8 @@
     <mergeCell ref="K23:M23"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="L4:N4"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="L15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>